<commit_message>
triple proposal mesh terms
</commit_message>
<xml_diff>
--- a/faculty_corresponding_unique_terms.xlsx
+++ b/faculty_corresponding_unique_terms.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,21 +453,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Education, Graduate; Skin Pigmentation; Loma; Carbon; Sphingomonas; Wildfires; Students; Metagenome; Climate; Program Evaluation; Climate Change; Ecosystem; Trees; Phylogeny; Mutation; Interdisciplinary Communication; Biological Evolution; Methane; Life History Traits; Metagenomics; Isoptera; Soil Microbiology; Soil; Faculty; Humanities; Nitrification; Workforce; Uncertainty; Temperature; Stress, Physiological; California; Environmental Science; Authorship; Environmental Microbiology; Biomass; Goals; Forests; Introduced Species; Grassland; Nitrogen; Microbial Interactions; Biodegradation, Environmental; Resilience, Psychological; Environmental Justice; Conservation of Natural Resources; Policy Making; Policy; Social Sciences; Plants; Extreme Weather; Droughts; Communication; Water; Ecological and Environmental Phenomena; Adaptation, Physiological; Universities; Curriculum; Coral Reefs; Wood; Genomics; Writing; Enzymes; Australia; Carbon Cycle; Greenhouse Gases; Plant Leaves; Microbiota; United States; Tropical Climate; Drought Resistance; Bacteria; Financial Management</t>
+          <t>Carbon Cycle; Policy Making; Authorship; Microbiota; Nitrogen; Policy; Students; Forests; Soil Microbiology; Ecological and Environmental Phenomena; Environmental Justice; Carbon; Social Sciences; Enzymes; Resilience, Psychological; Soil; Bacteria; Wildfires; Writing; Financial Management; Universities; Genomics; Loma; Temperature; Ecosystem; Environmental Science; Biodegradation, Environmental; Communication; Humanities; Goals; Droughts; Workforce; Faculty; Environmental Microbiology; Greenhouse Gases; Extreme Weather; Skin Pigmentation; Climate Change; Interdisciplinary Communication</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Arora, Kavita</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Transforming Growth Factor beta; Body Patterning; Mycobacterium tuberculosis; Drosophila Proteins; Heme Oxygenase-1; Drosophila melanogaster; Computational Biology; Signal Transduction; Tuberculosis; Bacterial Load; Mosaicism; N-Acetylglucosaminyltransferases; Genetics; Protoporphyrins; Lung; T-Lymphocytes; Synthetic Lethal Mutations; Gene Expression Regulation, Developmental; Enzyme Inhibitors; Metabolism; Drosophila; Transgenes; Metalloporphyrins; Treatment Outcome; Developmental Biology; Alleles; Immunologic Factors; Phenotype; Infertility, Female; Germ-Line Mutation</t>
-        </is>
-      </c>
+          <t>Arora, K</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -477,7 +473,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Chromatin; Small Cell Lung Carcinoma; Gene Regulatory Networks; Single-Cell Analysis; Carcinoma, Basosquamous; Tumor Microenvironment; Microphysiological Systems; Repressor Proteins; Bioprinting; Sirolimus; NIH 3T3 Cells; Lung Neoplasms; Immune System; Keratinocytes; Tissue Engineering; RNA-Seq; Epidermal Cells; Algorithms; Cell Line, Tumor; Trans-Activators; United States; Multiomics; Transcription Factor AP-1; Drug Resistance; Epidermis; Mutation; Zinc Finger Protein GLI1; Sebaceous Glands; Antineoplastic Agents; Organoids; Clone Cells; Epithelial Cells; Triazines; Computer Simulation; Chromatography, Liquid; Organ Culture Techniques; Hedgehogs; RNA; T-Lymphocytes; Carcinogenesis; Hyperplasia; Gene Expression Profiling; Carcinoma, Basal Cell; Neutrophils; Skin Neoplasms; Smad3 Protein; MAP Kinase Signaling System; Transforming Growth Factor beta; Cells, Cultured; Infant, Newborn; Ecosystem; Everolimus; Interleukin-1alpha; Homeostasis; Molecular Biology; Signal Transduction; Cell Differentiation; Foreskin; Tandem Mass Spectrometry; Cell Nucleus; Phosphorylation; Extracellular Matrix; Extrude; Allografts; Nucleosides; Genes, Suppressor; Hair Follicle; Imiquimod; Protein Binding; DNA-Binding Proteins; Prostate; Genetic Techniques; Brain; Psoriasis; Sequence Analysis, RNA; Mitogen-Activated Protein Kinase 1; Imidazoles; Immunity; cemiplimab; Stem Cells; Cell Communication; Conserved Sequence; Hedgehog Proteins; Protein Kinase C; Skin Diseases; DNA, Neoplasm; Skin Physiological Phenomena; Dermis; Binding Sites; Pluripotent Stem Cells; Gene Expression Regulation; TOR Serine-Threonine Kinases; Drug Resistance, Neoplasm; Immunohistochemistry; Patched-1 Receptor; Skin; Neoplasm Proteins; HhAntag691; Guanine Nucleotide Exchange Factors; Gene Ontology; Immunotherapy; Up-Regulation; Neutrophil Activation; Phosphotransferases; Transcriptome; Neoplasms; Cell Lineage; Preliminary Data; Transcription Factors</t>
+          <t>Cell Line, Tumor; Carcinoma, Basal Cell; Signal Transduction; Drug Resistance; Neutrophils; Immune System; Preliminary Data; Extrude; Immunotherapy; Phosphotransferases; Hedgehog Proteins; Neutrophil Activation; United States; Transcription Factors; Skin Neoplasms; Mutation; Clone Cells; Genetic Techniques; Skin; Hedgehogs; cemiplimab; Zinc Finger Protein GLI1; Prostate; Keratinocytes; Genes, Suppressor; Phosphorylation; HhAntag691; Dermis; Lung Neoplasms; Allografts; Molecular Biology; Protein Kinase C; Brain; Carcinogenesis; Small Cell Lung Carcinoma; Organoids; Immunity; T-Lymphocytes; Stem Cells</t>
         </is>
       </c>
     </row>
@@ -489,21 +485,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Connective Tissue; Bite Force; Isometric Contraction; Hindlimb; Achilles Tendon; Biomechanical Phenomena; Courtship; Swimming; Elasticity; Viscosity; Trees; Phylogeny; Masticatory Muscles; Running; Elastomers; Muscle Spindles; Robotics; Fishes; Jaw; Conservation of Energy Resources; Conus Snail; Locomotion; Temperature; Lizards; Alligators and Crocodiles; Electromyography; Forelimb; Poaceae; Predatory Behavior; Walking; Biomimetic Materials; Anura; Stress, Mechanical; Tendons; Exercise; Aging; Biocompatible Materials; Movement; Lower Extremity; Sand; Energy Metabolism; Galliformes; Muscular Atrophy; Physics; Body Temperature; Muscle, Skeletal; Robotic Surgical Procedures; Motor Activity; Sexual Behavior, Animal; Muscle Fibers, Skeletal; Torque; Extremities; Muscle Contraction; Gait; Environment; Bufo marinus; Kinetics; Virtual Reality</t>
+          <t>Movement; Virtual Reality; Biomimetic Materials; Swimming; Motor Activity; Biomechanical Phenomena; Robotics; Muscle, Skeletal; Muscle Fibers, Skeletal; Physics; Tendons; Exercise; Alligators and Crocodiles; Biocompatible Materials; Walking; Torque; Aging; Achilles Tendon; Sand; Robotic Surgical Procedures</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Baker, Nicholas</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Protein Kinases; Cell Communication; Basic Helix-Loop-Helix Transcription Factors; Inhibitor of Apoptosis Proteins; Caspase Inhibitors; Telomere-Binding Proteins; Mutation; Caspases; Carrier Proteins; Drosophila Proteins; Pancytopenia; Base Sequence; Membrane Proteins; Signal Transduction; Wnt Signaling Pathway; Organogenesis; Eye; Wings, Animal; Cell Differentiation; Cell Competition; Liver; Cell Survival; Repressor Proteins; Proto-Oncogene Proteins; Aneuploidy; Larva; Haploinsufficiency; Phosphorylation; Genes, Essential; Anemia, Diamond-Blackfan; Amino Acid Sequence; Mutation, Missense; Gene Dosage; Hematopoietic Stem Cells; Imaginal Discs; Shelterin Complex; Puromycin; Eukaryotic Initiation Factor-2; Protein Biosynthesis; Sequence Alignment; Up-Regulation; Oncogenes; YAP-Signaling Proteins; Genetic Loci; Animals, Genetically Modified; Gene Expression Regulation, Developmental; Compound Eye, Arthropod; Neurogenesis; Receptors, Notch; DNA-Binding Proteins; Protein Binding; Tumor Suppressor Protein p53; Neoplasms; Transcriptome; Ribosomes; Drosophila; MicroRNAs; Ubiquitin-Protein Ligases; Transcription Factors; Sequence Analysis, RNA; Erythropoiesis; Apoptosis; Glycogen Synthase Kinase 3; Transcription, Genetic; Gene Expression Profiling; Alleles; Trans-Activators; Wnt1 Protein; Photoreceptor Cells, Invertebrate; Ribosomal Proteins; Mammals; CRISPR-Associated Protein 9; Drosophila melanogaster; Cullin Proteins; Nuclear Proteins</t>
-        </is>
-      </c>
+          <t>Baker, Nicholas E</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -513,7 +505,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Proteins; MAP Kinase Kinase 2; Protein Serine-Threonine Kinases; DNA; Nuclear Matrix-Associated Proteins; Molecular Sequence Data; Repressor Proteins; Hydrophobic and Hydrophilic Interactions; Protein Domains; Saccharomyces cerevisiae; Sequence Alignment; Caenorhabditis elegans Proteins; Cyclin B; Hippo Signaling Pathway; Caenorhabditis elegans; Energy Metabolism; Mitosis; Phosphatidylinositol 3-Kinases; Evidence Gaps; Cell Line, Tumor; Zinc; Neuromuscular Junction; Protein Kinases; Diabetes Mellitus; Neurons; Synapses; Mutation; Zinc Finger Protein GLI1; Synaptic Transmission; Greig cephalopolysyndactyly syndrome; Protein Processing, Post-Translational; Ligands; Amino Acid Sequence; Axons; MAP Kinase Kinase 1; HeLa Cells; Congenital Hypothyroidism; Developmental Disabilities; Cyclin B2; Mammals; Cadmium; MAP Kinase Signaling System; Cells, Cultured; Infant, Newborn; MAP Kinase Kinase 4; Embryo, Nonmammalian; Homeostasis; Presynaptic Terminals; Signal Transduction; Stress, Physiological; Activating Transcription Factor 2; Inactivation, Metabolic; Phosphorylation; Larva; Cdc20 Proteins; Cyclin B1; Protein Binding; DNA-Binding Proteins; Tumor Suppressor Proteins; Clinical Relevance; Adenosine Triphosphate; Mitogen-Activated Protein Kinase 1; Transcription, Genetic; Drosophila melanogaster; Schizophrenia; Mitogen-Activated Protein Kinase 3; Thermodynamics; Comprehension; Transcriptional Activation; Conserved Sequence; Hedgehog Proteins; CDC2 Protein Kinase; Extracellular Signal-Regulated MAP Kinases; Binding Sites; Catalytic Domain; Drosophila Proteins; Protein Conformation; Recombinant Fusion Proteins; Gene Expression Regulation; Molecular Docking Simulation; Protein Subunits; MAP Kinase Kinase 6; Isoenzymes; ras GTPase-Activating Proteins; Phosphotransferases; Neoplasms; JNK Mitogen-Activated Protein Kinases; Mitogen-Activated Protein Kinases; Transcription Factors; Child; HEK293 Cells; Alleles; Transcription Factor MTF-1; Chaperonin Containing TCP-1</t>
+          <t>Congenital Hypothyroidism; Alleles; Signal Transduction; Ligands; Phosphatidylinositol 3-Kinases; DNA; Nuclear Matrix-Associated Proteins; Greig cephalopolysyndactyly syndrome; Hedgehog Proteins; ras GTPase-Activating Proteins; Transcription Factors; Diabetes Mellitus; Mutation; Protein Kinases; Neoplasms; Zinc Finger Protein GLI1; Phosphorylation; Extracellular Signal-Regulated MAP Kinases; Child; Schizophrenia; Infant, Newborn; Developmental Disabilities; Comprehension; Mitogen-Activated Protein Kinases; Clinical Relevance; Zinc; Transcriptional Activation; Evidence Gaps</t>
         </is>
       </c>
     </row>
@@ -525,7 +517,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pesticides; Child, Preschool; Inheritance Patterns; Insulysin; Epigenomics; Diabetes Mellitus; Bone and Bones; Zebrafish; Adolescent; Mesenchymal Stem Cells; Chromatin; Metabolomics; Obesity; Diabetes Mellitus, Type 2; Mutation; DNA; Genetic Predisposition to Disease; Xenobiotics; Fasting; 3T3-L1 Cells; Flutamide; Pregnane X Receptor; Fluorocarbons; Pandemics; Methylation; Cell Differentiation; Germ Cells; Liver; DNA Methylation; Receptors, Steroid; PPAR gamma; Trialkyltin Compounds; Noncommunicable Diseases; Lipolysis; Autism Spectrum Disorder; Autistic Disorder; Benzamides; Environmental Exposure; Weight Gain; Lipogenesis; Pyridines; Genetics; Retinoid X Receptors; Gastrointestinal Microbiome; Lipids; Sweetening Agents; Cell Line, Transformed; Endocrine Disruptors; Cannabidiol; Protein Binding; Prenatal Exposure Delayed Effects; Epigenesis, Genetic; Diet, Fat-Restricted; Adipose Tissue; vinclozolin; Oxazoles; Caenorhabditis elegans; MicroRNAs; Diet, High-Fat; Environmental Pollutants; Adipocytes; Drinking Water; Child; Dietary Fats; Receptors, Cytoplasmic and Nuclear; Rosiglitazone; Epidemiologic Studies; Insulin Resistance; Histones; Spermatozoa; Adipogenesis; Pregnancy; Multiomics; Phenotype</t>
+          <t>Pregnancy; Flutamide; Environmental Exposure; Receptors, Cytoplasmic and Nuclear; DNA; vinclozolin; Phenotype; Diabetes Mellitus, Type 2; Germ Cells; Obesity; Diabetes Mellitus; Diet, Fat-Restricted; Mutation; Epigenomics; Drinking Water; Liver; Chromatin; Epigenesis, Genetic; Insulysin; Endocrine Disruptors; Oxazoles; Dietary Fats; Fasting; Spermatozoa; Genetics; Noncommunicable Diseases; Multiomics</t>
         </is>
       </c>
     </row>
@@ -537,7 +529,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Chimera; Cell Proliferation; Chemotaxis; Complement C1q; Genetic Predisposition to Disease; Gene Regulatory Networks; Coculture Techniques; Cognitive Dysfunction; Gliosis; Amyloid beta-Peptides; Interleukin-17; Aging; Amyloidosis; Organic Chemicals; Tauopathies; Ferroptosis; Apolipoproteins E; Interferon-gamma; Oligodendrocyte Precursor Cells; Polymorphism, Single Nucleotide; Organelles; Microglia; Neurons; Induced Pluripotent Stem Cells; Neurodegenerative Diseases; Administration, Inhalation; Organoids; Endosomal Sorting Complexes Required for Transport; Presenilin-1; Sulfoxides; Aged; Xenon; Oxidative Stress; tau Proteins; Breast Neoplasms; Neuroinflammatory Diseases; Neutrophils; Sex Factors; Isothiocyanates; Cells, Cultured; Endoplasmic Reticulum; White Matter; Infant, Newborn; Calcium Signaling; Calcium; Cyclic AMP; Alzheimer Disease; Lipid Peroxidation; Contusions; Point Mutation; Interleukin-1beta; Cholesterol; Receptors, Granulocyte-Macrophage Colony-Stimulating Factor; Brain Neoplasms; Frontotemporal Dementia; Thalamus; Plaque, Amyloid; Astrocytes; Dementia; Brain; Endothelial Cells; Treatment Outcome; Brain Injuries, Traumatic; Transplantation, Heterologous; Cell Movement; Schizophrenia; Stem Cells; Twins, Monozygotic; Mitochondria; Leukoencephalopathies; Pluripotent Stem Cells; Phagocytosis; Gene Expression Regulation; Phenotype; Clusterin; Blood-Brain Barrier; Microscopy; NF-E2-Related Factor 2; Receptor, Macrophage Colony-Stimulating Factor; Cell- and Tissue-Based Therapy; Alleles; Apolipoprotein E4; Apolipoprotein E3; Inflammation</t>
+          <t>Alzheimer Disease; Pluripotent Stem Cells; Cell- and Tissue-Based Therapy; Microglia; Inflammation; Transplantation, Heterologous; Dementia; Stem Cells; Chimera</t>
         </is>
       </c>
     </row>
@@ -549,7 +541,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Carbon; Mytilus; Biodiversity; Physiological Phenomena; Students; Microalgae; Diet; Aquatic Organisms; Climate Change; Ecosystem; New Zealand; Kelp; Biological Evolution; Macrocystis; Alaska; Temperature; Carbon Dioxide; California; Stress, Physiological; Biomass; Marine Biology; Chondrus; Ammonium Compounds; Nitrogen; Portugal; Seawater; Seaweed; Mollusca; Conservation of Natural Resources; Extinction, Biological; Oxygen; Photosynthesis; Dose-Response Relationship, Drug; Oceans and Seas; Heat-Shock Response; Nitrates; Plants; Massachusetts; Mentors; Food Chain; Ecological and Environmental Phenomena; Fucus; Adaptation, Physiological; Universities; Curriculum; Maine; Urea; Symbiosis; Tidal Waves; Sea Anemones; Environment; Phenotype; Hydrogen-Ion Concentration</t>
+          <t>Marine Biology; Curriculum; Portugal; Ecological and Environmental Phenomena; Oceans and Seas; Ecosystem; Universities; Mentors; Biodiversity; Physiological Phenomena; Extinction, Biological; Seaweed; Climate Change; Students</t>
         </is>
       </c>
     </row>
@@ -561,7 +553,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Students; Heredity; Research Personnel; Carrier Proteins; Pupa; Aged, 80 and over; Temperature; Eye Proteins; Bees; Genotype; Predatory Behavior; Genetic Drift; Forests; Haplotypes; Rhodopsin; Mexico; Microscopy, Confocal; Polymerase Chain Reaction; RNA-Seq; Food Chain; Phylogeography; Mating Preference, Animal; Gene Expression; Heliconiaceae; Retinal Pigments; Light Signal Transduction; Biological Mimicry; Genetic Introgression; Evolution, Molecular; Retina; Polymorphism, Single Nucleotide; Rubiaceae; Farms; Reproduction; Blotting, Western; Genome, Insect; DNA Copy Number Variations; Mexican Americans; Vision, Ocular; Mutation; Genetic Variation; Clustered Regularly Interspaced Short Palindromic Repeats; Computational Biology; Iridescence; Ecuador; Wings, Animal; Insect Proteins; Body Temperature Regulation; Species Specificity; Goals; Sex Chromosomes; North America; Pigmentation; Acclimatization; short-wavelength opsin; Crystallization; Color; Writing; Photoreceptor Cells; Gene Expression Profiling; Translocation, Genetic; Kynurenine; Gene Duplication; Ultraviolet Rays; In Situ Hybridization; Sunlight; Ecosystem; Technology; Phylogeny; Trees; American Indian or Alaska Native; Biological Evolution; Heating; Florida; ommochrome; Sequence Analysis, DNA; Eye; Opsins; Sex Characteristics; Antibody Specificity; Infrared Rays; Pigments, Biological; Butterflies; Communication; Exons; Color Vision; Brain; Ecology; Genomics; Sexual Behavior, Animal; Drosophila melanogaster; Dosage Compensation, Genetic; RNA, Messenger; Gene Editing; Binding Sites; Faculty; Gene Expression Regulation; Birds; Costa Rica; Guyana; Perception; Immunohistochemistry; Phenotype; Spectrum Analysis; Selection, Genetic; Multigene Family; Gardening; Colombia; Gene Expression Regulation, Developmental; Sexual Selection; Plants, Edible; Transcriptome; Central Nervous System; Preliminary Data; Insecta; Colorado; Adaptation, Physiological; Electrophysiology; Optical Phenomena; Photoreceptor Cells, Vertebrate; Rod Opsins; long-wavelength opsin; Chromosomes; Fluorescence</t>
+          <t>Opsins; Costa Rica; long-wavelength opsin; Color Vision; Carrier Proteins; Preliminary Data; Sex Characteristics; Sexual Selection; Pupa; Students; Forests; Trees; Gene Editing; Colombia; short-wavelength opsin; Heating; Electrophysiology; Reproduction; Guyana; Bees; RNA, Messenger; Binding Sites; Rhodopsin; Retinal Pigments; Clustered Regularly Interspaced Short Palindromic Repeats; RNA-Seq; Antibody Specificity; Iridescence; Translocation, Genetic; Butterflies; Crystallization; In Situ Hybridization; Ecosystem; Genomics; ommochrome; Immunohistochemistry; Gene Duplication; Rod Opsins; Writing; Retina; Communication; Goals; Microscopy, Confocal; Heredity; Ultraviolet Rays; Phylogeny; Central Nervous System; Farms; Chromosomes; Perception; Gardening; Mexican Americans; Gene Expression Profiling; Transcriptome; American Indian or Alaska Native; Technology; Ecology; Blotting, Western</t>
         </is>
       </c>
     </row>
@@ -571,11 +563,7 @@
           <t>Burley, Nancy</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Universities; Problem-Based Learning; Students; Perception; Melopsittacus; Adolescent; Problem Solving; Sexual Behavior, Animal; Educational Measurement; Cell Adhesion Molecules, Neuronal</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -585,7 +573,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Trisomy 13 Syndrome; Cell Proliferation; Karyotype; Diabetes Mellitus, Type 2; Sphingolipids; Wound Healing; Quality of Life; Microtubule-Associated Proteins; Amyloid beta-Peptides; Aneuploidy; Aging; Calcium-Binding Proteins; Lymphocytes; Sphingosine; Insulin; Energy Metabolism; Hyperglycemia; Tauopathies; Delta Catenin; Atrophy; Reactive Oxygen Species; Drug Evaluation, Preclinical; Symporters; Microglia; Action Potentials; Neurons; Synapses; Disease Progression; Protein Kinase C-delta; Glucose; Antioxidants; Catenins; Synaptic Transmission; Cell Survival; Protein Stability; Aged; Cross-Sectional Studies; Oxidative Stress; Caspase 3; Down Syndrome; tau Proteins; Dendritic Spines; Neuroinflammatory Diseases; Basal Forebrain; Gene Expression Profiling; Cell Line; Pregnancy; Hippocampus; Nuclear Envelope; Child, Preschool; Cells, Cultured; Infant, Newborn; Adolescent; Trisomy 18 Syndrome; Glycogen Synthase Kinase 3 beta; Signal Transduction; Indoles; Cell Differentiation; Analgesics; Alzheimer Disease; Drug Repositioning; Adenosine Triphosphate; Cellular Senescence; Neuralgia; Longevity; Yeasts; Infant; Fibroblasts; Biomarkers; Biomedical Research; Mitochondria; gamma-Aminobutyric Acid; Nerve Degeneration; Gene Expression Regulation; Insulin-Secreting Cells; Chromosomes, Human, Pair 21; Catalase; Intracellular Signaling Peptides and Proteins; Benzazepines; Cytoprotection; Protein Biosynthesis; NF-E2-Related Factor 2; Membrane Potential, Mitochondrial; Muscle Proteins; Transcription Factors; Child; Young Adult; Spinal Cord Dorsal Horn; HEK293 Cells; Cancer Pain; Cytokines; Thrombospondin 1; Encephalitis</t>
+          <t>Alzheimer Disease; Down Syndrome; Oxidative Stress; Aging; Amyloid beta-Peptides; Microglia; Nerve Degeneration; Mitochondria; tau Proteins; Neuroinflammatory Diseases; Cellular Senescence</t>
         </is>
       </c>
     </row>
@@ -595,11 +583,7 @@
           <t>Cahill, Larry</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Bias; Face; Stroke; Magnetic Resonance Imaging; Research; Adolescent; Free Radical Scavengers; Huntingtin Protein; Biomedical Research; Frontal Lobe; Neuroprotective Agents; Trinucleotide Repeats; Tomography, Emission-Computed, Single-Photon; Amygdala; Neurosciences; Autistic Disorder; Pregnatrienes; Nerve Net; Huntington Disease; Neuropsychological Tests; Masculinity; Double-Blind Method; Sex Characteristics; Cognition; Brain Hemorrhage, Traumatic; Image Processing, Computer-Assisted; Contraceptives, Oral; Administration, Intranasal; Emotions; Intelligence; Brain; Subarachnoid Hemorrhage; Gyrus Cinguli; Estradiol; Memory, Episodic; Child; Young Adult; Brain Mapping; Brain Injuries, Traumatic; Polymorphism, Single Nucleotide; Memory; Reproduction; Oxytocin</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -609,7 +593,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Genes, Mitochondrial; Students; Chromatin; DNA; Protein Serine-Threonine Kinases; Gene Regulatory Networks; Wnt Signaling Pathway; Nutrients; Single-Cell Analysis; Liver; Time-Lapse Imaging; Otx Transcription Factors; Glycolysis; Machine Learning; Fatty Liver; Thinking; Consensus Sequence; Lysine; Hippo Signaling Pathway; Caenorhabditis elegans; Gene Expression; RNA Polymerase II; Enhancer Elements, Genetic; Lasers; Cell Line, Tumor; Reactive Oxygen Species; Zinc; Multiomics; High-Throughput Nucleotide Sequencing; Epigenomics; RNA Splicing; Deoxyribonuclease I; Xenopus laevis; Oogenesis; Neurulation; Epidermis; Mutation; Zygote; Computational Biology; Germ Layers; Blastula; Chromatin Immunoprecipitation; Gastrulation; Nervous System; Goals; Immunity, Innate; Fibroblast Growth Factors; Congenital Abnormalities; Chromatography, Liquid; Histone Deacetylase 2; HeLa Cells; RNA; Epigenesis, Genetic; Microscopy, Fluorescence; Drosophila; Regenerative Medicine; Gene Expression Profiling; Histones; Mammals; Cadmium; Cells, Cultured; Forkhead Transcription Factors; Embryo, Nonmammalian; Homeostasis; Signal Transduction; SOXB1 Transcription Factors; Histone Deacetylases; Endoderm; Biological Phenomena; Stress, Physiological; Cell Differentiation; Xenopus; Inactivation, Metabolic; Tandem Mass Spectrometry; Stem Cell Research; Embryonic Structures; Pregnancy Complications; Phosphorylation; Fetus; N-Myc Proto-Oncogene Protein; Histone Deacetylase 1; Acetylation; Preimplantation Diagnosis; Fertilization; Protein Binding; DNA-Binding Proteins; Genome; Tumor Suppressor Proteins; Histone Demethylases; Embryo, Mammalian; Embryo Implantation; Oxidative Phosphorylation; T-Box Domain Proteins; Genomics; Morpholinos; Curriculum; Proteome; Sequence Analysis, RNA; Gene Knockdown Techniques; Transcription, Genetic; Gastrula; Proteomics; Genes, Developmental; beta Catenin; Maternal Inheritance; SOXF Transcription Factors; Binding Sites; Neural Tube; Gene Expression Regulation; Regulatory Sequences, Nucleic Acid; Xenopus Proteins; Endodermal Sinus Tumor; animal cap; Embryo Culture Techniques; Gene Expression Regulation, Developmental; Ectoderm; Transcriptome; Oligonucleotides, Antisense; Central Nervous System; Cell Lineage; Embryonic Development; Transcription Factors; Mesoderm; HEK293 Cells; Developmental Biology; Wnt Proteins; Transcription Factor MTF-1; Uterus; Blastocyst; Phenotype</t>
+          <t>Fertilization; Signal Transduction; SOXB1 Transcription Factors; Gastrula; Blastula; Mammals; Xenopus laevis; Computational Biology; Neurulation; Genome; Phenotype; Gastrulation; Students; RNA; Embryonic Structures; Transcription Factors; Neural Tube; Mutation; Fetus; Nutrients; Germ Layers; Uterus; Cell Lineage; Transcription, Genetic; Endoderm; Gene Expression; Chromatin; Genomics; Biological Phenomena; Gene Regulatory Networks; Caenorhabditis elegans; Preimplantation Diagnosis; Epigenesis, Genetic; Genes, Developmental; Embryonic Development; Nervous System; Goals; Cell Differentiation; Pregnancy Complications; Central Nervous System; Ectoderm; Curriculum; Stem Cell Research; Drosophila; Gene Expression Profiling; Congenital Abnormalities; Regenerative Medicine; animal cap; Developmental Biology; Mesoderm; Sequence Analysis, RNA; Endodermal Sinus Tumor; Epidermis; Multiomics; Thinking</t>
         </is>
       </c>
     </row>
@@ -621,7 +605,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Theta Rhythm; White Matter; Magnetic Resonance Imaging; Diffusion Magnetic Resonance Imaging; Neurons; Functional Neuroimaging; Adolescent; Hand; Neuroimaging; Functional Laterality; Gray Matter; Temporal Lobe; Reaction Time; Menopause; Individuality; Cognitive Neuroscience; Spatial Navigation; Judgment; Figural Aftereffect; Goals; Alzheimer Disease; Head; Proprioception; Cognitive Science; Parietal Lobe; Depression; Computer Simulation; Confusion; Cognition; Motion Perception; Aged; Artificial Intelligence; Maze Learning; Cerebral Cortex; Imagination; Mentors; Gyrus Cinguli; Mentoring; Rotation; Brain; Interpersonal Relations; Learning; Space Perception; Memory, Episodic; Young Adult; Cues; Spatial Memory; Gestures; Pregnancy; Organ Size; Memory; Hippocampus; Spatial Learning; Motion; Virtual Reality</t>
+          <t>Pregnancy; Memory; Magnetic Resonance Imaging; Functional Neuroimaging; Virtual Reality; Depression; Interpersonal Relations; Parietal Lobe; Temporal Lobe; Neuroimaging; Individuality; Cognitive Science; Learning; Mentoring; Diffusion Magnetic Resonance Imaging; Spatial Navigation; Judgment; Goals; Cognitive Neuroscience; Alzheimer Disease; Computer Simulation; Menopause; Brain; Mentors; Confusion; Gyrus Cinguli; Artificial Intelligence; Cognition; Hippocampus; Memory, Episodic</t>
         </is>
       </c>
     </row>
@@ -633,7 +617,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Medicine; Cells, Cultured; Body Patterning; Feedback, Physiological; Mutation; Mutation Accumulation; Cell Plasticity; Gene Regulatory Networks; Sequence Analysis, DNA; Databases, Factual; Computational Biology; Stochastic Processes; Signal Transduction; Ovary; Gonads; Germ Cells; Software; Chromatin Immunoprecipitation; Single-Cell Analysis; Cell Differentiation; Models, Statistical; Liquid Biopsy; Replication Protein A; Mutation Rate; Noninvasive Prenatal Testing; M Phase Cell Cycle Checkpoints; Computer Simulation; DNA Repair; Cell Self Renewal; Starvation; Aging; Microscopy, Confocal; Gene Expression Regulation, Developmental; Artificial Intelligence; Receptors, Notch; Cell Cycle; Caenorhabditis elegans Proteins; DNA-Binding Proteins; Image Processing, Computer-Assisted; Neoplasms; Imaging, Three-Dimensional; Embryonic Development; Probability; Caenorhabditis elegans; Language; Signal-To-Noise Ratio; Transcription Factors; Colonic Neoplasms; Apoptosis; Algorithms; Cellular Senescence; Neoplastic Stem Cells; Cell Line; DNA Damage; Stem Cell Niche; Bayes Theorem; High-Throughput Screening Assays; Olfactory Mucosa; Blastocyst; Reproduction; Stem Cells; Systems Biology</t>
+          <t>Noninvasive Prenatal Testing; Aging; Neoplasms; Mutation; Systems Biology; Computational Biology; Artificial Intelligence; DNA Damage; Liquid Biopsy</t>
         </is>
       </c>
     </row>
@@ -645,7 +629,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Proteins; Hemoglobinopathies; Pesticides; Students; Furunculosis; Dronabinol; Molecular Sequence Data; Membrane Proteins; Temperature; Hispanic or Latino; Natural Science Disciplines; DNA, Satellite; Genotype; Magnets; Amino Sugars; Molecular Weight; Oligodeoxyribonucleotides; Bacterial Vaccines; Lipids; Medical Marijuana; Seasons; Biological Science Disciplines; Hydrogen; Nitrogen Isotopes; Cell Adhesion; Kinetics; Hydrogen-Ion Concentration; Myoglobin; Cerebral Hemorrhage; Seeds; Carbon-13 Magnetic Resonance Spectroscopy; Mutation; beta-myrcene; Goals; Protein Interaction Maps; Ligands; Drug Development; Amino Acid Sequence; Proton Magnetic Resonance Spectroscopy; Terpenes; Cannabinoids; Oxygen; Plant Extracts; Cannabidiol; Epigenesis, Genetic; caryophyllene oxide; Sequence Homology, Amino Acid; Chromatography, High Pressure Liquid; Erythrocytes; Fertilizers; Molecular Dynamics Simulation; Drug Resistance, Microbial; Sulfolobus; Marijuana Use; Recombinant Proteins; Cannabis; Employment; Oxides; Bacterial Outer Membrane Proteins; Gas Chromatography-Mass Spectrometry; Metabolome; Protein Binding; Magnetic Resonance Spectroscopy; Heinz Bodies; Brain; Genomics; Cellular Senescence; Herbicides; Flavonoids; Microbiota; Imidazoles; Helium; Hemoglobins; Mice, Inbred BALB C; Basic Helix-Loop-Helix Transcription Factors; Magnetic Resonance Imaging; voxelotor; Faculty; DNA-Directed DNA Polymerase; Amino Acids; Anemia, Sickle Cell; Sugars; Adjuvants, Immunologic; Chlamydia muridarum; Carcinogens; Arabidopsis; Neoplasms; Cell Membrane; Water; Ethanol; Information Sources; Chlamydia Infections; Biological Products; Oryza; Archaeal Proteins; Isotopes; Antibodies, Bacterial; Molecular Structure; Bacteria</t>
+          <t>Information Sources; Metabolome; Hemoglobins; Isotopes; Magnetic Resonance Imaging; Arabidopsis; Molecular Structure; Furunculosis; caryophyllene oxide; Microbiota; Hydrogen; Heinz Bodies; Cannabis; voxelotor; Students; Oryza; Seeds; Water; Mutation; Cerebral Hemorrhage; Cannabidiol; Terpenes; Hispanic or Latino; Helium; Drug Resistance, Microbial; Anemia, Sickle Cell; Cannabinoids; Erythrocytes; Marijuana Use; Proteins; Hydrogen-Ion Concentration; Lipids; Drug Development; Neoplasms; Cell Membrane; Dronabinol; Pesticides; Seasons; Membrane Proteins; Genotype; Bacteria; Biological Products; DNA, Satellite; Genomics; Temperature; Biological Science Disciplines; Amino Sugars; Epigenesis, Genetic; Fertilizers; Gas Chromatography-Mass Spectrometry; Chromatography, High Pressure Liquid; Goals; Natural Science Disciplines; Sugars; Medical Marijuana; Amino Acids; Magnetic Resonance Spectroscopy; Cellular Senescence; Cell Adhesion; beta-myrcene; Oxygen; Herbicides; Myoglobin; Protein Interaction Maps; Brain; Employment; Flavonoids; Faculty; Carcinogens; Hemoglobinopathies; Plant Extracts; Recombinant Proteins; Ethanol; Oxides; Magnets</t>
         </is>
       </c>
     </row>
@@ -657,7 +641,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Down-Regulation; Superior Colliculi; Cells, Cultured; In Situ Hybridization; Fatty Acids, Omega-3; Neurons; Synapses; Xenopus laevis; Dendrites; Vesicular Glutamate Transport Proteins; Brain-Derived Neurotrophic Factor; Membrane Proteins; Cell Tracking; Neural Pathways; Cell Differentiation; Amphibians; Immunohistochemistry; Intracellular Signaling Peptides and Proteins; Larva; Docosahexaenoic Acids; Xenopus Proteins; Transfection; Avoidance Learning; Luminescent Proteins; Nerve Growth Factors; Axons; Vesicular Inhibitory Amino Acid Transport Proteins; Anura; Retinal Ganglion Cells; Netrin-1; Microscopy, Confocal; Lipids; Green Fluorescent Proteins; Visual Pathways; Gene Expression Regulation, Developmental; Neurogenesis; Image Processing, Computer-Assisted; Cell Adhesion Molecules; Central Nervous System; Dose-Response Relationship, Drug; Tumor Suppressor Proteins; Morpholinos; Gene Expression; Time Factors; Disks Large Homolog 4 Protein; Photic Stimulation; Pregnancy; Retina; Kinetics</t>
+          <t>Cell Tracking; Axons; Synapses; Amphibians; Dendrites; Neurogenesis</t>
         </is>
       </c>
     </row>
@@ -669,7 +653,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mytilus; Anaerobiosis; Students; Diet; Hot Temperature; Metabolomics; Ecosystem; Academies and Institutes; Homeostasis; Water Movements; Temperature; Enzyme Assays; Body Size; Cellulase; Water Pollutants, Chemical; Acclimatization; Cold Temperature; Respiration; Metabolome; Oxygen; Heat-Shock Response; Protein Denaturation; Research Design; Toxicity Tests, Subacute; Gene Expression; Regression Analysis; Microplastics; Environment; Amylases; Mytilus edulis; Starch</t>
+          <t>Anaerobiosis; Metabolomics; Oxygen; Metabolome; Gene Expression; Heat-Shock Response; Academies and Institutes; Ecosystem; Hot Temperature; Mytilus; Respiration; Homeostasis; Research Design; Students</t>
         </is>
       </c>
     </row>
@@ -681,7 +665,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Neurodevelopmental Disorders; Ear; Evoked Potentials, Auditory, Brain Stem; Vestibule, Labyrinth; Cochlear Nerve; Sphingolipids; Auditory Threshold; Auditory Perception; Autism Spectrum Disorder; Cysteine; Ephrin-A2; Random Allocation; Morphogenesis; Myelin Sheath; GABAergic Neurons; Gene Expression; Postural Balance; Neuronal Plasticity; Cochlear Nucleus; Microglia; Neurons; Synapses; Mutation; Synaptic Transmission; Reaction Time; Peptide Hydrolases; Nervous System; Brain Stem; Fluorescent Antibody Technique; Axons; Trapezoid Body; Caspase 3; Diet, High-Fat; Apoptosis; Insulin Resistance; Mammals; Axon Guidance; Ephrin-A5; Phylogeny; Obesity; Biological Evolution; Gene Deletion; Functional Laterality; Presynaptic Terminals; Exosomes; Oligodendroglia; Tandem Mass Spectrometry; Receptors, Granulocyte-Macrophage Colony-Stimulating Factor; Sex Characteristics; Hearing; Astrocytes; Image Processing, Computer-Assisted; Brain; Mitochondrial Dynamics; Synaptic Potentials; Proteomics; Endopeptidases; Fragile X Syndrome; Acoustic Stimulation; Body Patterning; RNA, Long Noncoding; Rhombencephalon; Dendrites; Caspases; Cell Death; Auditory Pathways; Deafness; gamma-Aminobutyric Acid; Gene Expression Regulation; CX3C Chemokine Receptor 1; Neuroglia; Acoustics; Gene Ontology; Gene Expression Regulation, Developmental; Neurogenesis; Transcriptome; Embryonic Development; Ceramides; Vestibular Nuclei; Chick Embryo; Phenotype; Fragile X Mental Retardation Protein</t>
+          <t>Exosomes; Myelin Sheath; Brain Stem; Endopeptidases; Acoustics; Cochlear Nerve; Axon Guidance; Dendrites; Evoked Potentials, Auditory, Brain Stem; Neurodevelopmental Disorders; Microglia; Astrocytes; Neuroglia; Presynaptic Terminals; Oligodendroglia; Proteomics; Neuronal Plasticity; Peptide Hydrolases; Synapses; Gene Ontology; Axons; Cysteine; Deafness; Hearing; Embryonic Development; Nervous System; Cell Death; Apoptosis; Caspase 3; Brain; Synaptic Transmission; Transcriptome; Tandem Mass Spectrometry; Caspases; Neurons; Auditory Pathways</t>
         </is>
       </c>
     </row>
@@ -693,7 +677,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Connective Tissue; Students; Vertebrates; Elastomers; Conservation of Energy Resources; Chickens; Biophysics; Proprioception; Seizures; Cognition; Rats, Sprague-Dawley; Self-Help Devices; Social Cohesion; Fellowships and Scholarships; Dogs; Algorithms; Muscle, Skeletal; Dancing; Environment; History, 20th Century; Isometric Contraction; Synapses; Running; Interdisciplinary Research; Artificial Limbs; Feedback; Locomotion; Wings, Animal; Dog Diseases; Biomimetics; Walking; Computer Simulation; Tendons; Lumbosacral Region; Invertebrates; Epilepsy; Avatar; Movement; Cross-Sectional Studies; Mentors; Bioengineering; Wearable Electronic Devices; Galliformes; Behavior, Animal; Extremities; Muscle Contraction; Leadership; Biomechanical Phenomena; Feedback, Sensory; Forecasting; Muscles; Exoskeleton Device; Flight, Animal; Surveys and Questionnaires; Robotics; Precipitating Factors; Neuromuscular Diseases; Stress, Mechanical; Spinal Cord; Interneurons; Prostheses and Implants; Mentoring; Communication; Genomics; Universities; Robotic Surgical Procedures; Motor Activity; Biotechnology; Schools; Financial Management; Ownership; Elasticity; Viscosity; Leg; Sports; Faculty; Spinocerebellar Tracts; Birds; History, 21st Century; X-Ray Diffraction; Electromyography; Resilience, Psychological; Information Dissemination; Reflex; Aircraft; Muscle Proteins; Awards and Prizes; Social Media; Air; Chick Embryo; Gait; Motion</t>
+          <t>Locomotion; Muscles; Awards and Prizes; Behavior, Animal; Social Cohesion; Schools; Interdisciplinary Research; Sports; Self-Help Devices; X-Ray Diffraction; Movement; Leadership; Invertebrates; Social Media; Students; Motor Activity; Dancing; Muscle Contraction; Biomechanical Phenomena; Muscle Proteins; Bioengineering; Exoskeleton Device; Robotics; Muscle, Skeletal; Algorithms; Vertebrates; Biophysics; Artificial Limbs; Feedback; Resilience, Psychological; Mentoring; Wearable Electronic Devices; Connective Tissue; Prostheses and Implants; Universities; Neuromuscular Diseases; Financial Management; Communication; Computer Simulation; Fellowships and Scholarships; Faculty; Mentors; Cognition; Biotechnology; Information Dissemination</t>
         </is>
       </c>
     </row>
@@ -705,7 +689,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Transcriptional Activation; Cells, Cultured; Government Regulation; Chromatin; Transcription Factor 7-Like 1 Protein; Induced Pluripotent Stem Cells; Pluripotent Stem Cells; Neurobiology; Wnt Signaling Pathway; Primitive Streak; Signal Transduction; History, 21st Century; Cell Differentiation; CRISPR-Cas Systems; Genetic Engineering; Immunohistochemistry; Microarray Analysis; International Cooperation; Bone Morphogenetic Protein 4; Electrophoresis, Polyacrylamide Gel; Embryology; Proto-Oncogene Proteins c-akt; Genome, Human; Polymerase Chain Reaction; Reproductive Techniques, Assisted; Protein Binding; Ribonucleoproteins; Cell Lineage; Embryonic Stem Cells; Gene Expression; Kruppel-Like Factor 4; Proteome; Congresses as Topic; Retroelements; Mass Spectrometry; Cell Line; Developmental Biology; Consensus; Embryo Research; United States; Immunoprecipitation; Human Embryonic Stem Cells; History, 20th Century; Cellular Reprogramming; Stem Cells; Germ-Line Mutation</t>
+          <t>Neurobiology; Developmental Biology; Retroelements; Embryology; Stem Cells</t>
         </is>
       </c>
     </row>
@@ -717,7 +701,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Gene Expression Regulation, Viral; Herpes Labialis; Drug Resistance, Viral; Viral Proteins; Pandemics; Single-Cell Analysis; Herpesvirus 1, Equid; Single-Cell Gene Expression Analysis; Foscarnet; Encephalitis, Herpes Simplex; Machine Learning; Keratinocytes; Protein Interaction Mapping; SARS-CoV-2; Gene Expression; Genome, Viral; Acyclovir; Keratitis, Herpetic; Host Microbial Interactions; Herpesvirus 1, Human; Virology; DNA, Viral; Mutation; Clustered Regularly Interspaced Short Palindromic Repeats; Zygote; DNA Replication; Virus Replication; Organoids; Epithelial Cells; Vero Cells; COVID-19; Genes, Tumor Suppressor; RNA; Herpes Simplex; Antiviral Agents; Prevalence; Homeodomain Proteins; Ulcer; Herpesviridae; Cell Line; National Institute of Allergy and Infectious Diseases (U.S.); Serial Passage; Infant, Newborn; Skin Diseases, Viral; Virus Diseases; Herpesviridae Infections; Viruses; Chlorocebus aethiops; Cytomegalovirus; Cell Nucleus; Eukaryotic Cells; Cidofovir; Host-Pathogen Interactions; Interferons; Drug Repositioning; Blister; Sequence Analysis, RNA; Orthomyxoviridae; Decitabine; Systems Biology; Ficus; Merkel cell polyomavirus; Transferases; Fibroblasts; Immunocompromised Host; Cell Culture Techniques; Hepatitis C, Chronic; Surgery, Plastic; DNA-Directed DNA Polymerase; Gene Expression Regulation; Methylation; Simplexvirus; Thymidine Kinase; Drug Synergism; Life Cycle Stages; Kaposi Varicelliform Eruption; Preliminary Data; HEK293 Cells; Myelodysplastic Syndromes; Microfluidics; Phenotype</t>
+          <t>Ficus; Acyclovir; Host Microbial Interactions; Surgery, Plastic; Encephalitis, Herpes Simplex; Virus Diseases; Systems Biology; Preliminary Data; Simplexvirus; Skin Diseases, Viral; Herpesvirus 1, Human; Phenotype; Transferases; Cidofovir; RNA; Drug Repositioning; Herpes Simplex; Cell Culture Techniques; Foscarnet; Fibroblasts; Virology; Mutation; DNA, Viral; Pandemics; Herpesvirus 1, Equid; Cytomegalovirus; Microfluidics; Blister; Single-Cell Gene Expression Analysis; Hepatitis C, Chronic; Decitabine; DNA-Directed DNA Polymerase; Methylation; DNA Replication; Herpes Labialis; Clustered Regularly Interspaced Short Palindromic Repeats; Prevalence; Keratitis, Herpetic; Herpesviridae Infections; Life Cycle Stages; Gene Expression; Myelodysplastic Syndromes; Interferons; Keratinocytes; National Institute of Allergy and Infectious Diseases (U.S.); Antiviral Agents; Single-Cell Analysis; Kaposi Varicelliform Eruption; SARS-CoV-2; Host-Pathogen Interactions; Infant, Newborn; Immunocompromised Host; Viruses; Genes, Tumor Suppressor; Epithelial Cells; Machine Learning; Ulcer; Virus Replication; Organoids; Herpesviridae; Thymidine Kinase; Cell Line</t>
         </is>
       </c>
     </row>
@@ -729,7 +713,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Students; Sphingolipids; Proto-Oncogene Proteins B-raf; Cytoskeletal Proteins; Research Report; Nutrients; Morpholines; CRISPR-Cas Systems; Biological Transport; Tumor Microenvironment; Liver; Heterocyclic Compounds, 3-Ring; Amiloride; Lung Neoplasms; Saccharomyces cerevisiae; Autophagy; Biocompatible Materials; Sphingosine; patisiran; Aminopyridines; Enzyme Inhibitors; Energy Metabolism; Endocytosis; Cultural Diversity; Phosphoproteins; Phosphatidylinositol 3-Kinases; Acetals; Karyopherins; Cell Line, Tumor; Fluorouracil; Hydrogen-Ion Concentration; Drug Resistance; Sodium-Hydrogen Exchangers; Intercellular Signaling Peptides and Proteins; Cytoplasm; Metabolic Flux Analysis; Mutation; Lipid Nanoparticles; Codon, Terminator; Protein Phosphatase 2; Allergy and Immunology; Antineoplastic Agents; Oligonucleotides; Amino Acid Transport System y+; Piperazines; Membrane Transport Proteins; Cell Survival; Ligands; Phenothiazines; COVID-19; HeLa Cells; Oncogenes; Lung; Vacuoles; Dose-Response Relationship, Drug; Epigenesis, Genetic; Drosophila; Breast Neoplasms; Endosomes; Diet, High-Fat; Metabolic Networks and Pathways; Congresses as Topic; AMP-Activated Protein Kinases; Cell Transformation, Neoplastic; Asialoglycoprotein Receptor; Structure-Activity Relationship; Insulin Resistance; Cell Line; Mammals; Pinocytosis; Base Pairing; Feasibility Studies; Cells, Cultured; Hot Temperature; COVID-19 Vaccines; Obesity; Gene Deletion; Drug Design; ErbB Receptors; Minority Groups; Signal Transduction; Stress, Physiological; Fatty Acid Synthases; Nucleotides; Leukemia; Phosphatidylinositols; ADP-Ribosylation Factors; Codon, Nonsense; Bridged Bicyclo Compounds, Heterocyclic; Phosphorylation; Fingolimod Hydrochloride; Cytosol; Podocytes; Metabolism; Lysosomes; MCF-7 Cells; Proof of Concept Study; Genomics; Mitochondrial Dynamics; Fusion Regulatory Protein 1, Heavy Chain; PTEN Phosphohydrolase; Class III Phosphatidylinositol 3-Kinases; Plague; Proteomics; Schools; Oxazines; New York City; Microfilament Proteins; Ficus; Polypharmacology; Polyethylene Glycols; Mitochondria; Mixed Function Oxygenases; Proto-Oncogene Proteins p21(ras); Faculty; Gene Expression Regulation; ADP-Ribosylation Factor 6; Drug Resistance, Neoplasm; Vacuolar Proton-Translocating ATPases; RNA, Small Interfering; Kidney Glomerulus; LIM Domain Proteins; Oligonucleotides, Antisense; Neoplasms; Kidney; Preliminary Data; Cell Membrane; Ribosomes; Antimetabolites, Antineoplastic; Ceramides; Transcription Factors; Prostatic Neoplasms; Alleles; Adaptor Proteins, Signal Transducing; Drug Screening Assays, Antitumor; Molecular Structure; Hepatocytes</t>
+          <t>Ficus; RNA, Small Interfering; Alleles; Drug Resistance; Ligands; Hot Temperature; Preliminary Data; COVID-19; Oligonucleotides, Antisense; Endocytosis; Sphingolipids; Diet, High-Fat; Obesity; Plague; Transcription Factors; Codon, Nonsense; patisiran; Nutrients; Cytosol; Oncogenes; Sphingosine; Hepatocytes; Allergy and Immunology; Feasibility Studies; Proto-Oncogene Proteins B-raf; Neoplasms; Cell Membrane; Metabolism; Polypharmacology; Nucleotides; Liver; Intercellular Signaling Peptides and Proteins; Genomics; Protein Phosphatase 2; Karyopherins; Tumor Microenvironment; Ribosomes; Lipid Nanoparticles; COVID-19 Vaccines; Base Pairing; Oligonucleotides; Codon, Terminator; Lung Neoplasms; ErbB Receptors; CRISPR-Cas Systems; Proof of Concept Study; Mitochondria; Saccharomyces cerevisiae; Asialoglycoprotein Receptor; Proto-Oncogene Proteins p21(ras); Lysosomes; Lung; Prostatic Neoplasms</t>
         </is>
       </c>
     </row>
@@ -741,7 +725,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Diet; Chromatin; Malaria; Gene Regulatory Networks; DNA, Satellite; Introduced Species; DNA Transposable Elements; Rhodopsin; Snakes; Gene Expression; Heterozygote; Enhancer Elements, Genetic; Genetic Markers; Gene Frequency; Evolution, Molecular; Polymorphism, Single Nucleotide; High-Throughput Nucleotide Sequencing; Genome, Insect; Mosquito Vectors; DNA Copy Number Variations; Genetic Variation; Adaptation, Biological; Digestion; Computational Biology; Software; Species Specificity; Sex Chromosomes; Genome, Mitochondrial; Genes; Genetics; Chromatin Assembly and Disassembly; Epigenesis, Genetic; Euchromatin; Drosophila; Ecological and Environmental Phenomena; Drosophila simulans; Gene Expression Profiling; Cell Line; Gene Duplication; Mammals; Herbivory; Inheritance Patterns; Phylogeny; Biological Evolution; Fruit; Sequence Analysis, DNA; Eye; Genomic Structural Variation; Mosaicism; Opsins; Quantitative Trait Loci; Genome; Molecular Sequence Annotation; Genes, Duplicate; Butterflies; Color Vision; Genomics; Kynurenine 3-Monooxygenase; Anopheles; Gene Library; Drosophila melanogaster; RNA, Guide, CRISPR-Cas Systems; Genome, Plant; Drosophila Proteins; Fishes; Gene Expression Regulation; Genetics, Population; Insecticide Resistance; INDEL Mutation; Boidae; Sensory Receptor Cells; Selection, Genetic; Sensation; Heterochromatin; Green Fluorescent Proteins; Genome-Wide Association Study; Oviposition; Adaptation, Physiological; Oryza; Cues; Alleles; Molecular Conformation; Models, Genetic; CRISPR-Associated Protein 9; Domestication; Phenotype</t>
+          <t>Genomic Structural Variation; Gene Expression; Ecological and Environmental Phenomena; Genomics; Biological Evolution; Computational Biology; Genetics; Genetics, Population; High-Throughput Nucleotide Sequencing; Genome; Genes</t>
         </is>
       </c>
     </row>
@@ -753,7 +737,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Cell Communication; Pseudopodia; Muscles; Zebrafish; Macrophages; Cell Surface Extensions; Cell Shape; Extracellular Vesicles; Drosophila Proteins; Wnt Signaling Pathway; Signal Transduction; Endoderm; Biological Transport; Neoplasm Proteins; Organ Specificity; Matrix Metalloproteinase 9; Cytoplasmic Vesicles; Keratinocytes; Pigments, Biological; Drosophila; Neoplasms, Experimental; Connexins; Diffusion; Insulin-Like Growth Factor Binding Proteins; Wnt1 Protein; Drosophila melanogaster</t>
+          <t>Cell Surface Extensions; Macrophages; Pseudopodia; Pigments, Biological; Signal Transduction; Keratinocytes; Zebrafish; Extracellular Vesicles; Cell Communication; Connexins</t>
         </is>
       </c>
     </row>
@@ -765,7 +749,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Social Conditions; Carbon; Acer; Students; Photochemical Processes; Climate Change; Liquidambar; Mycorrhizae; Humans; Atmosphere; Ecosystem; Trees; Hot Temperature; Metabolomics; Los Angeles; Endophytes; Soil; Alabama; Feedback; Environmental Monitoring; Remote Sensing Technology; Ozone; Crops, Agricultural; Temperature; Carbon Dioxide; Wettability; Pacific Ocean; Acyclic Monoterpenes; Citizen Science; Goals; Poaceae; Models, Chemical; Oxidation-Reduction; Forests; Pilot Projects; Internship and Residency; Monoterpenes; Isomerism; Computer Simulation; Literacy; Terpenes; Environmental Justice; Resilience, Psychological; Radiation Injuries; Quercus; Air Pollution; Oxygen; Volatile Organic Compounds; Air Pollutants; Photosynthesis; Rhizosphere; Sesquiterpenes; Dehydration; Plants; Seasons; Droughts; Fossil Fuels; Colorado; Ecological and Environmental Phenomena; Aerosols; Curriculum; Environmental Pollutants; Bicyclic Monoterpenes; China; Plant Physiological Phenomena; Artemisia; Plant Leaves; Greenhouse Gases; Cities; Prognosis; Mortality, Premature; Schools; Drought Resistance; Demography</t>
+          <t>Metabolomics; Remote Sensing Technology; Rhizosphere; Photosynthesis; Schools; Los Angeles; Hot Temperature; Crops, Agricultural; Acer; Students; Forests; Plant Leaves; Air Pollution; Trees; Wettability; Atmosphere; Liquidambar; Ecological and Environmental Phenomena; Environmental Justice; Cities; Aerosols; Carbon; Plant Physiological Phenomena; Internship and Residency; Prognosis; Fossil Fuels; Mortality, Premature; Carbon Dioxide; Seasons; Environmental Pollutants; Feedback; Alabama; Mycorrhizae; Pilot Projects; Literacy; Soil; Resilience, Psychological; Dehydration; Colorado; Ecosystem; Temperature; Goals; Volatile Organic Compounds; Droughts; Artemisia; Ozone; Poaceae; Plants; Oxygen; Curriculum; Quercus; Social Conditions; Pacific Ocean; Citizen Science; Computer Simulation; Demography; Air Pollutants; Greenhouse Gases; Endophytes; Humans; Drought Resistance; Climate Change; Radiation Injuries</t>
         </is>
       </c>
     </row>
@@ -777,7 +761,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Theta Rhythm; Acoustic Stimulation; Leadership; Electrodes, Implanted; Computers; Neurons; Adolescent; Technology; Aged, 80 and over; Government; Substance-Related Disorders; Serial Learning; Auditory Perception; Stereotaxic Techniques; Rats, Long-Evans; Nerve Net; Computer Simulation; Prefrontal Cortex; Neuropsychological Tests; Cognition; Aging; Machine Learning; Aged; Mental Recall; Normal Distribution; Pattern Recognition, Visual; Academia; Image Processing, Computer-Assisted; Cluster Analysis; CA1 Region, Hippocampal; Smell; Brain; Electrophysiology; Memory, Episodic; Algorithms; Behavior, Animal; Memory Disorders; Young Adult; Time Factors; Decision Making; Olfactory Perception; Planning Techniques; Time; Odorants; Memory; Hippocampus; Perirhinal Cortex; Behavior</t>
+          <t>Time; Planning Techniques; Behavior; Brain; Academia; Computers; Memory; Electrophysiology; Technology; Cognition; Leadership; Hippocampus; Prefrontal Cortex; Memory, Episodic; Substance-Related Disorders; Algorithms; Government; Decision Making</t>
         </is>
       </c>
     </row>
@@ -789,7 +773,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Angiotensin-Converting Enzyme 2; Chromatin; Social Behavior; Dronabinol; Quality of Life; Nicotine; Allosteric Regulation; Receptors, Nicotinic; Cognition; Tobacco Use Disorder; Interpeduncular Nucleus; DNA Helicases; Rats, Sprague-Dawley; Xenograft Model Antitumor Assays; Dopamine; Medulloblastoma; Protein Transport; Therapeutics; Mass Spectrometry; Cell Line, Tumor; DNA, Complementary; United States; Cholinergic Neurons; Memory; Lynx; Nucleus Accumbens; Neurons; Vision, Ocular; Recurrence; Extracellular Vesicles; Synaptic Transmission; Clustered Regularly Interspaced Short Palindromic Repeats; RNA Helicases; Self Administration; Substance-Related Disorders; Administration, Inhalation; Analgesics, Opioid; Antineoplastic Agents; Tobacco Use; Goals; Hydrocarbons, Brominated; National Eye Institute (U.S.); Poly-ADP-Ribose Binding Proteins; Marketing; Pyrazoles; COVID-19; Lung; Cannabidiol; Epigenesis, Genetic; Ventral Tegmental Area; MicroRNAs; alpha7 Nicotinic Acetylcholine Receptor; Aerosols; Cerebellar Neoplasms; Apoptosis; Behavior, Animal; Habenula; Alcohol Drinking; In Situ Hybridization, Fluorescence; Pregnancy; Cytoplasmic Granules; Hippocampus; Behavior; Isoxazoles; Adolescent; Eating; Signal Transduction; Tobacco Use Cessation Devices; Receptor, Cannabinoid, CB1; Cannabis; Social Environment; Receptors, Purinergic P2; Huntington Disease; Prefrontal Cortex; Indole Alkaloids; Sex Characteristics; DNA-Binding Proteins; Prenatal Exposure Delayed Effects; Cocaine; Mice; Menthol; Brain; Genomics; Protein Isoforms; Substance Withdrawal Syndrome; Adenosine Triphosphate; E-Cigarette Vapor; Cell Movement; Consummatory Behavior; Proteomics; Craving; Biomedical Research; Dopaminergic Neurons; Rodentia; Electronic Nicotine Delivery Systems; Brain-Derived Neurotrophic Factor; Alcoholism; Nicotinic Agonists; Smoking; RNA Recognition Motif Proteins; Tobacco Products; Microscopy; Ethanol; Learning; Smoking Cessation; Electrophysiology; Child; Vaping; Eye Diseases</t>
+          <t>Lynx; Microscopy; Eating; Memory; E-Cigarette Vapor; Receptors, Nicotinic; Sex Characteristics; Dopaminergic Neurons; Dopamine; Cannabis; Electronic Nicotine Delivery Systems; Nucleus Accumbens; Analgesics, Opioid; Cocaine; Craving; Electrophysiology; Tobacco Use Disorder; Mice; Therapeutics; Alcoholism; Extracellular Vesicles; Clustered Regularly Interspaced Short Palindromic Repeats; Learning; Substance Withdrawal Syndrome; Social Behavior; Chromatin; Genomics; Epigenesis, Genetic; Marketing; Recurrence; Self Administration; Goals; Substance-Related Disorders; Nicotine; Behavior; Brain; Rodentia; Ethanol; Menthol; Ventral Tegmental Area; Brain-Derived Neurotrophic Factor; Consummatory Behavior; Social Environment; Alcohol Drinking</t>
         </is>
       </c>
     </row>
@@ -801,7 +785,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Inheritance Patterns; Students; Social Evolution; X Chromosome; Ergonomics; Ecosystem; Mutation; Biological Evolution; Life History Traits; Communicable Diseases; Neurobiology; Computational Biology; Software; Genetics, Population; Genotype; Access to Information; Public Health; Genetic Drift; Selection, Genetic; Computer Simulation; Immune System; Molecular Epidemiology; Immune System Diseases; Genetics; Host-Parasite Interactions; Artificial Intelligence; Neoplasms; Epigenesis, Genetic; Ecological and Environmental Phenomena; Disease; Language; Gene Expression; Natural Language Processing; Systems Biology; Sexual Behavior, Animal; Microbiota; Data Analysis; Evolution, Molecular; Cities; Models, Genetic; Chromosomes; Immunologic Factors; Cell Biology; Phenotype; Bacteria; Logic</t>
+          <t>Access to Information; Systems Biology; Microbiota; Computational Biology; Molecular Epidemiology; Students; Software; Ecological and Environmental Phenomena; Ergonomics; Public Health; Neoplasms; Social Evolution; Gene Expression; Biological Evolution; Host-Parasite Interactions; Selection, Genetic; Life History Traits; Computer Simulation; Neurobiology; Logic; Artificial Intelligence; Genetics; Genetics, Population; Genetic Drift; Communicable Diseases</t>
         </is>
       </c>
     </row>
@@ -813,7 +797,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Principal Component Analysis; Collateral Circulation; Diagnostic Imaging; Stroke; Action Potentials; Magnetic Resonance Imaging; Neurons; Biosensing Techniques; Physical Stimulation; Ischemic Stroke; Somatosensory Cortex; Brain Ischemia; Neuroimaging; Rodentia; Glutamic Acid; Reaction Time; gamma-Aminobutyric Acid; Ischemic Attack, Transient; Blood Flow Velocity; Wakefulness; Lactic Acid; Sense Organs; Social Isolation; Neuroprotection; Neurotransmitter Agents; Rats, Inbred SHR; Pharmacology; Head; Spatio-Temporal Analysis; Statistics as Topic; Computer Simulation; Rats, Inbred WKY; Infarction, Middle Cerebral Artery; Hypertension; Middle Cerebral Artery; Astrocytes; Normal Distribution; Rats, Sprague-Dawley; Electroencephalography; Image Processing, Computer-Assisted; Cerebrovascular Circulation; Brain Diseases, Metabolic; Cerebral Cortex; Neural Conduction; Cluster Analysis; Metabolism; Microelectrodes; Brain; Vibrissae; Electrophysiology; Algorithms; Behavior, Animal; Neuronal Plasticity; Anesthetics; United States; Histology; Afferent Pathways; Electric Stimulation</t>
+          <t>Behavior, Animal; Magnetic Resonance Imaging; Brain Diseases, Metabolic; Infarction, Middle Cerebral Artery; Microelectrodes; Stroke; Diagnostic Imaging; Sense Organs; Cerebrovascular Circulation; Ischemic Stroke; United States; Ischemic Attack, Transient; Astrocytes; Electrophysiology; Metabolism; Neuronal Plasticity; Lactic Acid; Social Isolation; Histology; Rodentia; Cerebral Cortex; Pharmacology; Neurons; Middle Cerebral Artery</t>
         </is>
       </c>
     </row>
@@ -825,7 +809,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Sterol Regulatory Element Binding Protein 2; Cell Proliferation; Mevalonic Acid; Diet; Staff Development; Macrophages; Research Personnel; Hydroxymethylglutaryl-CoA Reductase Inhibitors; Eukaryotic Initiation Factor-4E; Nutrients; Biosynthetic Pathways; Biological Transport; Blast Crisis; Hispanic or Latino; Sirolimus; Cobalt; Gene Dosage; Proteasome Endopeptidase Complex; YAP-Signaling Proteins; Mechanistic Target of Rapamycin Complex 1; Lymphocytes; Myeloid Cell Leukemia Sequence 1 Protein; Lipids; Xenograft Model Antitumor Assays; venetoclax; Neoplastic Processes; Protein Kinase Inhibitors; Lysine; Sterols; Pyrimidines; Gene Expression; Endocytosis; Phosphatidylinositol 3-Kinases; Standard of Care; Cell Line, Tumor; United States; GTP Phosphohydrolases; Mice, Nude; High-Throughput Nucleotide Sequencing; pitavastatin; Organelles; Antineoplastic Combined Chemotherapy Protocols; Prospective Studies; Mechanistic Target of Rapamycin Complex 2; Whole Genome Sequencing; Mutation; Recurrence; Clustered Regularly Interspaced Short Palindromic Repeats; Protein Prenylation; Polycomb Repressive Complex 1; Health Inequities; Fasting; National Institutes of Health (U.S.); Eukaryotic Initiation Factor-4F; Quinolines; Antineoplastic Agents; Oligonucleotides; Publishing; Chromatin Immunoprecipitation; Triple Negative Breast Neoplasms; Goals; Cell Survival; Mechanotransduction, Cellular; Polycomb Repressive Complex 2; Imatinib Mesylate; Philadelphia Chromosome; Precursor B-Cell Lymphoblastic Leukemia-Lymphoma; Lymphoma, B-Cell; Terpenes; Molecular Targeted Therapy; Cell Cycle Checkpoints; Proteolysis; Dasatinib; Diterpenes; Apoptosis Regulatory Proteins; Epigenesis, Genetic; Endosomes; Enhancer of Zeste Homolog 2 Protein; Metabolic Networks and Pathways; Leukemia, Myelogenous, Chronic, BCR-ABL Positive; Apoptosis; AMP-Activated Protein Kinases; Mice, Inbred NOD; Cell Line; Histones; Catalysis; Tyrosine Kinase Inhibitors; Glutamine; Pinocytosis; Precursor Cell Lymphoblastic Leukemia-Lymphoma; Multiple Myeloma; Prenylation; Feeding Behavior; Exome Sequencing; Proto-Oncogene Proteins c-bcl-2; Adolescent; Data Interpretation, Statistical; Ubiquitin; Sulfonamides; Reperfusion Injury; ruxolitinib; Retrospective Studies; Communicable Diseases; Protein-Tyrosine Kinases; Guanosine Triphosphate; Signal Transduction; Heterografts; Cell Differentiation; Doxorubicin; Immunosuppressive Agents; Leukemia; Bridged Bicyclo Compounds, Heterocyclic; Phosphorylation; Cholesterol; Extracellular Matrix; Proto-Oncogene Proteins c-akt; Efficiency; Food-Drug Interactions; Quinolones; Drug Repositioning; Tumor Suppressor Protein p53; Phosphoinositide-3 Kinase Inhibitors; Leukemia, Lymphocytic, Chronic, B-Cell; Protein Isoforms; Drug Delivery Systems; Multiprotein Complexes; Prognosis; Mice, Inbred BALB C; Biomarkers; Hematologic Neoplasms; Mitochondria; Melanoma; Cell Death; TOR Serine-Threonine Kinases; Methylation; Interinstitutional Relations; Leukemia, Myeloid, Acute; Drug Resistance, Neoplasm; DNA Methylation; Dietary Supplements; Fusion Proteins, bcr-abl; Mice, SCID; Gene Expression Regulation, Leukemic; Lactams; Janus Kinases; DNA Adducts; Drug Synergism; Heart Diseases; RNA, Small Interfering; Gene Ontology; Up-Regulation; Receptors, Cytokine; Datasets as Topic; Transcriptome; Neoplasms; Oligonucleotides, Antisense; Preliminary Data; Cell Membrane; Survival Rate; Tumor Cells, Cultured; Ubiquitin-Protein Ligases; Farnesyltranstransferase; Transcription Factors; Child; Young Adult; MTOR Inhibitors; Polyisoprenyl Phosphates; Lymphoma; Cytokines; Therapeutic Index; Alkyl and Aryl Transferases; Inflammation</t>
+          <t>Lymphocytes; Prospective Studies; Young Adult; Biosynthetic Pathways; Preliminary Data; Leukemia, Lymphocytic, Chronic, B-Cell; Hematologic Neoplasms; Cytokines; Sirolimus; Cell Cycle Checkpoints; Prognosis; Cell Membrane; Gene Expression; Heart Diseases; TOR Serine-Threonine Kinases; Cell Death; Mitochondria; Protein Prenylation; Dasatinib; Cell Line; Health Inequities; Diet; GTP Phosphohydrolases; Cholesterol; Lymphoma; ruxolitinib; MTOR Inhibitors; Hispanic or Latino; Up-Regulation; Lipids; Precursor Cell Lymphoblastic Leukemia-Lymphoma; Clustered Regularly Interspaced Short Palindromic Repeats; Molecular Targeted Therapy; Antineoplastic Agents; Standard of Care; venetoclax; Child; Fasting; Neoplastic Processes; Transcriptome; Cell Proliferation; Proto-Oncogene Proteins c-bcl-2; Signal Transduction; Heterografts; Drug Repositioning; Transcription Factors; Therapeutic Index; Biomarkers; Mechanistic Target of Rapamycin Complex 1; Cell Survival; Guanosine Triphosphate; Mechanistic Target of Rapamycin Complex 2; Protein-Tyrosine Kinases; Organelles; Philadelphia Chromosome; Mevalonic Acid; Adolescent; Leukemia; Phosphatidylinositol 3-Kinases; Sterols; Tumor Suppressor Protein p53; Apoptosis Regulatory Proteins; AMP-Activated Protein Kinases; Survival Rate; Nutrients; Terpenes; Fusion Proteins, bcr-abl; Receptors, Cytokine; Recurrence; Phosphorylation; Goals; pitavastatin; Apoptosis; Leukemia, Myeloid, Acute; Tyrosine Kinase Inhibitors; Janus Kinases; Hydroxymethylglutaryl-CoA Reductase Inhibitors</t>
         </is>
       </c>
     </row>
@@ -837,7 +821,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Students; Climate Change; Chromatin; DNA; Metagenomics; Protoplasts; Agriculture; Temperature; California; Hispanic or Latino; Genotype; Genetic Drift; DNA Transposable Elements; Gene Expression Regulation, Plant; Climate Models; Droughts; Gene Expression; Heterozygote; Phenomics; Plant Physiological Phenomena; Evolution, Molecular; Polymorphism, Single Nucleotide; Europe; Persea; Drought Resistance; Sphingomonas; Epigenomics; Genetic Variation; Mutation; DNA-Directed RNA Polymerases; Chromosome Mapping; Soil Microbiology; Setaria Plant; Biological Variation, Population; Crops, Agricultural; Parasites; Software; Goals; Altitude; Sorghum; North America; Grassland; Cellulases; Epigenome; Microscopy, Electron, Scanning Transmission; Genetics; Epigenesis, Genetic; Mentors; RNA, Plant; Extreme Weather; Ecological and Environmental Phenomena; MicroRNAs; Zea mays; Tibet; Social Mobility; Demography; Hot Temperature; Ecosystem; Phylogeny; Biological Evolution; Nucleic Acid Conformation; Sequence Analysis, DNA; Molecular Biology; Base Sequence; Stress, Physiological; Genome Size; Genomic Instability; Genetic Fitness; Quantitative Trait Loci; Mentoring; Genomics; Ecology; Microbiota; Rho Factor; Genetic Background; Escherichia coli; Plant Breeding; Escherichia coli Proteins; Histidine Kinase; Genome, Plant; Faculty; Clergy; Genetics, Population; DNA Methylation; Host Specificity; Salt Tolerance; Disease Vectors; RNA, Small Interfering; Genes, Plant; Gene Flow; Genome-Wide Association Study; Plants; Adaptation, Physiological; Oryza; Epistasis, Genetic; China; Alleles; Vitis; Periodicals as Topic; Plant Diseases; Hyperspectral Imaging; Domestication; Phenotype; Xylella</t>
+          <t>Genome, Plant; Alleles; Disease Vectors; Crops, Agricultural; Metagenomics; DNA; Phenotype; Sorghum; Parasites; Students; Base Sequence; Oryza; Persea; Protoplasts; Ecological and Environmental Phenomena; Mutation; Epigenomics; Hispanic or Latino; DNA Transposable Elements; Genomic Instability; Microscopy, Electron, Scanning Transmission; Plant Physiological Phenomena; Tibet; Hyperspectral Imaging; Domestication; Genotype; Altitude; Mentoring; Gene Expression; Genetic Drift; Chromatin; Genomics; Ecosystem; Temperature; MicroRNAs; Climate Models; Epigenesis, Genetic; Biological Evolution; Epigenome; Goals; DNA Methylation; Biological Variation, Population; Droughts; Gene Flow; Genetic Variation; Genome Size; Phylogeny; Phenomics; Salt Tolerance; Stress, Physiological; Plants; Agriculture; Zea mays; Social Mobility; Faculty; Demography; Mentors; Genetics; Extreme Weather; Ecology; Genetics, Population; Drought Resistance; Climate Change; Setaria Plant; Vitis</t>
         </is>
       </c>
     </row>
@@ -849,7 +833,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Mytilus; Reproducibility of Results; Diet; Stomach; Zebrafish; Ecosystem; Leucine; Phylogeny; Eating; Biological Evolution; Digestion; Fishes; Nutrients; Temperature; Lizards; Carbon Isotopes; California; Trypsin; Esters; Fermentation; Diet, Food, and Nutrition; Body Size; Sharks; Perciformes; Alismatales; Digestive System Physiological Phenomena; Carnivory; Cellulases; Animal Husbandry; Acclimatization; Gastropoda; Zebrafish Proteins; Physiology; Cold Temperature; Herbivory; Genetics; Lipase; Fires; Gastrointestinal Microbiome; Cannibalism; Aminopeptidases; alpha-Glucosidases; Heat-Shock Response; Genome; Transcriptome; Skates, Fish; Animal Nutritional Physiological Phenomena; Food Chain; Seasons; Dietary Proteins; Ecological and Environmental Phenomena; Adaptation, Physiological; Genomics; Dietary Fiber; Ovum; Enzymes; Alkaline Phosphatase; Gene Expression Profiling; RNA, Ribosomal, 16S; Microbiota; Intestines; Zinc; Amylases; Chromosomes; Pancreatic alpha-Amylases; Gastrointestinal Tract; Marine Biology</t>
+          <t>Diet; Marine Biology; Physiology; Ecological and Environmental Phenomena; Diet, Food, and Nutrition; Gene Expression Profiling; Fishes; Genomics; Ecosystem; Microbiota; Genetics; Fermentation; Digestion; Enzymes</t>
         </is>
       </c>
     </row>
@@ -861,7 +845,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Receptors, Complement; Cell Proliferation; Deep Learning; Neural Stem Cells; Ubiquitination; Chromatin; Transcription Factor 7-Like 1 Protein; DNA; Viral Proteins; Complement C1q; Wnt Signaling Pathway; Membrane Proteins; Eukaryotic Initiation Factor-4E; Ankyrin Repeat; Giant Viruses; Tumor Microenvironment; Coculture Techniques; Lymphocytic choriomeningitis virus; Tissue Scaffolds; Phosphoric Monoester Hydrolases; Disease Outbreaks; RNA, Viral; Proteasome Endopeptidase Complex; Gene Expression Regulation, Plant; Morphogenesis; Haplorhini; Cell Transplantation; Poliovirus; Protein Transport; Colonic Neoplasms; DNA Viruses; Genome, Viral; A549 Cells; Vaccines; Mass Spectrometry; Cell Line, Tumor; Evolution, Molecular; Nucleoproteins; Cytoplasm; Virology; Vaccinia; DNA-Directed RNA Polymerases; Induced Pluripotent Stem Cells; Protein Processing, Post-Translational; RNA Helicases; Computational Biology; Virus Replication; Myocytes, Cardiac; Triple Negative Breast Neoplasms; Chloroplasts; Epithelial Cells; Arabidopsis Proteins; Immunity, Innate; Peptides; Amino Acid Sequence; Proteolysis; HeLa Cells; Lung; Virion; Apoptosis Regulatory Proteins; Uridine; RNA, Plant; Antiviral Agents; Microscopy, Fluorescence; Smallpox; Breast Neoplasms; Zea mays; Cell Line; Models, Molecular; Ribosomal Proteins; Antigens, Differentiation; Nuclear Proteins; Cells, Cultured; Neovascularization, Pathologic; Technology; Phylogeny; Obesity; Poxviridae; Nucleic Acid Conformation; Culture Media, Conditioned; Signal Transduction; Spinal Cord Injuries; Cell Differentiation; Hyaluronan Receptors; Tandem Mass Spectrometry; Genome Size; Cell Nucleus; Phosphorylation; Extracellular Matrix; Open Reading Frames; Eukaryotic Cells; Allografts; Kalinin; Host-Pathogen Interactions; Protein Binding; Cell Adhesion Molecules; Adipose Tissue; MCF-7 Cells; Protein C; Rhinovirus; Proteome; Cattle; Transcription, Genetic; Adipogenesis; Cell Movement; Proteomics; Systems Biology; Viral Replication Compartments; Escherichia coli; Conserved Sequence; RNA, Messenger; Myocardium; Genes, Viral; Rodentia; Binding Sites; Poliomyelitis; Intracellular Signaling Peptides and Proteins; RNA Editing; Protein Biosynthesis; Mimiviridae; Arabidopsis; Vaccinia virus; Artificial Intelligence; Fascia; Ankyrins; Active Transport, Cell Nucleus; Recombination, Genetic; Membrane Glycoproteins; PTB-Associated Splicing Factor; Tumor Cells, Cultured; Mpox (monkeypox); Viral Fusion Proteins; HEK293 Cells; DNA Damage; Adaptor Proteins, Signal Transducing; Human Embryonic Stem Cells; Cytidine; RNA-Binding Proteins</t>
+          <t>Systems Biology; DNA; Escherichia coli; Vaccines; Virology; Mass Spectrometry; Vaccinia; Viral Replication Compartments; Membrane Proteins; Vaccinia virus; Smallpox; Proteome; Virion; Antiviral Agents; Disease Outbreaks; Mpox (monkeypox); Morphogenesis; Protein C; Technology; Artificial Intelligence; Poxviridae; Cell Nucleus; Proteomics</t>
         </is>
       </c>
     </row>
@@ -873,7 +857,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Virulence; Aged, 80 and over; Amyloid; Epitopes; Amyloid beta-Peptides; Protein Array Analysis; Amyloidogenic Proteins; Low Density Lipoprotein Receptor-Related Protein-1; Antibodies, Monoclonal; Hypertension; Synaptosomes; Aging; Cognition; Myocardial Ischemia; Protein Multimerization; Aminopyridines; Cerebral Cortex; Particle Size; CA1 Region, Hippocampal; Energy Metabolism; Protein Aggregates; Statistics, Nonparametric; Algorithms; Vaccines; Neuronal Plasticity; Apolipoproteins E; Microtomy; Mass Spectrometry; Cell Line, Tumor; United States; Polymorphism, Single Nucleotide; Memory; High-Throughput Nucleotide Sequencing; Receptors, LDL; Microglia; PC12 Cells; Neurons; Synapses; Hypoglycemic Agents; Mutation; Neurodegenerative Diseases; Protein Processing, Post-Translational; Computational Biology; Allergy and Immunology; Proteostasis; Myocytes, Cardiac; Nootropic Agents; Goals; Peptide Library; Single-Chain Antibodies; Immunity, Innate; alpha-Crystallins; Peptides; Peptide Fragments; Amino Acid Sequence; Mutagenesis, Site-Directed; Crystallography, X-Ray; Aged; Adaptive Immunity; Microscopy, Electron, Transmission; Drosophila; tau Proteins; Endosomes; Catechin; Islet Amyloid Polypeptide; Synucleins; Protein Conformation, beta-Strand; Pressure; Pregnancy; Models, Molecular; Hippocampus; Amino Acid Substitution; Cells, Cultured; Single-Domain Antibodies; Drug Design; Glutamic Acid; Communicable Diseases; Pre-Eclampsia; Calcium; Genetic Vectors; Autophagosomes; Recombinant Proteins; Alzheimer Disease; Dependovirus; Phosphorylation; Receptors, Granulocyte-Macrophage Colony-Stimulating Factor; Plaque, Amyloid; Epitope Mapping; Positron-Emission Tomography; Antibody Specificity; Antibodies; Protein Binding; Lysosomes; Brain; Supranuclear Palsy, Progressive; Congo Red; Disks Large Homolog 4 Protein; Immunity; Neurofibrillary Tangles; Infant; Heart Failure; Mitochondria; Binding Sites; Protein Conformation; Brain-Derived Neurotrophic Factor; Indicators and Reagents; Amino Acids; Insulin-Secreting Cells; Amyloid beta-Protein Precursor; Glutathione; Pyrroles; Immunohistochemistry; Protein Folding; Protein Aggregation, Pathological; Bacteriophages; Phosphatidylinositol-3,4,5-Trisphosphate 5-Phosphatases; Immunotherapy; Protein Biosynthesis; Maze Learning; Desmin; Ribosomes; Gene Transfer Techniques; HEK293 Cells; beta-Crystallins; Proteinuria; Adaptor Proteins, Signal Transducing; Serum Amyloid A Protein; Molecular Structure; Apolipoprotein E4</t>
+          <t>Amyloidogenic Proteins; Peptides; Antibodies; Synucleins; Epitopes; Virulence; Immunotherapy; Bacteriophages; United States; Vaccines; Indicators and Reagents; Allergy and Immunology; High-Throughput Nucleotide Sequencing; Algorithms; Antibody Specificity; Brain-Derived Neurotrophic Factor; Serum Amyloid A Protein; Adaptive Immunity; Amyloid; Statistics, Nonparametric; Goals; Antibodies, Monoclonal; Amino Acids; Neurodegenerative Diseases; Alzheimer Disease; Protein Conformation, beta-Strand; Aging; Brain; Immunity, Innate; Cognition; Immunity; Communicable Diseases</t>
         </is>
       </c>
     </row>
@@ -885,7 +869,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Proteins; Molecular Dynamics Simulation; Deep Learning; Organometallic Compounds; Apoproteins; Negative Staining; Binding Sites; Protein Conformation; Homeostasis; Conus Snail; Eye; Cation Transport Proteins; Membranes; Protein Domains; Protein Folding; Computer Systems; Cobalt; Heart; Proteolysis; Microscopy; Crystallography, X-Ray; Ferroportin; Image Processing, Computer-Assisted; Neoplasms; Single Molecule Imaging; Cryoelectron Microscopy; Algorithms; Biochemistry; Hepcidins; Multiprotein Complexes; Models, Molecular; Molecular Structure; Iron; Conotoxins</t>
+          <t>Protein Folding; Microscopy; Molecular Structure; Cryoelectron Microscopy; Eye; Membranes; Heart; Biochemistry; Neoplasms</t>
         </is>
       </c>
     </row>
@@ -897,7 +881,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Proteins; Uracil; Yersinia; Protein Sorting Signals; Uridine Kinase; Bacterial Toxins; Macrophages; Citric Acid Cycle; Nucleoside-Phosphate Kinase; Carrier Proteins; Virulence; Glycation End Products, Advanced; Membrane Proteins; Nutrients; Tuberculosis; Pandemics; Coculture Techniques; Lipid Metabolism; Protein Domains; Bacterial Secretion Systems; Necrosis; NIH 3T3 Cells; Heme; Sequence Analysis, Protein; Latent Tuberculosis; Enzyme Inhibitors; Lysine; RNA, Bacterial; Endonucleases; Electron Transport Complex IV; Protein Interaction Mapping; Hemagglutinins; Arginine; Deoxyuridine; Vaccines; Bacterial Proteins; Mass Spectrometry; Chemokines; Evolution, Molecular; Biliverdine; Kinetics; Mycobacterium tuberculosis; Drug Discovery; Heme Oxygenase (Decyclizing); Protein Processing, Post-Translational; Computational Biology; Parasites; Software; Membranes; Ribonucleases; Goals; Ligands; RNA, Transfer; Substrate Specificity; Cytochromes c; Amino Acid Sequence; Mutagenesis, Site-Directed; Proteolysis; HeLa Cells; RNA; Crystallography, X-Ray; Antigens, Bacterial; Guanine; Uridine; Vaccination; Metabolic Networks and Pathways; Structure-Activity Relationship; Biochemistry; Models, Molecular; Azides; Phagosomes; Carbon; Molecular Dynamics Simulation; Infant, Newborn; Endoribonucleases; Nucleic Acid Conformation; Trypanosoma cruzi; Communicable Diseases; Molecular Biology; Cholesterol; Eukaryotic Cells; Mycobacteriaceae; Isotope Labeling; Klebsiella pneumoniae; Nucleosides; Host-Pathogen Interactions; Toxin-Antitoxin Systems; Glycerol; Anti-Bacterial Agents; Glyoxylates; Protein Binding; Pertussis Vaccine; Bordetella pertussis; Colicins; Cattle; Virulence Factors; Hemoglobins; Whooping Cough; Escherichia coli; Infant; Escherichia coli Proteins; Alanine Dehydrogenase; Histidine Kinase; Electrons; Ribonuclease, Pancreatic; Type VII Secretion Systems; Binding Sites; Catalytic Domain; Bacteriological Techniques; Protein Conformation; Siderophores; Peptide Elongation Factor Tu; Recombinant Fusion Proteins; Protein Folding; Multigene Family; Pyruvaldehyde; RNA, Small Interfering; Biotinylation; Arabidopsis; Disulfides; Toxins, Biological; Protein Engineering; Water; Cryoelectron Microscopy; Enterobacter cloacae; BCG Vaccine; HEK293 Cells; Molecular Structure; Tomography, X-Ray Computed; Iron; Phenotype; Bacteria</t>
+          <t>Iron; Latent Tuberculosis; Hemoglobins; Molecular Structure; Ligands; Histidine Kinase; Carrier Proteins; Protein Interaction Mapping; Virulence; Electrons; Nutrients; Mass Spectrometry; Pandemics; Biliverdine; Hemagglutinins; Virulence Factors; Vaccination; Pertussis Vaccine; Proteins; Anti-Bacterial Agents; Heme; Bordetella pertussis; Protein Sorting Signals; Mycobacterium tuberculosis; Tuberculosis; Bacteria; Cryoelectron Microscopy; Infant; Goals; Eukaryotic Cells; Molecular Biology; Heme Oxygenase (Decyclizing); Infant, Newborn; Tomography, X-Ray Computed; Toxins, Biological; Whooping Cough; Communicable Diseases; Biochemistry</t>
         </is>
       </c>
     </row>
@@ -909,7 +893,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Macrophages; ATP-Binding Cassette Transporters; Gene Regulatory Networks; Aged, 80 and over; Amyloid; Pandemics; Single-Cell Analysis; Genotype; Trimethoprim; Amyloid beta-Peptides; Risk Factors; Mutation, Missense; Bone Marrow; Cystatins; Double-Blind Method; Gene Knock-In Techniques; Monocytes; Cognition; Aging; Demyelinating Diseases; Tauopathies; SARS-CoV-2; NLR Family, Pyrin Domain-Containing 3 Protein; Gene Expression; Apolipoproteins E; Microglia; RNA Splicing; Neurons; Synapses; Metabolomics; Disease Progression; Mutation; Genetic Variation; Genes, fms; Cuprizone; COVID-19; Aged; Myeloid Cells; Down Syndrome; tau Proteins; Breast Neoplasms; Neuroinflammatory Diseases; Gene Expression Profiling; White Matter; Receptors, Immunologic; Murine hepatitis virus; Coronavirus Infections; Homeostasis; Alzheimer Disease; Cell Nucleus; Phosphorylation; Receptors, Granulocyte-Macrophage Colony-Stimulating Factor; Brain Neoplasms; Macrophage Colony-Stimulating Factor; Plaque, Amyloid; Sex Characteristics; Astrocytes; Proof of Concept Study; Brain; Treatment Outcome; Niacinamide; Microbiota; Cell Communication; Biomarkers; Dendrimers; Phagocytosis; Nerve Degeneration; Neurites; Amyloid beta-Protein Precursor; Neuroglia; Resilience, Psychological; Vitamin B Complex; Immunotherapy; Gastrointestinal Microbiome; Remyelination; Transcriptome; Membrane Glycoproteins; Central Nervous System Diseases; Nerve Regeneration</t>
+          <t>Macrophage Colony-Stimulating Factor; Immunotherapy; Microglia; Bone Marrow; Myeloid Cells; Nerve Regeneration; Macrophages; Gene Expression; Synapses; Trimethoprim; Monocytes; Disease Progression; Amyloid; Homeostasis; Central Nervous System Diseases; Alzheimer Disease; Aging; Brain; Gene Expression Profiling; Genes, fms; Nerve Degeneration; Cell Proliferation; NLR Family, Pyrin Domain-Containing 3 Protein; Cognition; Neurons; Neurites</t>
         </is>
       </c>
     </row>
@@ -921,7 +905,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Proteins; Cell Proliferation; Nonheme Iron Proteins; Lewis Acids; Genetic Predisposition to Disease; Aged, 80 and over; Spectrum Analysis, Raman; Risk Factors; Candidemia; Cysteine; Heme; Gene Expression Regulation, Neoplastic; Administration, Intravenous; Cerebral Cortex; Nitrogen Fixation; SARS-CoV-2; Candidiasis, Invasive; Polymorphism, Single Nucleotide; Histidine; Evoked Potentials; Chloride Peroxidase; Protons; Density Functional Theory; Bias; Mutation; Triazoles; Dioxygenases; Ligands; Hydroxides; Oxidation-Reduction; Amino Acid Sequence; Ferric Compounds; COVID-19; Crystallography, X-Ray; Oxygen; Psychotic Disorders; Metals; Hydrogen Bonding; Vaccination; Iron Compounds; Apoptosis; Nitric Oxide; Coordination Complexes; Catalysis; Cytochromes; Models, Molecular; Psychomotor Performance; Child, Preschool; Serine; Adolescent; Biomarkers, Tumor; Communicable Diseases; X-Ray Absorption Spectroscopy; Cytochrome b Group; Proto-Oncogene Proteins c-jun; Nitrogen; Ammonia; Oxides; Feedback, Psychological; Logistic Models; Protein Binding; Magnetic Resonance Spectroscopy; Genomics; B7-H1 Antigen; Cohort Studies; Treatment Outcome; Metalloproteins; Prognosis; Schizophrenia; Metals, Heavy; Electron Transport; Thermodynamics; Mitogen-Activated Protein Kinase 8; Infant; Escherichia coli; Affective Disorders, Psychotic; RNA, Messenger; Escherichia coli Proteins; Electrons; Binding Sites; Catalytic Domain; Infectious Disease Medicine; Antifungal Agents; Ascorbate Peroxidases; Cytochrome P-450 Enzyme System; Cytidine Deaminase; Genome-Wide Association Study; Disulfides; Protein Engineering; Neoplasms; Tumor Cells, Cultured; Hemeproteins; Chemistry, Bioinorganic; Child; Alleles; Nitrogenase; Electron Spin Resonance Spectroscopy; Molecular Structure; Molecular Conformation; Executive Function; Iron</t>
+          <t>Catalysis; Cytochrome P-450 Enzyme System; Electrons; Hemeproteins; Electron Transport; Ligands; X-Ray Absorption Spectroscopy; Cytochromes; Thermodynamics; Chemistry, Bioinorganic; Metals; Metalloproteins; Spectrum Analysis, Raman; Bias</t>
         </is>
       </c>
     </row>
@@ -933,7 +917,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>White; Medicaid; Biomarkers; Clinical Trials, Phase II as Topic; Philippines; Adolescent; Drug-Related Side Effects and Adverse Reactions; American Indian or Alaska Native; Vietnam; Racial Groups; Data Collection; Focus Groups; Aged, 80 and over; Amyloid; Medicare; California; Research Subjects; Cognitive Dysfunction; Disease Management; Hispanic or Latino; Black or African American; Alzheimer Disease; Disclosure; Motivation; Amyloid beta-Peptides; Clinical Trials, Phase III as Topic; Phosphorylation; Republic of Korea; Amyloidogenic Proteins; Patient Selection; Exercise; Vitamin B Complex; Double-Blind Method; Asian; Aging; Insurance Coverage; Positron-Emission Tomography; Clinical Trials as Topic; Aged; Ethnicity; Proof of Concept Study; tau Proteins; Brain; Registries; Young Adult; Treatment Outcome; Niacinamide; Randomized Controlled Trials as Topic; Prognosis; United States; Antibodies, Monoclonal, Humanized; Centers for Medicare and Medicaid Services, U.S.</t>
+          <t>Alzheimer Disease; Clinical Trials as Topic; Research Subjects</t>
         </is>
       </c>
     </row>
@@ -945,21 +929,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Proteins; Vancomycin; DNA, Bacterial; Kinesins; Adjuvants, Pharmaceutic; Macrophages; DNA; Carrier Proteins; Biological Transport; Microtubule-Associated Proteins; Biophysics; Optical Tweezers; Protein Domains; Saccharomyces cerevisiae; Anti-Infective Agents; Protein Transport; Mitosis; Molecular Motor Proteins; Cell Line, Tumor; GTP Phosphohydrolases; Clostridioides difficile; Kinetics; Organelles; Protons; 14-3-3 Proteins; Neurons; Synapses; Cytoskeleton; Cathelicidins; Mutation; Neurodegenerative Diseases; Protein Processing, Post-Translational; Computational Biology; Feedback; Lipid Droplets; Immunity, Innate; Computer Simulation; Amino Acid Sequence; Models, Neurological; Antimicrobial Peptides; HeLa Cells; 1-Alkyl-2-acetylglycerophosphocholine Esterase; Drosophila; Chromosome Structures; Chromosomes, Bacterial; Staphylococcus aureus; Histones; Polymyxin B; Models, Molecular; Mammals; Adenosine Diphosphate; Microtubules; Molecular Dynamics Simulation; Tubulin; Biomechanical Phenomena; Glycogen Synthase Kinase 3 beta; Cytoplasmic Dyneins; Fatty Acids; Chlorocebus aethiops; Metronidazole; Dyneins; Pyramidal Cells; Interneurons; Host-Pathogen Interactions; Protein Binding; Anti-Bacterial Agents; Lysosomes; Brain; Muscular Atrophy, Spinal; Sequence Analysis, RNA; Clostridioides; Diffusion; Cyclin-Dependent Kinase 5; Microbiota; Motor Neuron Disease; Dynactin Complex; Lipopolysaccharides; Cell Communication; Escherichia coli; Viscosity; Mitochondria; Drosophila Proteins; Protein Conformation; Antimicrobial Cationic Peptides; COS Cells; Adjuvants, Immunologic; Drug Synergism; RNA, Small Interfering; Sensation; Preliminary Data; Imaging, Three-Dimensional; Biophysical Phenomena; Parkinson Disease; HEK293 Cells; Motion; Bacteria</t>
+          <t>Motor Neuron Disease; Dynactin Complex; Lipid Droplets; Mammals; Cytoskeleton; Tubulin; Parkinson Disease; Preliminary Data; Microbiota; Anti-Infective Agents; Microtubules; Mutation; Protein Processing, Post-Translational; Muscular Atrophy, Spinal; Antimicrobial Peptides; Biophysics; Molecular Motor Proteins; Kinesins; Optical Tweezers; Neurodegenerative Diseases; Brain; Histones; Saccharomyces cerevisiae; Neurons</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Guzowski, John</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>In Situ Hybridization; Microglia; Action Potentials; Electrodes, Implanted; Neurons; Mitochondria; Antioxidants; Allergy and Immunology; Health; Antineoplastic Agents; Cognitive Dysfunction; Immunohistochemistry; Rats, Long-Evans; Resilience, Psychological; Cognition; Stress, Psychological; Oxidative Stress; Transcriptome; Neoplasms; Cisplatin; Space Perception; Apoptosis; Neuroimmunomodulation; Neuronal Plasticity; In Situ Hybridization, Fluorescence; Cytokines; Mental Health; Memory; Hippocampus; Genes, Immediate-Early; Behavior</t>
-        </is>
-      </c>
+          <t>Guzowski, JF</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -969,7 +949,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Uracil; Cell Proliferation; Mevalonic Acid; Macrophages; CRISPR-Cas Systems; Tumor Microenvironment; Fibrosis; Oxidoreductases; Amiloride; Flow Cytometry; Autophagy; Research Design; Energy Metabolism; geranylgeranyl pyrophosphate; Pyrimidines; Arginine; Standard of Care; Cell Line, Tumor; Adenocarcinoma; Sodium-Hydrogen Exchangers; Anti-Inflammatory Agents; Metabolomics; CD8-Positive T-Lymphocytes; Asparagine; Pancreatitis, Chronic; Arginase; Organoids; Clone Cells; Goals; Epithelial Cells; Pancreatic Diseases; Oxidation-Reduction; Chromatography, Liquid; RNA; Myeloid Cells; Staining and Labeling; Epigenesis, Genetic; Carcinogenesis; Metabolic Networks and Pathways; Cell Transformation, Neoplastic; Gene Expression Profiling; Histones; Pinocytosis; Hepatocyte Growth Factor; Hospitalization; Gemcitabine; Stromal Cells; Acute Disease; Signal Transduction; Tandem Mass Spectrometry; Critical Pathways; Allografts; Granulocyte-Macrophage Colony-Stimulating Factor; Pancreatic Hormones; Pain Management; Pancreatic Neoplasms; Communication; 3-hydroxy-3-methylglutaryl-coenzyme A; Sequence Analysis, RNA; Symbiosis; Cancer-Associated Fibroblasts; Deoxycytidine; Prognosis; Proteomics; Regeneration; Fibroblasts; Catalytic Domain; Indicators and Reagents; Methylation; Glutathione; Drug Resistance, Neoplasm; Liver Neoplasms; Early Diagnosis; Metabolic Reprogramming; Immunotherapy; Tumor-Associated Macrophages; Transcriptome; Survival Rate; Neoplasms; Preliminary Data; Cytotoxins; Cell Lineage; Transcription Factors; Pancreatitis; Cues; Pancreas; Carcinoma, Pancreatic Ductal</t>
+          <t>Metabolic Networks and Pathways; Flow Cytometry; Staining and Labeling; Signal Transduction; Cell Transformation, Neoplastic; Preliminary Data; Uracil; Pancreatic Hormones; Pancreatic Diseases; Survival Rate; Immunotherapy; Hepatocyte Growth Factor; RNA; Glutathione; Asparagine; Cancer-Associated Fibroblasts; Drug Resistance, Neoplasm; Pancreatitis, Chronic; Fibroblasts; Fibrosis; Catalytic Domain; Cues; Clone Cells; Myeloid Cells; 3-hydroxy-3-methylglutaryl-coenzyme A; Indicators and Reagents; Acute Disease; Cell Lineage; Tumor-Associated Macrophages; Pyrimidines; Autophagy; Methylation; Metabolic Reprogramming; Carcinoma, Pancreatic Ductal; Prognosis; Energy Metabolism; Neoplasms; Macrophages; Standard of Care; Pain Management; Tumor Microenvironment; Liver Neoplasms; Epigenesis, Genetic; Gemcitabine; Communication; Goals; Hospitalization; Research Design; Anti-Inflammatory Agents; Oxidation-Reduction; Cytotoxins; Allografts; Stromal Cells; Critical Pathways; Pancreas; Gene Expression Profiling; Oxidoreductases; Transcriptome; Carcinogenesis; Cell Proliferation; Histones; geranylgeranyl pyrophosphate; Mevalonic Acid; Epithelial Cells; Pancreatitis; Regeneration; Adenocarcinoma; Sequence Analysis, RNA; Organoids; Pancreatic Neoplasms</t>
         </is>
       </c>
     </row>
@@ -981,7 +961,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Biodiversity; Students; Anthropogenic Effects; Ecosystem; Social Behavior; Biological Evolution; Metagenomics; Dysbiosis; Agriculture; Feedback; Crops, Agricultural; Parasites; Magnolia; Coral Bleaching; Health; Bees; Goals; Motivation; Crithidia; Genetics; Gastrointestinal Microbiome; Preliminary Data; Mentors; Seasons; Insecta; Ecological and Environmental Phenomena; Ecology; Quality Indicators, Health Care; Disease Resistance; Symbiosis; Microbiota; RNA, Ribosomal, 16S; Host Microbial Interactions; Longevity; Pollination; Data Analysis; Human Activities; Reproduction; Schools; Bacteria; Social Interaction</t>
+          <t>Anthropogenic Effects; Host Microbial Interactions; Schools; Microbiota; Preliminary Data; Crops, Agricultural; Metagenomics; Magnolia; Parasites; Social Interaction; Dysbiosis; Students; Coral Bleaching; Ecological and Environmental Phenomena; Reproduction; Bees; Seasons; Feedback; Bacteria; Social Behavior; Disease Resistance; Health; Quality Indicators, Health Care; Ecosystem; Motivation; Gastrointestinal Microbiome; Goals; Pollination; Data Analysis; Agriculture; Symbiosis; Longevity; Mentors; Insecta; Human Activities; Genetics; Crithidia</t>
         </is>
       </c>
     </row>
@@ -993,7 +973,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Density Functional Theory; Escherichia coli; Anaerobiosis; Molybdenum; Ecosystem; Technology; Phylogeny; Electrons; Tellurium; X-Ray Absorption Spectroscopy; Protein Conformation; Formate Dehydrogenases; Hydrogenase; Recombinant Proteins; Carbon Dioxide; Biosynthetic Pathways; Circular Dichroism; Oxidoreductases; Bioreactors; Models, Chemical; Oxidation-Reduction; Coenzymes; Nitrogen; Ammonia; Nitrogen Cycle; Molybdoferredoxin; Carbon Monoxide; S-Adenosylmethionine; Crystallography, X-Ray; Oxygen; Aldehyde Oxidoreductases; Hydrocarbons; Methanosarcina; Protein Binding; Selenious Acid; Rotation; Azotobacter vinelandii; Nitrogen Fixation; Enzymes; Gene Expression; Methyltransferases; Chemistry, Bioinorganic; Adenosine Triphosphate; Archaeal Proteins; Bacterial Proteins; Hydrogen; Metalloproteins; Nitrogenase; Catalysis; Models, Molecular; Electron Spin Resonance Spectroscopy; Molecular Structure; Iron-Sulfur Proteins; Sulfur; Biotechnology; Multienzyme Complexes</t>
+          <t>Iron-Sulfur Proteins; Biosynthetic Pathways; Nitrogen; Hydrogen; Escherichia coli; Catalysis; Electrons; Ammonia; Carbon Monoxide; Enzymes; Hydrocarbons; Nitrogen Cycle; Anaerobiosis; Carbon Dioxide; Molybdenum; Ecosystem; Chemistry, Bioinorganic; Sulfur; Metalloproteins; Nitrogenase; Oxygen; Bioreactors; Nitrogen Fixation; Technology; Rotation</t>
         </is>
       </c>
     </row>
@@ -1005,7 +985,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>cdc42 GTP-Binding Protein; Stroke; Capillaries; Apolipoprotein E2; Paclitaxel; Tumor Microenvironment; Coculture Techniques; Liver; Microphysiological Systems; Rare Diseases; Basement Membrane; Telangiectasia, Hereditary Hemorrhagic; Single-Cell Gene Expression Analysis; rho GTP-Binding Proteins; Cytoreduction Surgical Procedures; Drug Interactions; Tissue Engineering; Insulin; Neoplastic Processes; Thrombosis; Snail Family Transcription Factors; Gene Expression; Colonic Neoplasms; Colorectal Neoplasms; Cell Line, Tumor; Bayes Theorem; Fluorouracil; Arteries; Microglia; Diabetes Mellitus; Neurons; Glucose; Prospective Studies; Mutation; Induced Pluripotent Stem Cells; Clustered Regularly Interspaced Short Palindromic Repeats; Endoglin; Blood Vessels; Breast; Drug Evaluation; Arteriovenous Malformations; Islets of Langerhans; Hyperthermia, Induced; Triple Negative Breast Neoplasms; Biomimetics; Goals; Drug Development; Peritoneal Cavity; Leucovorin; Peptides; Peritoneal Neoplasms; RNA; Microvessels; Lung; Anemia; Neoadjuvant Therapy; Stomach Neoplasms; Patient Advocacy; Neovascularization, Pathologic; Obesity; Biomarkers, Tumor; Stromal Cells; Signal Transduction; Exosomes; Alzheimer Disease; Islets of Langerhans Transplantation; Extracellular Matrix; Huntington Disease; Allografts; Epistaxis; Astrocytes; Pancreatic Neoplasms; Drug Repositioning; Anxiety; Adipose Tissue; Oxaliplatin; Brain; Endothelial Cells; Pazopanib; Hyperthermic Intraperitoneal Chemotherapy; Vascular Malformations; Transcytosis; Adipogenesis; Follow-Up Studies; Myocytes, Smooth Muscle; Incidence; Infant; Heart Failure; Fibroblasts; Sturge-Weber Syndrome; Rodentia; Splenic Neoplasms; Pericytes; peptide I; Port-Wine Stain; Immunotherapy; Blood-Brain Barrier; Angiogenesis; Fascia; Transcriptome; Neoplasms; Immunotherapy, Adoptive; Lab-On-A-Chip Devices; Survival Rate; Endothelium, Vascular; Transcription Factors; Cell- and Tissue-Based Therapy; Tight Junctions; Microfluidics; Apolipoprotein E4; Pancreas; Phenotype; Peritoneum</t>
+          <t>Endoglin; Apolipoprotein E2; Cell Line, Tumor; Prospective Studies; peptide I; Patient Advocacy; Extracellular Matrix; Biomimetics; Epistaxis; Snail Family Transcription Factors; Fibroblasts; Astrocytes; Basement Membrane; Blood Vessels; Pazopanib; Neoplasms; Incidence; Gene Expression; Tissue Engineering; Heart Failure; Transcytosis; Hyperthermia, Induced; Telangiectasia, Hereditary Hemorrhagic; Arteriovenous Malformations; Microphysiological Systems; Neoadjuvant Therapy; Pericytes; Follow-Up Studies; Induced Pluripotent Stem Cells; Microglia; Lab-On-A-Chip Devices; Anemia; Single-Cell Gene Expression Analysis; Drug Development; Clustered Regularly Interspaced Short Palindromic Repeats; Peritoneal Cavity; Blood-Brain Barrier; Myocytes, Smooth Muscle; Liver; Fluorouracil; Alzheimer Disease; Pancreas; Neoplastic Processes; Rare Diseases; Endothelial Cells; Peritoneal Neoplasms; Neurons; Lung; Signal Transduction; Stroke; Phenotype; Drug Repositioning; Neovascularization, Pathologic; Transcription Factors; Drug Evaluation; Microfluidics; Arteries; Oxaliplatin; Capillaries; Stomach Neoplasms; Infant; Vascular Malformations; Peritoneum; Leucovorin; Colorectal Neoplasms; Splenic Neoplasms; Angiogenesis; Peptides; Hyperthermic Intraperitoneal Chemotherapy; Anxiety; Survival Rate; Mutation; Tight Junctions; Cytoreduction Surgical Procedures; Goals; Drug Interactions; Huntington Disease; Stromal Cells; Colonic Neoplasms; Brain; Apolipoprotein E4; Sturge-Weber Syndrome</t>
         </is>
       </c>
     </row>
@@ -1017,7 +997,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Water Cycle; Carbon; Population Dynamics; Population Density; Physiology, Comparative; Climate; Climate Change; Seeds; Hot Temperature; Ecosystem; Trees; Brazil; Phylogeny; Chlorophyll; Agriculture; Soil; Water Supply; Remote Sensing Technology; Humidity; Groundwater; Temperature; Human Activities; Carbon Dioxide; Stress, Physiological; California; Wind; Biomass; Poaceae; Gases; Xylem; Plant Transpiration; Germination; Forests; Introduced Species; Urbanization; Magnoliopsida; Cycadopsida; Atmospheric Pressure; Volunteers; Health Surveys; Photosynthesis; Metals, Rare Earth; Museums; Climate Models; Plants; Metabolism; Seasons; Droughts; Desert Climate; Eucalyptus; Water; Water Resources; Ecology; Ecological and Environmental Phenomena; Hydrology; Time Factors; Mustard Plant; Light; Plant Stomata; Environmental Policy; Plant Leaves; El Nino-Southern Oscillation; Southwestern United States; Longevity; Cactaceae; Tropical Climate; Rainforest; Reproduction; Phenotype; Arizona; Demography</t>
+          <t>Hydrology; Remote Sensing Technology; Volunteers; Humidity; Desert Climate; Water; Ecological and Environmental Phenomena; Carbon; Ecosystem; Temperature; Water Supply; Museums; Physiology, Comparative; Plants; Wind; Groundwater; Water Resources; Ecology; Health Surveys; Climate Change</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1009,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Saliva; Graft vs Host Disease; Yolk Sac; Macrophages; Membrane Proteins; Toxoplasmosis; CRISPR-Cas Systems; Liver; Oxidoreductases; Amyloid beta-Peptides; Endothelial Protein C Receptor; Bone Marrow; Leptospiraceae; Aging; Flow Cytometry; Antigens, CD34; X-Linked Combined Immunodeficiency Diseases; Parvovirinae; SARS-CoV-2; Gene Expression; Algorithms; DNA, Complementary; Neural Crest; Microglia; Mutation; Induced Pluripotent Stem Cells; Autoimmunity; Fluticasone; Healthy Volunteers; Real-Time Polymerase Chain Reaction; Hematopoietic Stem Cells; Hemangioblasts; T-Lymphocytes; Myeloid Cells; Proto-Oncogene Proteins c-kit; Erythroid Cells; Blood Cells; Lateral Ventricles; Interleukin Receptor Common gamma Subunit; Erythropoiesis; Cell Line; Mice, Inbred NOD; Pregnancy; Codon, Initiator; White Matter; Cells, Cultured; Vesicular Transport Proteins; Gene Deletion; Receptors, Cell Surface; Coronavirus Infections; Homeostasis; Genetic Vectors; Hematopoietic Stem Cell Transplantation; Transplantation Chimera; Transplantation, Homologous; Immunosuppressive Agents; Alzheimer Disease; Dependovirus; Receptors, Granulocyte-Macrophage Colony-Stimulating Factor; Fetus; Bone Marrow Cells; Primary Cell Culture; Receptors, CCR2; Diabetes Mellitus, Type 1; Bone Marrow Transplantation; Exons; Brain; Transduction, Genetic; Specimen Handling; Transplantation, Heterologous; Cell Separation; Radiation Chimera; Stem Cells; Lipopolysaccharides; Molecular Diagnostic Techniques; Biomarkers; Gene Editing; Radiation Injuries, Experimental; Pluripotent Stem Cells; Phagocytosis; Nucleic Acid Amplification Techniques; Pericytes; Integrases; Antigens, Ly; CX3C Chemokine Receptor 1; Poly I-C; COVID-19 Nucleic Acid Testing; Blood-Brain Barrier; Tumor Necrosis Factor Receptor Superfamily, Member 7; Mice, Inbred Strains; CD11a Antigen; Gene Expression Regulation, Developmental; Cell Lineage; Adaptation, Physiological; Immunoglobulin G; Tight Junctions; Time Factors; Fetal Blood; Mesoderm; Animals, Newborn; Inflammation</t>
+          <t>Hematopoietic Stem Cell Transplantation; Leptospiraceae; Graft vs Host Disease; T-Lymphocytes; Stem Cells</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1021,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Transcriptional Activation; Mosquito Vectors; Gene Expression Regulation, Enzymologic; Tubulin; Magnetic Resonance Imaging; Hedgehog Proteins; Vision, Ocular; Malaria; Mutagenesis, Insertional; Cell Death; Family; Dengue; Functional Laterality; Blood Vessels; Aedes; Peptide Hydrolases; Insecticides; Zika Virus; Case-Control Studies; CRISPR-Cas Systems; Genetic Engineering; Disease Vectors; Sporozoites; Gene Drive Technology; Culicidae; DNA Transposable Elements; Betalains; Sex Differentiation; Vector Borne Diseases; Genetics; Plasmodium falciparum; RNA; Animals, Genetically Modified; Culex; Oviposition; Pigments, Biological; Cerebral Cortex; Promoter Regions, Genetic; Drosophila; Brain; Zika Virus Infection; Mosquito Control; Gene Expression; Gene Transfer Techniques; Color; Malaria, Falciparum; Transgenes; Dengue Virus; Bombyx; Anopheles; Genetic Introgression; Rabbits; Plasmodium; Global Health; Schizophrenia; Reproduction; RNA, Guide, CRISPR-Cas Systems; Filariasis</t>
+          <t>Dengue; Gene Transfer Techniques; Genetics; Gene Drive Technology; Blood Vessels; Malaria; Global Health; Genetic Engineering</t>
         </is>
       </c>
     </row>
@@ -1053,7 +1033,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>White Matter; Magnetic Resonance Imaging; Physical Functional Performance; Neurons; Disease Progression; Racial Groups; Dementia, Vascular; Extracellular Vesicles; Retrospective Studies; Amyotrophic Lateral Sclerosis; Medical History Taking; Frontotemporal Lobar Degeneration; Databases, Factual; Aged, 80 and over; Angiotensin-Converting Enzyme Inhibitors; Geriatric Assessment; Hand Strength; Amyloid; Hippocampal Sclerosis; Case-Control Studies; Cognitive Dysfunction; Alzheimer Disease; Amyloid beta-Peptides; Risk Factors; Reference Values; Limbic System; Epidemiology; Neuropsychological Tests; Plaque, Amyloid; TDP-43 Proteinopathies; Lewy Bodies; Cryopreservation; Cognition; Adrenergic beta-Antagonists; Neuroglia; Aging; Positron-Emission Tomography; Clinical Trials as Topic; Ethylene Glycols; Aged; Amyloidosis; Aniline Compounds; Logistic Models; Dementia; Cerebrovascular Circulation; DNA-Binding Proteins; RNA-Seq; Cerebral Cortex; Self-Help Devices; Cataract; Sleep Duration; Sleep; Ethnicity; Brain; Autopsy; Tauopathies; Neuropathology; Cohort Studies; Nervous System Diseases; Self Report; Syncope; Apolipoproteins E; Atrophy; Longitudinal Studies; Sex Factors; Centenarians; Walking Speed; Cell Separation; Lewy Body Disease; Nonagenarians; Organ Size; Executive Function; Hippocampus; Educational Status; Neurofibrillary Tangles</t>
+          <t>Alzheimer Disease; Aging; Aged, 80 and over; Dementia, Vascular; Epidemiology; Clinical Trials as Topic; Cognitive Dysfunction; Dementia</t>
         </is>
       </c>
     </row>
@@ -1065,7 +1045,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Ascitic Fluid; Diabetes Mellitus, Type 2; Ovarian Neoplasms; DNA; Protein Serine-Threonine Kinases; Chromatin; Carrier Proteins; Wnt Signaling Pathway; Membrane Proteins; National Center for Advancing Translational Sciences (U.S.); Nutrients; Early Detection of Cancer; Single-Cell Analysis; Quality of Life; Tumor Microenvironment; Lipid Metabolism; Morbidity; Diet, Ketogenic; Risk Factors; Phosphoric Monoester Hydrolases; Carcinoma; Mammary Neoplasms, Experimental; Appendiceal Neoplasms; Gene Expression Regulation, Neoplastic; Glycolysis; Lipids; Cytoreduction Surgical Procedures; Vitamins; Thyroid Hormone-Binding Proteins; Xenograft Model Antitumor Assays; Lubricants; Neoplastic Processes; Lysine; Energy Metabolism; Arginine; Gene Expression; Colonic Neoplasms; Colorectal Neoplasms; Standard of Care; Cell Line, Tumor; United States; Vitamin B 6; Adenocarcinoma; Mice, Nude; Thiazolidinediones; Epigenomics; Diabetes Mellitus; Glucose; Weight Loss; Mutation; Cell Plasticity; Micronutrients; Peptide Hydrolases; Protein Phosphatase 2; Histone Methyltransferases; Antineoplastic Agents; Lactic Acid; Organoids; Dioxygenases; PPAR gamma; Goals; Cell Survival; Sex Chromosomes; Peritoneal Cavity; Ketones; Substrate Specificity; Pilot Projects; Chromatography, Liquid; Peritoneal Neoplasms; Genes, Tumor Suppressor; Genetics; Proteolysis; Crystallography, X-Ray; Pyruvate Kinase; T-Lymphocytes; RNA; Intestinal Mucosa; Phosphofructokinase-1, Type C; Epigenesis, Genetic; Prevalence; Breast Neoplasms; MicroRNAs; Diet, High-Fat; Carcinogenesis; Metabolic Networks and Pathways; AMP-Activated Protein Kinases; Adipocytes; Adenomatous Polyposis Coli; Neoplastic Stem Cells; Mice, Inbred NOD; Cell Line; Histones; High-Throughput Screening Assays; Glutamine; Liquid Chromatography-Mass Spectrometry; Cost of Illness; Vitamin A; Neoplasms, Second Primary; Serine; Muscles; Adolescent; Mesenchymal Stem Cells; Obesity; Hospitalization; Protein-Arginine N-Methyltransferases; Gastrointestinal Neoplasms; Homeostasis; Signal Transduction; Heterografts; Chemistry, Pharmaceutical; Stress, Physiological; Cell Differentiation; Tandem Mass Spectrometry; Metabolic Diseases; Phosphorylation; Allografts; Sex Characteristics; Pyruvic Acid; Pancreatic Neoplasms; Oxidative Phosphorylation; Tumor Suppressor Protein p53; Genes, p16; Cell Cycle; Histone Demethylases; Clinical Relevance; Metabolism; Peroxisome Proliferator-Activated Receptors; Protein Isoforms; Hyperthermic Intraperitoneal Chemotherapy; Sequence Analysis, RNA; Transcription, Genetic; Adipogenesis; Histone Code; Immunity; Appendectomy; Incidence; Stem Cells; Ficus; Neoplasm Metastasis; RNA, Long Noncoding; Fibroblasts; Mitochondria; Melanoma; Pioglitazone; Catalytic Domain; Metformin; Methylation; Military Personnel; Pseudomyxoma Peritonei; Drug Resistance, Neoplasm; Dietary Supplements; Mice, SCID; Cachexia; Liver Neoplasms; Monocarboxylic Acid Transporters; Lipogenesis; Thyroid Hormones; Rectal Neoplasms; Immunotherapy; Up-Regulation; Ketoglutaric Acids; Microscopy; Transcriptome; Neoplasms; Adaptation, Physiological; Transcription Factors; Biological Products; Adenocarcinoma, Mucinous; Isotopes; Prostatic Neoplasms; HEK293 Cells; TWEAK Receptor; Abdominal Cavity; Cytokines; Ketone Bodies; Phosphoprotein Phosphatases; Amino Acid Transport Systems, Basic; Phenotype; Carcinoma, Pancreatic Ductal; Peritoneum</t>
+          <t>Ficus; Cell Line, Tumor; Isotopes; Chemistry, Pharmaceutical; Cytokines; Immunotherapy; Metabolic Diseases; Melanoma; Pyruvic Acid; Cost of Illness; Incidence; Neoplasms; Metabolism; Protein Serine-Threonine Kinases; Appendiceal Neoplasms; Gene Expression; Oxidative Phosphorylation; Lipid Metabolism; Chromatography, Liquid; Lactic Acid; Allografts; Cell Cycle; National Center for Advancing Translational Sciences (U.S.); Tandem Mass Spectrometry; Appendectomy; Organoids; Cell Line; Peroxisome Proliferator-Activated Receptors; Adenomatous Polyposis Coli; Wnt Signaling Pathway; Monocarboxylic Acid Transporters; Vitamin A; DNA; Gastrointestinal Neoplasms; Lubricants; High-Throughput Screening Assays; RNA; Diabetes Mellitus; Drug Resistance, Neoplasm; Catalytic Domain; Pseudomyxoma Peritonei; Lipids; Peritoneal Cavity; Cachexia; Glutamine; Biological Products; Antineoplastic Agents; Standard of Care; Pilot Projects; Chromatin; Tumor Microenvironment; Liver Neoplasms; Diet, Ketogenic; Hospitalization; Liquid Chromatography-Mass Spectrometry; Pioglitazone; Neoplastic Processes; Peritoneal Neoplasms; Cell Proliferation; Thiazolidinediones; Immunity; Prevalence; PPAR gamma; Intestinal Mucosa; Stem Cells; Prostatic Neoplasms; Muscles; Neoplasms, Second Primary; Ovarian Neoplasms; Weight Loss; Signal Transduction; Phosphoric Monoester Hydrolases; Heterografts; Glucose; Phenotype; Phosphoprotein Phosphatases; Diabetes Mellitus, Type 2; Obesity; Transcription Factors; Substrate Specificity; Epigenomics; Abdominal Cavity; Neoplastic Stem Cells; Carcinoma; Epigenesis, Genetic; Risk Factors; Peritoneum; Carcinogenesis; Metformin; Colorectal Neoplasms; Genes, Tumor Suppressor; Genetics; Sequence Analysis, RNA; Dietary Supplements; T-Lymphocytes; Metabolic Networks and Pathways; Adolescent; Microscopy; Hyperthermic Intraperitoneal Chemotherapy; Diet, High-Fat; Genes, p16; AMP-Activated Protein Kinases; Early Detection of Cancer; United States; Quality of Life; Dioxygenases; Nutrients; Military Personnel; Mutation; Ketoglutaric Acids; Ascitic Fluid; Cytoreduction Surgical Procedures; Histone Demethylases; Ketone Bodies; Lipogenesis; Protein Phosphatase 2; Phosphorylation; Homeostasis; Ketones; Goals; Cell Differentiation; Colonic Neoplasms; Clinical Relevance; Rectal Neoplasms; Morbidity</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1057,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Africa; Isocitrate Dehydrogenase; Karyotype; Animal Fins; Chromatin; Chromosomes, Human, Pair 8; Chromosomal Proteins, Non-Histone; Virulence; Gene Regulatory Networks; Single-Cell Analysis; CRISPR-Cas Systems; Autism Spectrum Disorder; Polydactyly; DNA Transposable Elements; Marsupialia; Otx Transcription Factors; Extinction, Biological; CCCTC-Binding Factor; Gene Rearrangement; Gene Expression; Enhancer Elements, Genetic; Evolution, Molecular; Polymorphism, Single Nucleotide; Intellectual Disability; Piwi-Interacting RNA; Epigenomics; Genetic Variation; Mutation; Clustered Regularly Interspaced Short Palindromic Repeats; Locomotion; Craniofacial Abnormalities; Organoids; Autistic Disorder; Fetal Heart; Congenital Abnormalities; Epigenome; Mutagenesis, Site-Directed; Ectopic Gene Expression; Homeodomain Proteins; MicroRNAs; Cohesins; South America; Australia; Gene Expression Profiling; Extremities; Mammals; Cell Cycle Proteins; Limb Buds; Phylogeny; Base Sequence; Genome Size; Brain Neoplasms; DNA, Intergenic; Genome; Embryo, Mammalian; Promoter Regions, Genetic; Clinical Relevance; Brain; Genomics; Introns; Drosophila melanogaster; Transcriptional Activation; RNA, Long Noncoding; Hedgehog Proteins; Conserved Sequence; Cell Culture Techniques; Gene Editing; Fishes; Gene Expression Regulation; Genes, Reporter; Regulatory Sequences, Nucleic Acid; Heart Diseases; Zinc Fingers; Gene Expression Regulation, Developmental; Gain of Function Mutation; Glioma; Transcription Factors; Gene Transfer Techniques; Time Factors; Alleles; Chromosomes; Phenotype</t>
+          <t>Fetal Heart; Alleles; Regulatory Sequences, Nucleic Acid; Phenotype; Virulence; Base Sequence; Hedgehog Proteins; Limb Buds; Transcription Factors; Cell Culture Techniques; Gene Expression Regulation; Ectopic Gene Expression; Autistic Disorder; Gene Expression; Chromatin; Enhancer Elements, Genetic; RNA, Long Noncoding; Epigenome; Intellectual Disability; Chromosomes; Heart Diseases; Extremities; Congenital Abnormalities; Transcriptional Activation; Clinical Relevance; Gain of Function Mutation; Polydactyly; Organoids</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1069,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Down-Regulation; Microglia; NF-kappa B; Fibroblasts; RNA Splicing; Receptors, Immunologic; Neurons; Response Elements; Metabolomics; Synapses; ATP-Binding Cassette Transporters; Genetic Variation; Mutation; Synaptic Transmission; Phagocytosis; Neurodegenerative Diseases; Gene Regulatory Networks; Signal Transduction; Calcium; Amyloid beta-Protein Precursor; Cognitive Dysfunction; Genotype; Alzheimer Disease; Amyloid beta-Peptides; Glial Fibrillary Acidic Protein; Cuprizone; Neuroglia; Plaque, Amyloid; Resilience, Psychological; Gene Ontology; Cognition; Gene Knock-In Techniques; Sex Characteristics; Gastrointestinal Microbiome; Astrocytes; Aged; Tetracycline; RNA-Seq; Demyelinating Diseases; Membrane Glycoproteins; Cognition Disorders; Brain; tau Proteins; Tauopathies; Doxycycline; Cathepsin D; Behavior, Animal; Long-Term Potentiation; Myeloid Differentiation Factor 88; Apolipoproteins E; Gene Expression Profiling; Neuronal Plasticity; Microbiota; Translational Research, Biomedical; Proteomics; Hippocampus; Phenotype</t>
+          <t>Alzheimer Disease; Neurodegenerative Diseases; Translational Research, Biomedical</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1081,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Biodiversity; Students; Climate; Food Contamination; Climate Change; Hot Temperature; Ecosystem; Kelp; Mutation; Macrocystis; Housing; Faculty; Environmental Monitoring; Remote Sensing Technology; Temperature; Environmental Science; Behavioral Sciences; Environmental Microbiology; Goals; Motivation; Urbanization; One Health; Disease Outbreaks; Acclimatization; Seaweed; Indonesia; Conservation of Natural Resources; Seawater; Policy; Oceans and Seas; Anthozoa; Water; Ecological and Environmental Phenomena; Coral Reefs; Seafood; Refugees; Germ Cells, Plant; Microbiota; Cities; Reproduction; Myanmar; Aquaculture; Marine Biology</t>
+          <t>Remote Sensing Technology; Hot Temperature; Microbiota; Behavioral Sciences; Housing; Policy; Students; Water; Mutation; Ecological and Environmental Phenomena; Cities; Reproduction; Conservation of Natural Resources; Kelp; Marine Biology; Ecosystem; Temperature; Germ Cells, Plant; Environmental Science; Motivation; Goals; Disease Outbreaks; One Health; Faculty; Oceans and Seas; Environmental Microbiology; Macrocystis; Acclimatization</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1093,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Proteins; Vibrio; Feedback, Physiological; Chromatin; Chromosomal Proteins, Non-Histone; Proto-Oncogene Proteins B-raf; Nevus, Pigmented; Gene Regulatory Networks; Nevus; Single-Cell Analysis; Prodrugs; Saccharomyces cerevisiae; Aging; Melanocytes; Morphogenesis; Protein Kinase Inhibitors; Research Design; Gene Expression; Algorithms; De Lange Syndrome; Heterozygote; Retina; Bayes Theorem; Down-Regulation; Zebrafish; Mutation; Databases, Factual; Feedback; Computational Biology; Wings, Animal; Gastrulation; Organoids; Congenital Abnormalities; CHO Cells; Imaginal Discs; Oncogenes; Drosophila; Leukemia, Myelogenous, Chronic, BCR-ABL Positive; Cohesins; Gene Expression Profiling; Pregnancy; Tyrosine Kinase Inhibitors; Mammals; Cell Cycle Proteins; Homeostasis; Signal Transduction; Hematopoiesis; Recombinant Proteins; Metronidazole; Myelopoiesis; Mass Behavior; Animals, Genetically Modified; Promoter Regions, Genetic; Communication; Brain; Sequence Analysis, RNA; Drosophila melanogaster; Stem Cells; Systems Biology; Body Patterning; Cell Communication; X-Ray Microtomography; Hedgehog Proteins; Melanoma; Drosophila Proteins; Cell Division; Gene Expression Regulation; Growth and Development; Drug Resistance, Neoplasm; Cricetulus; Fusion Proteins, bcr-abl; Nitroreductases; Green Fluorescent Proteins; Gene Expression Regulation, Developmental; Protein Engineering; Transcriptome; Neoplasms; Cell Lineage; Embryonic Development; Extracellular Matrix Proteins; HEK293 Cells; Proto-Oncogene Mas; Phenotype</t>
+          <t>Growth and Development; Congenital Abnormalities; Systems Biology; Computational Biology; Stem Cells; Neoplasms</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1105,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Bacterial Infections; Stroke; Neural Stem Cells; Macrophages; Angiotensin-Converting Enzyme 2; Activin Receptors; Protease Inhibitors; Pandemics; Cognitive Dysfunction; Chemotactic Factors; Amyloid beta-Peptides; Risk Factors; Cysteine; Immune System; Receptors, Chemokine; RNA, Viral; Memory Consolidation; Cystatins; Aging; Monocytes; Cognition; Organic Chemicals; Protein Multimerization; Myelin Sheath; Demyelinating Diseases; Research Design; Secretome; SARS-CoV-2; Gene Expression; Muscle, Skeletal; Chemokines; Encephalomyelitis, Autoimmune, Experimental; Drug Evaluation, Preclinical; Microglia; Stem Cell Transplantation; Neurons; Chemokine CXCL10; Disease Progression; Ischemia; Mutation; Induced Pluripotent Stem Cells; Synaptic Transmission; Dysgeusia; Receptors, CXCR3; Central Nervous System Viral Diseases; Neurodegenerative Diseases; Allergy and Immunology; Virus Replication; Goals; Drug Development; Immunity, Innate; Oxidation-Reduction; Vero Cells; Adiposity; Amino Acid Sequence; Axons; COVID-19; B-Lymphocytes; Crystallography, X-Ray; T-Lymphocytes; Aged; Lung; Autoimmune Diseases of the Nervous System; Antiviral Agents; Neuroinflammatory Diseases; Congresses as Topic; Neutrophils; Gene Expression Profiling; Cell Line; Models, Molecular; CD4-Positive T-Lymphocytes; Translational Research, Biomedical; White Matter; Murine hepatitis virus; Coronavirus 3C Proteases; Virus Diseases; Chemokine CXCL1; Forkhead Transcription Factors; Coronavirus Infections; Signal Transduction; Chlorocebus aethiops; Cell Differentiation; Monomeric GTP-Binding Proteins; Encephalitis, Viral; Oligodendroglia; Alzheimer Disease; T-Lymphocytes, Regulatory; Allosteric Site; Coronavirus; Tetracyclines; Mental Fatigue; Spinal Cord; Host-Pathogen Interactions; Astrocytes; Animals, Genetically Modified; Dementia; Bone Marrow Transplantation; Lysosomal Membrane Proteins; Brain; CD4 Antigens; Muscular Atrophy; Sequence Analysis, RNA; Sweden; Immunity; Inflammation Mediators; Multiple Sclerosis; Headache; Stem Cells; Hashimoto's encephalitis; Infant; RNA, Messenger; Rodentia; Catalytic Domain; Pluripotent Stem Cells; Amino Acids; Receptors, Interleukin-8B; Tamoxifen; Societies, Medical; Neuroglia; Meningitis; Mitochondrial Diseases; Matrix Metalloproteinase 9; Receptor Protein-Tyrosine Kinases; Disulfides; Remyelination; Central Nervous System; Preliminary Data; Single Molecule Imaging; Anosmia; Lymphocyte Activation; Neuroimmunomodulation; Immunity, Cellular; Cytokine Release Syndrome; Parkinson Disease; Human Embryonic Stem Cells; Apolipoprotein E4; Encephalitis; Inflammation</t>
+          <t>Preliminary Data; Parkinson Disease; B-Lymphocytes; Hashimoto's encephalitis; Astrocytes; Pandemics; Memory Consolidation; Gene Expression; Axons; Mitochondrial Diseases; Amino Acids; Anosmia; Cytokine Release Syndrome; Rodentia; Cognition; Angiotensin-Converting Enzyme 2; Induced Pluripotent Stem Cells; Immune System; Neural Stem Cells; Cognitive Dysfunction; Lysosomal Membrane Proteins; Dysgeusia; Microglia; Coronavirus Infections; Ischemia; Single Molecule Imaging; Neuroinflammatory Diseases; Macrophages; Coronavirus; Inflammation; Disease Progression; Inflammation Mediators; Alzheimer Disease; RNA, Viral; Neurodegenerative Diseases; Synaptic Transmission; Neurons; Dementia; Amyloid beta-Peptides; Immunity; Lung; Myelin Sheath; Aged; Mental Fatigue; COVID-19; Stroke; Sweden; Animals, Genetically Modified; Neuroglia; Meningitis; Amino Acid Sequence; Infant; Risk Factors; Remyelination; Central Nervous System; Encephalitis; Murine hepatitis virus; Immunity, Innate; Virus Replication; Sequence Analysis, RNA; T-Lymphocytes; Virus Diseases; Headache; Mutation; Allergy and Immunology; Human Embryonic Stem Cells; Encephalitis, Viral; Bacterial Infections; Monocytes; Spinal Cord; Multiple Sclerosis; Goals; Research Design; SARS-CoV-2; Brain; Gene Expression Profiling; Apolipoprotein E4</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1117,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Centers for Disease Control and Prevention, U.S.; Neocortex; CDC2 Protein Kinase; Anaphase-Promoting Complex-Cyclosome; Protein Serine-Threonine Kinases; Clustered Regularly Interspaced Short Palindromic Repeats; Embryo, Nonmammalian; Germ Cells; Cell Differentiation; Microtubule-Associated Proteins; Goals; Repressor Proteins; Phosphorylation; Cdc20 Proteins; M Phase Cell Cycle Checkpoints; Aging; Cyclins; Cyclin B1; Cell Cycle Checkpoints; Kinetochores; Microscopy; Cell Cycle; Caenorhabditis elegans Proteins; Neoplasms; Cyclin B; Embryonic Development; Caenorhabditis elegans; Tetratricopeptide Repeat; Spindle Apparatus; Genomics; Mitosis; Cues; Cyclin B2; United States; Cell Cycle Proteins; Ependymoglial Cells</t>
+          <t>Microscopy; Cyclins; Germ Cells; Repressor Proteins; Cues; Clustered Regularly Interspaced Short Palindromic Repeats; Neoplasms; Genomics; Caenorhabditis elegans; Cyclin B; Embryonic Development; Goals; Cell Differentiation; Cell Cycle; Aging; Mitosis; Cell Proliferation; M Phase Cell Cycle Checkpoints; Anaphase-Promoting Complex-Cyclosome</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1129,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Vancomycin; Health Policy; Diet; Area Under Curve; Chromatin; DNA; Nutrients; Early Detection of Cancer; Risk Factors; DNA Transposable Elements; Infection Control; Genome, Human; Stress, Psychological; Keratinocytes; Carrier State; Microbial Sensitivity Tests; Fellowships and Scholarships; Prostatic Hyperplasia; Self Report; Intensive Care Units; Urodela; Evolution, Molecular; Bayes Theorem; United States; Multiomics; Health Status; Serogroup; Epigenomics; Drug-Related Side Effects and Adverse Reactions; Epidermis; Cost-Benefit Analysis; Mutation; Sleep Apnea Syndromes; Tetraodontiformes; Models, Economic; Parasites; Pneumococcal Vaccines; Organoids; Goals; Species Specificity; Epigenome; Genetics; RNA; Cross-Sectional Studies; Fertility; Obesity, Abdominal; Massachusetts; Epigenesis, Genetic; Social Responsibility; Drosophila; Ecological and Environmental Phenomena; Embolization, Therapeutic; Gene Expression Profiling; Multiparametric Magnetic Resonance Imaging; Osteitis Deformans; Mammals; Valosin Containing Protein; Child, Preschool; Markov Chains; Heptavalent Pneumococcal Conjugate Vaccine; Surveys and Questionnaires; Obesity; Sequence Homology; Eating; Biological Evolution; Immunization; Base Sequence; Health; Cell Differentiation; Genomic Instability; Eukaryotic Cells; Frontotemporal Dementia; Genome; Anti-Bacterial Agents; Acute Kidney Injury; Genomics; Population Surveillance; Retroelements; Pneumococcal Infections; Infant; Staphylococcal Infections; Body Mass Index; Magnetic Resonance Imaging; Acculturation; Streptococcus pneumoniae; Amyotrophic Lateral Sclerosis; Waist-Hip Ratio; Chlorhexidine; Genetics, Population; Skin; Emigrants and Immigrants; Asian; Methicillin-Resistant Staphylococcus aureus; Heterochromatin; Transcriptome; Neoplasms; Hospital Costs; Sleep; Sleep Wake Disorders; Child; Prostatic Neoplasms; Time Factors; Anti-Infective Agents, Local; Pharmaceutical Preparations; Chromosomes; East Asian People</t>
+          <t>Diet; Tetraodontiformes; Sequence Homology; Eating; Heterochromatin; Mammals; DNA; Fertility; Genome; Parasites; Base Sequence; RNA; Urodela; Early Detection of Cancer; Ecological and Environmental Phenomena; Nutrients; Epigenomics; DNA Transposable Elements; Genomic Instability; Neoplasms; Evolution, Molecular; Retroelements; Drug-Related Side Effects and Adverse Reactions; Chromatin; Health; Genomics; Biological Evolution; Epigenesis, Genetic; Species Specificity; Epigenome; Goals; Chromosomes; Eukaryotic Cells; Fellowships and Scholarships; Drosophila; Gene Expression Profiling; Social Responsibility; Pharmaceutical Preparations; Genetics; Genome, Human; Genetics, Population; Multiomics</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1141,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Thromboinflammation; Gasdermins; Human Umbilical Vein Endothelial Cells; Cell Proliferation; Macrophages; Lipoproteins; Protein Serine-Threonine Kinases; Virulence; Neuroprotective Agents; Gene Regulatory Networks; Syk Kinase; Toxoplasmosis; Amyloid; Coculture Techniques; Liver; Oxidoreductases; Neuroprotection; Amyloid beta-Peptides; Inflammasomes; YAP-Signaling Proteins; Monocytes; Cognition; Cerebrovascular Circulation; RNA-Seq; Antigen Presentation; Hippo Signaling Pathway; Anti-Infective Agents; NLR Family, Pyrin Domain-Containing 3 Protein; Blood Coagulation; Algorithms; Ion Channels; Acquired Immunodeficiency Syndrome; Memory T Cells; Chemokines; Rabbits; Caspase 8; Immune Evasion; Organelles; Microglia; Inflammation; Cytoskeleton; Toxoplasma; Perfusion; CD8-Positive T-Lymphocytes; Induced Pluripotent Stem Cells; Clustered Regularly Interspaced Short Palindromic Repeats; Neurodegenerative Diseases; Allergy and Immunology; Parasites; Goals; Cell Survival; Mechanotransduction, Cellular; Immunity, Innate; Hemodynamics; Cell Membrane Permeability; HIV Infections; Microvessels; Myeloid Cells; T-Lymphocytes; Skull; Adaptive Immunity; Caspase 3; Infections; Proliferating Cell Nuclear Antigen; Optical Imaging; Neuroinflammatory Diseases; Apoptosis; CARD Signaling Adaptor Proteins; Gene Expression Profiling; Neutrophils; Cell Line; Chemokine CCL2; Capparis; CD4-Positive T-Lymphocytes; Fibrin; Platelet Aggregation; Receptor-Interacting Protein Serine-Threonine Kinases; Persistent Infection; Cells, Cultured; NF-kappa B; Neoplasm Recurrence, Local; Signal Transduction; Coleoptera; Antigens, CD; Phosphate-Binding Proteins; Intercellular Adhesion Molecule-1; Necroptosis; Alzheimer Disease; Metabolic Diseases; T-Lymphocytes, Regulatory; Interleukin-1beta; Extracellular Matrix; Toxoplasmosis, Cerebral; Plaque, Amyloid; Cytosol; Host-Pathogen Interactions; Astrocytes; Receptors, CCR2; AIDS Dementia Complex; Bone Marrow Transplantation; Brain; Heart Transplantation; Endothelial Cells; Communicable Disease Control; Sequence Analysis, RNA; Virulence Factors; Immunity; Coinfection; Caspase 1; THP-1 Cells; Inflammation Mediators; Host-Parasite Interactions; beta Catenin; Lipopolysaccharides; Receptors, Scavenger; Fibroblasts; Protozoan Proteins; Actins; Cell Death; Caspases; Central Nervous System Infections; Neuroimaging; Phagocytosis; Antigens, Ly; CX3C Chemokine Receptor 1; Intracellular Signaling Peptides and Proteins; Blood-Brain Barrier; Up-Regulation; Microscopy; CD11a Antigen; Gene Expression Regulation, Developmental; Life Cycle Stages; Central Nervous System; Stress Fibers; Transcriptome; Preliminary Data; Cell Membrane; Cell Polarity; Transcription Factors; Animals, Newborn; Adaptor Proteins, Signal Transducing; Cytokines; Dendritic Cells; Encephalitis; Phenotype; Cadherins</t>
+          <t>AIDS Dementia Complex; Plaque, Amyloid; Microscopy; Signal Transduction; Adaptor Proteins, Signal Transducing; CD4-Positive T-Lymphocytes; Induced Pluripotent Stem Cells; Syk Kinase; Toxoplasma; Receptors, Scavenger; Hippo Signaling Pathway; Preliminary Data; Fibrin; Antigen Presentation; Phagocytosis; Phenotype; HIV Infections; Anti-Infective Agents; Parasites; Cytokines; Persistent Infection; Cerebrovascular Circulation; Metabolic Diseases; Platelet Aggregation; Dendritic Cells; Microglia; Ion Channels; CD8-Positive T-Lymphocytes; Myeloid Cells; Allergy and Immunology; Neuroimaging; Communicable Disease Control; Central Nervous System Infections; Neuroinflammatory Diseases; Clustered Regularly Interspaced Short Palindromic Repeats; Hemodynamics; Cell Membrane; Neuroprotective Agents; Blood-Brain Barrier; Macrophages; Mechanotransduction, Cellular; Microvessels; Liver; Inflammation; Monocytes; T-Lymphocytes, Regulatory; Adaptive Immunity; Heart Transplantation; Inflammation Mediators; Infections; Neuroprotection; Amyloid; Goals; Chemokine CCL2; Thromboinflammation; Coculture Techniques; Lipoproteins; Encephalitis; Neurodegenerative Diseases; Alzheimer Disease; Memory T Cells; Chemokines; Host-Pathogen Interactions; Brain; Endothelial Cells; Cell Proliferation; Toxoplasmosis, Cerebral; Coinfection; Acquired Immunodeficiency Syndrome; Immunity, Innate; Cognition; Perfusion; Immunity; T-Lymphocytes</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1153,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Crustacea; Computers; Databases, Genetic; Macrophages; Chromatin; DNA; Genetic Predisposition to Disease; OspA protein; Web Browser; Genes, Insect; CRISPR-Cas Systems; Disease Reservoirs; Genotype; Reverse Genetics; Sirolimus; Haplotypes; Animals, Laboratory; Saccharomyces cerevisiae; Drug Resistance, Fungal; Aging; Organ Specificity; Genome, Human; Sequence Homology, Nucleic Acid; Pseudogenes; Research Design; Reactive Nitrogen Species; Tick Bites; Hemocytes; Phosphatidylinositol 3-Kinases; Algorithms; Heterozygote; Arachnid Vectors; Gene Frequency; Evolution, Molecular; United States; Polymorphism, Single Nucleotide; High-Throughput Nucleotide Sequencing; Penaeidae; Genome, Insect; Diptera; Quantitative Trait, Heritable; Genes, MHC Class II; Tick-Borne Diseases; Whole Genome Sequencing; Parents; Genetic Variation; Mutation; Adaptation, Biological; Chromosome Mapping; Animals, Wild; Genetic Association Studies; Insecticides; Software; Species Specificity; Sex Chromosomes; Deer; Chromatin Immunoprecipitation Sequencing; Genes, Homeobox; Muridae; Amino Acid Sequence; Computer Simulation; Genetics; Malathion; Beauveria; Sex Determination Processes; Nerve Tissue; Euchromatin; Homeodomain Proteins; Drosophila; Ecological and Environmental Phenomena; Nitric Oxide; Antibody Formation; Kansas; Gene Expression Profiling; Translational Research, Biomedical; Cell Cycle Proteins; Persistent Infection; Markov Chains; Peromyscus; Genome, Fungal; Lyme Disease; Reproducibility of Results; Ecosystem; Crosses, Genetic; Phylogeny; Sequence Homology; Biological Evolution; Immunization; Saccharomycetales; Breeding; Borrelia; Cell Differentiation; Genomic Structural Variation; Rodent Diseases; Gene Knockout Techniques; Quantitative Trait Loci; Arthropod Proteins; Genome; Molecular Sequence Annotation; Models, Genetic; Ixodes; Exons; Genomics; Sequence Analysis, RNA; Diploidy; DNA, Mitochondrial; Anopheles; Reproduction, Asexual; Borrelia Infections; Drosophila melanogaster; Fungal Proteins; Phagocytes; New Mexico; Genetics, Population; Insecticide Resistance; Selection, Genetic; Spirochaetales; Multifactorial Inheritance; Gene Flow; Genome-Wide Association Study; Saccharomyces cerevisiae Proteins; Hydroxyurea; Recombination, Genetic; Genetic Linkage; Adaptation, Physiological; Immunoglobulin G; Epistasis, Genetic; Alleles; Gene Order; Microsatellite Repeats; Alternative Splicing; Borrelia burgdorferi; Hermaphroditic Organisms; Domestication; Phenotype</t>
+          <t>Antibody Formation; Alleles; OspA protein; Reverse Genetics; Breeding; DNA; Lyme Disease; Phenotype; Kansas; Parents; Haplotypes; Reactive Nitrogen Species; Persistent Infection; Borrelia burgdorferi; Computers; Ecological and Environmental Phenomena; Multifactorial Inheritance; Translational Research, Biomedical; Genes, MHC Class II; Polymorphism, Single Nucleotide; Immunoglobulin G; Genotype; Macrophages; Diptera; Genomics; Biological Evolution; Recombination, Genetic; Models, Genetic; Gene Knockout Techniques; Research Design; Selection, Genetic; Aging; CRISPR-Cas Systems; Peromyscus; Drosophila; Saccharomyces cerevisiae; Immunization; Genetics; Gene Frequency; Genetics, Population; Genome-Wide Association Study; Phagocytes; Nitric Oxide</t>
         </is>
       </c>
     </row>
@@ -1185,7 +1165,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Proteins; Escherichia coli; Molecular Dynamics Simulation; Biomarkers; Glucose 1-Dehydrogenase; Drug Discovery; Protein Serine-Threonine Kinases; Mutation; Binding Sites; Entropy; Protein Conformation; Computational Biology; Signal Transduction; Amino Acids; Early Detection of Cancer; Antineoplastic Agents; Glycine; Loss of Function Mutation; Oxidoreductases; Protein Tyrosine Phosphatase, Non-Receptor Type 11; Bioreactors; Liver Neoplasms; NAD; Allosteric Site; Oxidation-Reduction; NADP; Carbohydrates; Head and Neck Neoplasms; Peptides; Mutation, Missense; Biocatalysis; Allosteric Regulation; Lung Neoplasms; Static Electricity; Neurofibromin 2; Protein Biosynthesis; Gas Chromatography-Mass Spectrometry; Polymers; Volatile Organic Compounds; Protein Binding; Neoplasms; Amines; Hippo Signaling Pathway; Water; Pyrimidines; Carcinoma, Hepatocellular; Proteome; Adenosine Triphosphate; Phase Separation; Artificial Cells; Nicotinamide Mononucleotide; Hydrogen; Cell Line; Adaptor Proteins, Signal Transducing; Cell Line, Tumor; Drug Delivery Systems; Models, Molecular; Molecular Conformation; Dipeptides; Proteomics; Reproduction; Liver Cirrhosis; Nucleic Acids; Intrinsically Disordered Proteins</t>
+          <t>Molecular Dynamics Simulation; Allosteric Regulation; Computational Biology; Protein Biosynthesis; Intrinsically Disordered Proteins</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1177,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Receptors, AMPA; Memory; Noise; Action Potentials; Swimming; Neurons; Synapses; Adolescent; Calcium Signaling; Neuroimaging; Synaptic Transmission; Electronic Nicotine Delivery Systems; Functional Laterality; GABA Agonists; Patch-Clamp Techniques; Feedback; Signal Transduction; Calcium; Wakefulness; Ketamine; Video Recording; Software; Neurosciences; Postsynaptic Potential Summation; Nicotinic Agonists; Muscimol; Nicotine; Immunohistochemistry; Memory, Short-Term; Neurotransmitter Agents; Receptors, GABA; Receptors, Purinergic P2; Parietal Lobe; Nerve Net; Pyramidal Cells; Depression; Prefrontal Cortex; Electrophysiological Phenomena; Restraint, Physical; Interneurons; Cognition; Models, Neurological; Genetics; Movement; Stress, Psychological; Adverse Childhood Experiences; Central Nervous System; Cerebral Cortex; Vasoactive Intestinal Peptide; Brain; N-Methylaspartate; Antidepressive Agents; Electrophysiology; Adenosine Triphosphate; Algorithms; Behavior, Animal; Habenula; Spatial Memory; Decision Making; Calcium Channels; Synaptic Potentials; Photons; Glutamine; Cholinergic Neurons; Optogenetics; Psychomotor Performance; Reward; Visual Perception</t>
+          <t>Stress, Psychological; Parietal Lobe; Memory; Postsynaptic Potential Summation; Memory, Short-Term; Synapses; Electrophysiology; Optogenetics; Adverse Childhood Experiences; Patch-Clamp Techniques; Cognition; Genetics; Decision Making; Calcium Channels; Central Nervous System</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1189,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Temperature; Behavior, Animal; Hibernation; Physiology, Comparative; Stress, Physiological; Ecological and Environmental Phenomena; Body Temperature Regulation; Periodicity; Life History Traits; Hormones; Seasons; Neurobiology; Brain</t>
+          <t>Stress, Physiological; Life History Traits; Seasons; Neurobiology; Hormones; Hibernation; Behavior, Animal; Ecological and Environmental Phenomena; Temperature; Periodicity; Body Temperature Regulation; Physiology, Comparative</t>
         </is>
       </c>
     </row>
@@ -1219,11 +1199,7 @@
           <t>MacGregor, Grant</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>ATP-Binding Cassette Transporters; Gene Regulatory Networks; Single-Cell Analysis; Genotype; Amyloid beta-Peptides; Risk Factors; NAV1.1 Voltage-Gated Sodium Channel; Seizures; Mutation, Missense; Cystatins; Gene Knock-In Techniques; Melanocytes; Insulin; RNA-Seq; Demyelinating Diseases; Energy Metabolism; Tauopathies; Phosphatidylinositol 3-Kinases; Apolipoproteins E; Neuronal Plasticity; Cell Line, Tumor; Reactive Oxygen Species; Microglia; RNA Splicing; Diabetes Mellitus; Neurons; Disease Progression; Metabolomics; Mutation; Genetic Variation; Synaptic Transmission; Mitochondria, Heart; Cuprizone; Pigmentation; Microphthalmia-Associated Transcription Factor; tau Proteins; Neuroinflammatory Diseases; Behavior, Animal; Apoptosis; Gene Expression Profiling; Retinoids; Hippocampus; Receptors, Immunologic; Murine hepatitis virus; Reperfusion Injury; Coronavirus Infections; Homeostasis; Signal Transduction; Eye; Alzheimer Disease; T-Lymphocytes, Regulatory; Plaque, Amyloid; Interneurons; Proto-Oncogene Proteins c-akt; Sex Characteristics; Astrocytes; Oxidative Phosphorylation; Protein Binding; Promoter Regions, Genetic; Acute Kidney Injury; Brain; Heart Transplantation; Protein Isoforms; Seizures, Febrile; Adenosine Triphosphate; DNA, Mitochondrial; Microbiota; Myocardium; Mitochondria; Diabetic Cardiomyopathies; Binding Sites; Phagocytosis; Amyloid beta-Protein Precursor; Neuroglia; Resilience, Psychological; Gene Ontology; Gastrointestinal Microbiome; Transcriptome; Kidney; Retinoic Acid Receptor alpha; Membrane Glycoproteins; Long-Term Potentiation; Renal Insufficiency, Chronic; HEK293 Cells; Phenotype</t>
-        </is>
-      </c>
+      <c r="B66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1233,7 +1209,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Ovarian Reserve; Ovarian Follicle; Nucleus Accumbens; Behavior, Addictive; Designer Drugs; Adolescent; Retention, Psychology; Dopaminergic Neurons; Rodentia; Dronabinol; Neurobiology; gamma-Aminobutyric Acid; Substance-Related Disorders; Analgesics, Opioid; Neural Pathways; Growth and Development; Neurosciences; Cannabis; Tandem Mass Spectrometry; Motivation; Amphetamine; Rats, Long-Evans; Anhedonia; Endocannabinoids; Rats, Transgenic; Prefrontal Cortex; Cognition; Clozapine; Genetics; Adverse Childhood Experiences; Stress, Psychological; Rats, Sprague-Dawley; Dose-Response Relationship, Drug; Dopamine; Cannabidiol; GABAergic Neurons; Ventral Tegmental Area; Basolateral Nuclear Complex; Choice Behavior; Arachidonic Acids; Brain; Aerosols; Learning; Corticotropin-Releasing Hormone; Memory, Episodic; Behavior, Animal; Basal Forebrain; Vaping; Time Factors; Sex Factors; Mass Spectrometry; Chromatography, High Pressure Liquid; Polyunsaturated Alkamides; Olfactory Perception; Microsomes; Reward</t>
+          <t>Growth and Development; Vaping; Neurobiology; Analgesics, Opioid; Neural Pathways; Genetics; Motivation; Basal Forebrain; Substance-Related Disorders; Cannabis</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1221,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Carbon; Biomechanical Phenomena; Swimming; Natural History; Ecosystem; Phylogeny; Biological Evolution; Somatotypes; Fishes; Jaw; Predatory Behavior; Perciformes; Mandible; Movement; Extinction, Biological; Water; Ecological and Environmental Phenomena; Coral Reefs; Evolution, Molecular; Motion; Feeding Behavior; Genetic Speciation</t>
+          <t>Feeding Behavior; Ecological and Environmental Phenomena; Natural History; Fishes; Biological Evolution; Biomechanical Phenomena; Movement; Motion; Swimming; Genetic Speciation; Evolution, Molecular</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1233,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Carbon; Escherichia coli; Biodiversity; Metagenome; Aquatic Organisms; Climate Change; Genome, Microbial; Ecosystem; Phylogeny; Genetic Variation; Life History Traits; Metagenomics; Adaptation, Biological; Soil Microbiology; Soil; Nutrients; Uncertainty; Temperature; Drug Resistance, Multiple, Bacterial; Stress, Physiological; Escherichia coli Infections; Phosphorus; California; Oceanography; Pacific Ocean; Plankton; Ecotype; Synechococcus; Nitrogen; Microbiology; Drug Resistance, Bacterial; Seawater; Genetics; Genomic Library; Atlantic Ocean; Indian Ocean; Oceans and Seas; Anti-Bacterial Agents; Nitrates; Seasons; Phylogeography; Ecological and Environmental Phenomena; Nitrogen Fixation; Adaptation, Physiological; Microbial Sensitivity Tests; Genomics; Proteome; Genes, Bacterial; Phytoplankton; Carbon Cycle; Prochlorococcus; Phosphates; Microbiota; El Nino-Southern Oscillation; Bayes Theorem; Iron; Bacteria</t>
+          <t>Carbon Cycle; Ecological and Environmental Phenomena; Plankton; Genomics; Microbiology; Oceanography; Ecosystem; Microbiota; Genetics; Climate Change</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1245,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Students; Human Body; Diet; Climate Change; Databases, Genetic; Oregon; Metagenomics; Ambulatory Care Facilities; Uncertainty; California; Noncommunicable Diseases; Cyanobacteria; Droughts; Nitrogen Fixation; Gene Transfer, Horizontal; Masks; Ohio; United States; Drought Resistance; Biodiversity; Metagenome; Diabetes Mellitus; Feces; Metabolomics; Probiotics; Genetic Variation; Mutation; Soil Microbiology; Computational Biology; Feedback; Cervix Uteri; Metadata; Goals; Interspersed Repetitive Sequences; Ecotype; Carbohydrates; Chromatography, Liquid; Healthy Volunteers; Microbiology; Mentors; Pacific Island People; Ecological and Environmental Phenomena; Pregnancy; Mycobiome; Actinomycetales; Carbon; Wildfires; Leadership; Reproducibility of Results; Ecosystem; American Indian or Alaska Native; Phylogeny; Biological Evolution; Vagina; Stress, Physiological; Genetic Engineering; Fermentation; Tandem Mass Spectrometry; Workflow; Nitrogen; Internship and Residency; Cardiovascular Diseases; Metabolome; Anti-Bacterial Agents; Bays; Prebiotics; Desert Climate; Genomics; Universities; Curriculum; Ecology; Cohort Studies; Bifidobacterium; Greenhouse Gases; Plant Leaves; Microbiota; Follow-Up Studies; Biotechnology; Schools; Infant; Electrons; Life History Traits; New Mexico; Soil; DNA Methylation; Actinobacteria; Carbon Sequestration; Resilience, Psychological; Gastrointestinal Microbiome; Neoplasms; Water Purification; Adaptation, Physiological; Dietary Fiber; Plasmids; Young Adult; Time Factors; RNA, Ribosomal, 16S; Bacteria</t>
+          <t>Diet; Metagenome; Follow-Up Studies; Schools; Actinomycetales; Gene Transfer, Horizontal; Microbiota; Computational Biology; Leadership; Metagenomics; Genetic Engineering; Pacific Island People; Human Body; Plasmids; Students; United States; Diabetes Mellitus; Electrons; Ecological and Environmental Phenomena; Mutation; Microbiology; New Mexico; Ambulatory Care Facilities; Cardiovascular Diseases; Fermentation; Oregon; Internship and Residency; Anti-Bacterial Agents; Time Factors; Interspersed Repetitive Sequences; Neoplasms; Masks; Water Purification; Feedback; Soil; Bacteria; Probiotics; Resilience, Psychological; Bifidobacterium; Ohio; Genomics; Carbohydrates; Universities; Biological Evolution; Gastrointestinal Microbiome; Goals; Metadata; DNA Methylation; Bays; Droughts; Genetic Variation; Curriculum; Dietary Fiber; Prebiotics; American Indian or Alaska Native; Carbon Sequestration; Mentors; Workflow; Ecology; Biotechnology; Noncommunicable Diseases; Climate Change</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1257,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Crustacea; Hydrodynamics; Biomechanical Phenomena; Swimming; Students; Zebrafish; Technology; Vision, Ocular; Smegmamorpha; Social Behavior; Fundulidae; Robotics; Faculty; Fishes; Organizations; Video Recording; Water Movements; Animals, Wild; Locomotion; Mechanoreceptors; Spatial Navigation; Perception; Schools; Goals; Predatory Behavior; Fresh Water; Perciformes; Sense Organs; Lateral Line System; Larva; Cockroaches; Walking; Skeleton; Mantodea; Cypriniformes; Oligochaeta; Characidae; Movement; Starfish; Escape Reaction; Scyphozoa; Mentors; Food Chain; Interpersonal Relations; Communication; Mentoring; Ecological and Environmental Phenomena; Genomics; Behavior, Animal; Animal Communication; Cues; Stroboscopy; Gait; Environment; Educational Status; Feeding Behavior</t>
+          <t>Locomotion; Predatory Behavior; Behavior, Animal; Fishes; Schools; Lateral Line System; Movement; Swimming; Organizations; Sense Organs; Students; Hydrodynamics; Ecological and Environmental Phenomena; Smegmamorpha; Biomechanical Phenomena; Cues; Fresh Water; Animals, Wild; Mentoring; Communication; Goals; Faculty; Mentors; Cypriniformes</t>
         </is>
       </c>
     </row>
@@ -1293,7 +1269,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Acoustic Stimulation; Hindlimb; Action Potentials; Deep Learning; Neurons; Neural Networks, Computer; Ketanserin; Hallucinogens; Evoked Potentials, Auditory; Frontal Lobe; Temporal Lobe; Amygdala; Wakefulness; History, 21st Century; Software; Neurosciences; Spatial Navigation; Consciousness; Cognitive Reserve; Default Mode Network; Forelimb; Sleep, REM; Reward; Anesthesia, General; Evoked Potentials, Visual; Memory, Short-Term; Sleep, Slow-Wave; Brain Diseases; Computer Simulation; Serotonin 5-HT2 Receptor Antagonists; Electrophysiological Phenomena; Memory Consolidation; Cognition; Models, Neurological; Auditory Cortex; Place Cells; Maze Learning; Electroencephalography; Voltage-Sensitive Dye Imaging; Cerebral Cortex; Imaging, Three-Dimensional; Sleep; Gyrus Cinguli; Systems Theory; Sensory Thresholds; Brain; Psilocybin; Learning; Space Perception; Memory, Episodic; Electrophysiology; Young Adult; Brain Mapping; Nesting Behavior; Cues; Brain Waves; Time Factors; Electrocorticography; Neuronal Plasticity; Grid Cells; Photic Stimulation; Optogenetics; History, 20th Century; Memory; Hippocampus; Electric Stimulation; Neocortex</t>
+          <t>Sleep; Deep Learning; Memory; Electronic Mail; Memory, Short-Term; Memory Disorders; Brain Stem; Cognitive Reserve; Behavior Therapy; Brain Diseases; Stroke; GABAergic Neurons; Hippocampal Sclerosis; Default Mode Network; Neocortex; ET protocol; Cues; Sleep Deprivation; Feasibility Studies; Autistic Disorder; Imaging, Three-Dimensional; Memory Consolidation; Learning; Pilot Projects; Neuronal Plasticity; Synapses; Universities; Adverse Childhood Experiences; Goals; Place Cells; Control Groups; Computer Simulation; Schizophrenia; Brain; Neuroanatomy; Optogenetics; Hippocampus; Memory, Episodic; Silicon; Neurons; Grid Cells</t>
         </is>
       </c>
     </row>
@@ -1305,7 +1281,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Proteins; Regeneration; Gasdermins; Fructose; Bacterial Infections; Interleukin-18; Lipidomics; DNA, Viral; Macrophages; Drug Discovery; Cell Culture Techniques; DNA; Toll-Like Receptors; Mitochondria; Gene Editing; Binding Sites; Interleukin-1; Protein Processing, Post-Translational; Capsid; Signal Transduction; Allergy and Immunology; Acetyl Coenzyme A; Protein Subunits; Pyrin; Fluorocarbons; CRISPR-Cas Systems; Goals; Cell Survival; Cryopyrin-Associated Periodic Syndromes; Ligands; Liver Neoplasms; Inflammasomes; Virus Assembly; Interleukin-1beta; Endodeoxyribonucleases; Lipogenesis; Clostridium acetobutylicum; Immune System; Oxides; Galium; Non-alcoholic Fatty Liver Disease; Mitochondrial Diseases; Gastrointestinal Microbiome; Macromolecular Substances; Pathogen-Associated Molecular Pattern Molecules; RNA; Oxidative Stress; Protein Binding; Heat-Shock Response; Neoplasms; Imaging, Three-Dimensional; Microscopy, Electron, Transmission; Cryoelectron Microscopy; Endotoxemia; NLR Family, Pyrin Domain-Containing 3 Protein; DNA Glycosylases; Signal-To-Noise Ratio; Membrane Fluidity; Epithelium; Carcinoma, Hepatocellular; Apoptosis; Fructosephosphates; Mass Spectrometry; DNA, Mitochondrial; Mutagenesis; Host Microbial Interactions; Cytokines; Pyrin Domain; Intestines; Molecular Structure; Caspase 1; Bacteria; Bacteriophage P22; Hepatocytes; Nucleic Acids; Inflammation</t>
+          <t>Mutagenesis; Interleukin-1; Host Microbial Interactions; Signal Transduction; Molecular Structure; Ligands; Immune System; Pyrin; Cryopyrin-Associated Periodic Syndromes; Pathogen-Associated Molecular Pattern Molecules; Cytokines; Gene Editing; Cell Culture Techniques; Macromolecular Substances; Protein Processing, Post-Translational; Allergy and Immunology; Fluorocarbons; Interleukin-18; Binding Sites; Epithelium; Neoplasms; Interleukin-1beta; Membrane Fluidity; Pyrin Domain; Oxidative Stress; Caspase 1; Bacteria; Cryoelectron Microscopy; Inflammation; Cell Survival; Bacterial Infections; Heat-Shock Response; Galium; Liver Neoplasms; Mitochondrial Diseases; DNA, Mitochondrial; Carcinoma, Hepatocellular; Goals; Gasdermins; Apoptosis; Non-alcoholic Fatty Liver Disease; CRISPR-Cas Systems; Mitochondria; Inflammasomes; NLR Family, Pyrin Domain-Containing 3 Protein; Oxides</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1293,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Evoked Potentials, Auditory, Brain Stem; Fluorescent Dyes; GABA Agents; Non-Smokers; Evoked Potentials, Auditory; Aged, 80 and over; Neural Pathways; Auditory Perception; Cognitive Dysfunction; Nicotine; Receptors, Nicotinic; Aging; Cognition; Analysis of Variance; Electrical Synapses; Rats, Sprague-Dawley; Cerebral Cortex; Research Design; Signal-To-Noise Ratio; Sensation Disorders; GABA-A Receptor Agonists; Cross-Over Studies; Receptors, GABA-B; Action Potentials; Neurons; Tissue Distribution; Nootropic Agents; Muscimol; Attention; Inhibitory Postsynaptic Potentials; Healthy Volunteers; Auditory Cortex; Aged; Oxygen; Dose-Response Relationship, Drug; Cognition Disorders; Vasoactive Intestinal Peptide; Oximetry; Optical Imaging; Structure-Activity Relationship; Psychomotor Performance; Hippocampus; Macaca mulatta; Adolescent; Pitch Perception; Oxadiazoles; Alzheimer Disease; Pyramidal Cells; Thalamus; Physiology; Discrimination, Psychological; Interneurons; Sex Characteristics; Hearing; Positron-Emission Tomography; Protein Binding; Brain; Schizophrenia; Nicotine Chewing Gum; Acoustic Stimulation; Receptors, N-Methyl-D-Aspartate; Binding Sites; Auditory Pathways; Entorhinal Cortex; Affect; Auditory Perceptual Disorders; Nicotinic Agonists; Pyrroles; Pyridines; Acoustics; Microinjections; Receptors, Glutamate; Acetylcholine; Young Adult; Time Factors; HEK293 Cells; Molecular Structure; Pharmaceutical Preparations; Single-Blind Method</t>
+          <t>Alzheimer Disease; Entorhinal Cortex; Nicotine; Nicotinic Agonists; Auditory Cortex; Physiology; Acetylcholine; Interneurons; Receptors, Nicotinic; Pharmaceutical Preparations; Cognition; Hippocampus; Hearing; Auditory Perceptual Disorders; Neurons; Nootropic Agents; Auditory Perception; Cognitive Dysfunction</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1305,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Home Environment; Ficus; Biodiversity; Students; Climate; Climate Change; Seeds; Plant Development; Trees; Ecosystem; Genetic Variation; Biological Evolution; Songbirds; Flowers; Natural Resources; Brassicaceae; Birds; Temperature; Biological Phenomena; Biota; Snow; Biomass; Genotype; Schools; Predatory Behavior; Ecotype; Larva; Oxylipins; Monoterpenes; Host-Parasite Interactions; Quercus; Weather; Wasps; Volatile Organic Compounds; Quantitative Trait Loci; Sesquiterpenes; Plants; Food Chain; Seasons; Insecta; Droughts; Reproduction; Mentoring; Ecology; Colorado; Curriculum; Ants; Arthropods; Behavior, Animal; Symbiosis; Cues; Aphids; Plant Physiological Phenomena; Lepidoptera; Alleles; Artemisia; Plant Leaves; Genotyping Techniques; Herbivory; Baccharis; Phenotype; Drought Resistance</t>
+          <t>Ficus; Alleles; Schools; Ecotype; Herbivory; Phenotype; Students; Home Environment; Snow; Colorado; Mentoring; Biological Phenomena; Quantitative Trait Loci; Biological Evolution; Droughts; Genetic Variation; Brassicaceae; Curriculum; Natural Resources; Biota; Drought Resistance; Climate Change</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1317,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Proteins; Ribonucleotides; cyclic guanosine monophosphate-adenosine monophosphate; Lipopolysaccharides; Postdoctoral Training; Toll-Like Receptor 4; Autoimmune Diseases; Prokaryotic Cells; Phylogeny; Biological Evolution; Virus Diseases; Cell Death; Drug Resistance, Microbial; Cyclization; Membrane Proteins; Signal Transduction; Second Messenger Systems; Allergy and Immunology; Amino Acids; Phage Therapy; Virus Replication; Oligonucleotides; Cyclic AMP; Nucleotides; CRISPR-Cas Systems; Pandemics; Nucleotidyltransferases; NAD; Immunity, Innate; Bacteriophages; Immune System; Microbiology; Archaea; Eukaryota; Cytosol; Genome, Human; Crystallography, X-Ray; Cyclic GMP; Defense Mechanisms; Interferons; Neoplasms; Preliminary Data; Antiviral Agents; cyclic 3',5'-uridine monophosphate; Virus Activation; Anti-Infective Agents; Delivery of Health Care; Cryoelectron Microscopy; Pyrimidines; Ion Channels; Chromatography, High Pressure Liquid; Biochemistry; Mutagenesis; Host Microbial Interactions; Evolution, Molecular; Uridine Monophosphate; Molecular Structure; Planets; Microbiota; Mammals; Nucleotides, Cyclic; 2',5'-oligoadenylate; Incidence; Nucleic Acids; Bacteria</t>
+          <t>Nucleotides, Cyclic; Autoimmune Diseases; Mutagenesis; Signal Transduction; Cyclization; Host Microbial Interactions; Virus Diseases; Immune System; Mammals; Postdoctoral Training; Molecular Structure; Microbiota; Preliminary Data; Anti-Infective Agents; Bacteriophages; Second Messenger Systems; Ion Channels; Cytosol; Phage Therapy; cyclic guanosine monophosphate-adenosine monophosphate; Pandemics; Microbiology; Drug Resistance, Microbial; Allergy and Immunology; Delivery of Health Care; Pyrimidines; Proteins; Ribonucleotides; Evolution, Molecular; Crystallography, X-Ray; Incidence; cyclic 3',5'-uridine monophosphate; Nucleotides; Bacteria; Nucleotidyltransferases; Interferons; Cryoelectron Microscopy; Nucleic Acids; Biological Evolution; Defense Mechanisms; Chromatography, High Pressure Liquid; Lipopolysaccharides; Archaea; Oligonucleotides; Eukaryota; Phylogeny; Amino Acids; Uridine Monophosphate; NAD; Cell Death; Antiviral Agents; Toll-Like Receptor 4; 2',5'-oligoadenylate; CRISPR-Cas Systems; Immunity, Innate; Virus Replication; Virus Activation; Genome, Human; Planets; Biochemistry</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1329,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Bacterial Infections; Tetrahymena; Cell Proliferation; Vertebrates; Databases, Genetic; Malaria; Virulence; Molecular Sequence Data; pironetin; Thioredoxin-Disulfide Reductase; Toxoplasmosis; Germ Cells; Paclitaxel; Microtubule-Associated Proteins; Embryophyta; Morbidity; Mutation, Missense; Heme; Colchicine; Meiosis; Histamine Antagonists; Protein Multimerization; Helminths; Electron Transport Complex IV; pendimethalin; Protein Transport; Mitosis; Reactive Oxygen Species; User-Computer Interface; Clemastine; Drug Resistance; Auranofin; Cytoskeleton; Xenopus laevis; Toxoplasma; Mutation; Parasites; Goals; Tropism; Ligands; Immunity, Innate; Micronucleus, Germline; Cytochromes c; Vero Cells; Amino Acid Sequence; Transfection; Protein Stability; HeLa Cells; Staining and Labeling; Mammals; Amino Acid Substitution; Microtubules; Tubulin; Cells, Cultured; Cryptosporidium; Household Work; Phospholipases; Trypanosoma cruzi; Communicable Diseases; Centrosome; Paromomycin; Chemistry, Pharmaceutical; Chlorocebus aethiops; Genes, Essential; oryzalin; Eukaryota; Kinetochores; Host-Pathogen Interactions; Cell Compartmentation; Protein Binding; Spindle Apparatus; Protein Structure, Secondary; Treatment Outcome; Macronucleus; Herbicides; Solubility; Virulence Factors; Cryptosporidium parvum; pronamide; Haploidy; Apicoplasts; Mice, Inbred BALB C; Biolistics; Protozoan Proteins; Cryptosporidiosis; Binding Sites; Chlamydomonas; Carbohydrate Metabolism; Amino Acids; Glycoproteins; Recombination, Genetic; Neoplasms; Chromosome Segregation; Plasmids; Antiparasitic Agents; Pharmaceutical Preparations; Tubulin Modulators</t>
+          <t>Treatment Outcome; Chlamydomonas; Drug Resistance; Chemistry, Pharmaceutical; Mammals; Toxoplasma; Tubulin; pronamide; pironetin; Transfection; Parasites; Plasmids; Germ Cells; Microtubules; Cryptosporidiosis; Tetrahymena; Micronucleus, Germline; Household Work; Malaria; Vertebrates; pendimethalin; Macronucleus; oryzalin; Mutation, Missense; Cryptosporidium parvum; Neoplasms; Meiosis; Recombination, Genetic; Paromomycin; Biolistics; Tropism; Helminths; Goals; Eukaryota; Colchicine; Herbicides; Embryophyta; Solubility; Mitosis; Cryptosporidium; Paclitaxel; Pharmaceutical Preparations; Morbidity; Genes, Essential; Haploidy; Communicable Diseases; Amino Acid Substitution</t>
         </is>
       </c>
     </row>
@@ -1365,7 +1341,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Microglia; Deep Learning; Neurons; ATP-Binding Cassette Transporters; Chromatin; Genetic Variation; Receptor, Anaphylatoxin C5a; Phagocytosis; Gene Regulatory Networks; Signal Transduction; Single-Cell Analysis; Cell Differentiation; Amyloid beta-Protein Precursor; Electromyography; DNA Methylation; Alzheimer Disease; Amyloid beta-Peptides; Neuroglia; Plaque, Amyloid; Resilience, Psychological; Astrocytes; Machine Learning; Transcriptome; RNA-Seq; Molecular Sequence Annotation; Wearable Electronic Devices; Homeodomain Proteins; Brain; Myoblasts; Genomics; Sequence Analysis, RNA; Algorithms; Gene Expression Profiling; Gestures; Muscle Fibers, Skeletal; Muscular Dystrophy, Facioscapulohumeral; In Situ Hybridization, Fluorescence; Hippocampus; Forearm; High-Throughput Nucleotide Sequencing</t>
+          <t>Alzheimer Disease; Chromatin; Genomics; Gene Regulatory Networks; Machine Learning; Sequence Analysis, RNA; High-Throughput Nucleotide Sequencing; DNA Methylation; Muscular Dystrophy, Facioscapulohumeral; Single-Cell Analysis</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1353,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Proteins; Cell Fractionation; Cell Proliferation; Diet; Diabetes Mellitus, Type 2; Ovarian Neoplasms; Research Personnel; Carrier Proteins; B-Lymphocyte Subsets; Pandemics; Quality of Life; Coculture Techniques; Lipid Metabolism; Autoantibodies; Losartan; Gonadal Steroid Hormones; Lymphocytic choriomeningitis virus; Heterocyclic Compounds, 3-Ring; Lymphocytic Choriomeningitis; Protein Array Analysis; Risk Factors; Single-Cell Gene Expression Analysis; Sphingosine-1-Phosphate Receptors; Interleukin-17; Aging; Flow Cytometry; Gene Expression Regulation, Neoplastic; Glycolysis; Lactones; Biocompatible Materials; Lipids; Pituitary Diseases; Androgens; Enzyme Inhibitors; Insulin; Antigen Presentation; Protein Transport; Anilides; Infertility; Autoantigens; Cell Line, Tumor; Reproduction; Drug Evaluation, Preclinical; Diabetes Mellitus; Antibodies, Neutralizing; Autoimmune Diseases; Anti-Inflammatory Agents; Glucose; Mexican Americans; Weight Loss; Disease Progression; CD8-Positive T-Lymphocytes; Cell Plasticity; polyvinylidene fluoride; Luteinizing Hormone; Industrial Development; Allergy and Immunology; Organoids; Goals; Cell Survival; Polycystic Ovary Syndrome; Glucose Transporter Type 1; Adiposity; Computer Simulation; Palatine Tonsil; COVID-19; Aged; T-Lymphocytes; Cross-Sectional Studies; Anabolic Androgenic Steroids; Fertility; H3B-8800; Solvents; Prevalence; Adaptive Immunity; Diet, High-Fat; Metabolic Networks and Pathways; Apoptosis; Antibody Formation; Gene Expression Profiling; Neoplastic Stem Cells; Cell Line; Follicle Stimulating Hormone; Insulin Resistance; Persistent Infection; Th17 Cells; Technology; Blood Glucose; Obesity; Homeostasis; Culture Media, Conditioned; Signal Transduction; Receptor, PAR-1; Sulfones; Sedentary Behavior; Lymphoid Tissue; Cell Differentiation; Ethnic and Racial Minorities; Workflow; Pyrrolidines; Cardiovascular Diseases; Preceptorship; Platelet Aggregation Inhibitors; Proto-Oncogene Proteins c-akt; Antibodies; Mice, Obese; Antigens, CD1; Adipose Tissue; Metabolism; Cardiac Output; Pituitary Gland; Endothelial Cells; Protein C; Proprotein Convertase 9; Influenza Vaccines; Sequence Analysis, RNA; Phosphotransferases (Alcohol Group Acceptor); Cellular Senescence; Glycated Hemoglobin; Professional Competence; Gonadotropins; Methanol; Inflammation Mediators; Follow-Up Studies; lobeglitazone; Lipopolysaccharides; Memory B Cells; RNA, Long Noncoding; beta-Arrestin 2; Gene Expression Regulation; Gonadotropins, Pituitary; Phenotype; Laboratories; Pyridines; Endocrinology; Immunotherapy; Printing, Three-Dimensional; Up-Regulation; Transcriptome; Cell Membrane; Preliminary Data; Testosterone; Organophosphonates; Cytokines; Immunophenotyping; Inflammation</t>
+          <t>Carrier Proteins; Preliminary Data; Lymphoid Tissue; Culture Media, Conditioned; Cytokines; Th17 Cells; Printing, Three-Dimensional; Immunotherapy; Memory B Cells; Palatine Tonsil; Mice, Obese; Metabolism; Testosterone; Lipid Metabolism; Coculture Techniques; Cellular Senescence; Anti-Inflammatory Agents; Luteinizing Hormone; Endocrinology; Technology; Organoids; Cell Line; Flow Cytometry; Diet; Follow-Up Studies; Immunophenotyping; Antigen Presentation; Fertility; Diabetes Mellitus; Solvents; Reproduction; Single-Cell Gene Expression Analysis; Polycystic Ovary Syndrome; Proteins; Lipids; Research Personnel; Influenza Vaccines; Inflammation; Disease Progression; Antigens, CD1; Inflammation Mediators; Glucose Transporter Type 1; Glycated Hemoglobin; Cross-Sectional Studies; Aging; Mexican Americans; Workflow; Glycolysis; Infertility; Sedentary Behavior; Prevalence; Antibody Formation; Autoimmune Diseases; Anabolic Androgenic Steroids; Weight Loss; H3B-8800; Losartan; Aged; Antibodies; Glucose; Phenotype; Industrial Development; Diabetes Mellitus, Type 2; Obesity; Preceptorship; Insulin Resistance; Drug Evaluation, Preclinical; B-Lymphocyte Subsets; Autoantigens; Follicle Stimulating Hormone; Gonadotropins; Biocompatible Materials; Adaptive Immunity; Gonadal Steroid Hormones; Risk Factors; Methanol; polyvinylidene fluoride; Interleukin-17; Antibodies, Neutralizing; Sequence Analysis, RNA; Cardiac Output; T-Lymphocytes; Metabolic Networks and Pathways; Pituitary Gland; Diet, High-Fat; Autoantibodies; Androgens; Quality of Life; Professional Competence; Cardiovascular Diseases; Allergy and Immunology; Protein Array Analysis; Blood Glucose; Homeostasis; Lipopolysaccharides; Goals; Adipose Tissue; lobeglitazone; Computer Simulation; Gene Expression Profiling; Ethnic and Racial Minorities</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1365,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Proteins; Macrophages; RANK Ligand; Wound Healing; Gene Regulatory Networks; Single-Cell Analysis; Rosacea; Lipid Metabolism; Chickens; Programmed Cell Death 1 Receptor; Single-Cell Gene Expression Analysis; Marsupialia; Oligodeoxyribonucleotides; Schwann Cells; Gelatin; Lymphocytes; Biocompatible Materials; Morphogenesis; Keratinocytes; RNA-Seq; SARS-CoV-2; Algorithms; Lamin Type A; Cell Line, Tumor; Evolution, Molecular; Adjuvants, Vaccine; Multiomics; Down-Regulation; Lipid A; Cartilage; RNA Splicing; Epigenomics; Antibodies, Neutralizing; Mutation; CD8-Positive T-Lymphocytes; Induced Pluripotent Stem Cells; Orthomyxoviridae Infections; Immune Checkpoint Inhibitors; Computational Biology; Islets of Langerhans; Locomotion; Software; Myocytes, Cardiac; Lipid Droplets; Computer Simulation; COVID-19; T-Lymphocytes; Vacuoles; Epithelial-Mesenchymal Transition; Cluster Analysis; Homeodomain Proteins; Connectome; Adipocytes; Gene Expression Profiling; Biomechanical Phenomena; Phylogeny; Obesity; Homeostasis; Signal Transduction; Cell Differentiation; Alzheimer Disease; T-Lymphocytes, Regulatory; Extracellular Matrix; Interleukin-2; Drug Repositioning; Embryo, Mammalian; Genome; Brain; Influenza Vaccines; Genomics; Endothelial Cells; Sequence Analysis, RNA; Pericardium; Influenza A Virus, H5N1 Subtype; Antibodies, Viral; Systems Biology; Melanoma, Experimental; Mice, Inbred BALB C; Cell Communication; Fibroblasts; RNA, Messenger; Melanoma; Cardiomyopathy, Dilated; Gene Expression Regulation; Squalene; Cross-Linking Reagents; Regulatory Sequences, Nucleic Acid; Skin; Haploinsufficiency; Lipogenesis; Adjuvants, Immunologic; Immunotherapy; Gene Expression Regulation, Developmental; Transcriptome; Cell Lineage; Embryonic Development; Hydrogels; Polysorbates; Transcription Factors; Young Adult; Big Data; Developmental Biology; Inducible T-Cell Co-Stimulator Protein; Phenotype; Inflammation</t>
+          <t>Computer Simulation; Systems Biology; Computational Biology; Developmental Biology; Multiomics; Single-Cell Analysis</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1377,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Students; BRCA2 Protein; Genetic Testing; Tyrphostins; Diabetes Mellitus, Type 2; Ovarian Neoplasms; Estrogens; Genetic Predisposition to Disease; Quinazolines; Liver; Hispanic or Latino; BRCA1 Protein; Penetrance; Genotype; Risk Factors; White People; Head and Neck Neoplasms; Lung Neoplasms; Animals, Laboratory; Volunteers; Enzyme Inhibitors; Antigen Presentation; Thinking; Hyperglycemia; Colorectal Neoplasms; Bayes Theorem; Cilia; Polymorphism, Single Nucleotide; Adenocarcinoma; Optimism; Insulins; Inflammation; RNA Splicing; Diabetes Mellitus; Zebrafish; Prospective Studies; Disease Progression; Genetic Variation; Mutation; Risk Assessment; Chromosome Mapping; Workforce; Homozygote; Feedback; Islets of Langerhans; Bicarbonates; Case-Control Studies; Triple Negative Breast Neoplasms; Pancreas, Exocrine; Mental Disorders; Genetic Phenomena; Breast Neoplasms; Epithelium; Carcinogenesis; Epithelial Cell Adhesion Molecule; Gene Expression Profiling; Endocrine Cells; Cell Line; Carcinoma, Ovarian Epithelial; MAP Kinase Signaling System; Demography; Inheritance Patterns; Leadership; Mitomycin; Technology; Vesicular Transport Proteins; Biomarkers, Tumor; ErbB Receptors; Homeostasis; Base Sequence; Signal Transduction; Acinar Cells; Cell Differentiation; Metronidazole; Liver Regeneration; Gene Knockout Techniques; Larva; Quantitative Trait Loci; Animals, Genetically Modified; Pancreatic Neoplasms; Diabetes Mellitus, Type 1; Exons; Genomics; Cohort Studies; Metaplasia; Sequence Analysis, RNA; Calibration; Prognosis; Cell Movement; Stem Cells; Regeneration; Financial Support; RNA, Messenger; Likelihood Functions; Extracellular Signal-Regulated MAP Kinases; Receptors, Estrogen; Medical History Taking; SOX9 Transcription Factor; Integrases; Insulin-Secreting Cells; Growth and Development; Regulatory Sequences, Nucleic Acid; Neoplasm Proteins; Smoking; Nitroreductases; Gastrointestinal Microbiome; Carcinogens; Linkage Disequilibrium; Genome-Wide Association Study; Transcriptome; Neoplasms; Water; Academic Performance; Language; Child; Pancreatitis; Prostatic Neoplasms; Butadienes; Developmental Biology; Alleles; Nitriles; Models, Genetic; Hepatocytes; Pancreas; Phenotype; Carcinoma, Pancreatic Ductal</t>
+          <t>Volunteers; Signal Transduction; Pancreas, Exocrine; Metaplasia; Financial Support; Zebrafish; Leadership; Diabetes Mellitus, Type 1; Homozygote; Bicarbonates; Antigen Presentation; Diabetes Mellitus, Type 2; Students; Diabetes Mellitus; Water; Larva; Hispanic or Latino; Insulin-Secreting Cells; Insulins; Academic Performance; Epithelium; Neoplasms; Endocrine Cells; Language; Growth and Development; Thinking; Feedback; Acinar Cells; Liver; Islets of Langerhans; Inflammation; Disease Progression; Optimism; Homeostasis; Gastrointestinal Microbiome; Cell Differentiation; Workforce; Child; Demography; Pancreas; Carcinogens; Transcriptome; Regeneration; Pancreatitis; Technology; Developmental Biology; Adenocarcinoma; Sequence Analysis, RNA; Animals, Laboratory; Genetic Phenomena; Stem Cells; Pancreatic Neoplasms</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1389,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Saliva; Students; Research; Macrophages; RANK Ligand; Chromatin; Brazil; West Nile virus; Research Personnel; Wound Healing; Gene Regulatory Networks; Wnt Signaling Pathway; Nevus; Inflammatory Bowel Diseases; Pandemics; Single-Cell Analysis; Lipid Metabolism; Elephants; DNA, Ancient; Hispanic or Latino; Fibrosis; NAD; Sirolimus; Single-Cell Gene Expression Analysis; Marsupialia; Senotherapeutics; Gelatin; YAP-Signaling Proteins; Aging; Gene Expression Regulation, Neoplastic; Melanocytes; Glycolysis; Biocompatible Materials; Keratinocytes; Nociceptors; Secretome; Yellow Fever; Gene Expression; Zika Virus Infection; Colorectal Neoplasms; Vaccines; Urodela; Evidence Gaps; Cell Line, Tumor; Evolution, Molecular; Senescence-Associated Secretory Phenotype; United States; Multiomics; Cartilage; Mosquito Vectors; Collagen; Epigenomics; TRPV Cation Channels; Zebrafish; Disease Progression; Mechanistic Target of Rapamycin Complex 2; Epidermis; Fossils; Dengue; Computational Biology; Locomotion; Software; Zika Virus; Organoids; Black or African American; Goals; Pandemic Preparedness; Lipid Droplets; Epithelial Cells; Computer Simulation; Pruritus; Aged; Vacuoles; RNA; Intestinal Mucosa; Epigenesis, Genetic; Mentors; Homeodomain Proteins; Hair; Adipocytes; Physical Examination; Gene Expression Profiling; Mammals; Reptiles; Skin Pigmentation; Phosphofructokinase-2; Biomechanical Phenomena; Cicatrix; Mesenchymal Stem Cells; Phylogeny; Obesity; Homeostasis; Signal Transduction; Pain; Hyaluronan Receptors; Ovosiston; R-Loop Structures; Necroptosis; Public Health; Myofibroblasts; Extracellular Matrix; Ambystoma mexicanum; World Health Organization; Internship and Residency; Culicidae; Proto-Oncogene Proteins c-akt; Pigmentation Disorders; Hair Follicle; Genome; DNA-Binding Proteins; Mammoths; Mentoring; Genomics; Universities; Casein Kinase 1 epsilon; Sequence Analysis, RNA; Cellular Senescence; Consensus; Schools; Stem Cells; Regeneration; Body Patterning; Cell Communication; Fibroblasts; X Chromosome; Mitochondria; Dermis; Skin Physiological Phenomena; Flavivirus; Birds; Skin Aging; TOR Serine-Threonine Kinases; Cross-Linking Reagents; Regulatory Sequences, Nucleic Acid; Skin; Lipogenesis; Keloid; RNA, Small Interfering; Vaccinology; Multifactorial Inheritance; Gene Expression Regulation, Developmental; Transcriptome; Neoplasms; Latin America; Preliminary Data; Embryonic Development; Hydrogels; Ethnicity; Osteopontin; Transcription Factors; Young Adult; China; Calcitonin Gene-Related Peptide; Adaptor Proteins, Signal Transducing; Cytokines; Amputation, Surgical; Phenotype; Inflammation</t>
+          <t>Young Adult; Extracellular Matrix; Preliminary Data; Cytokines; Wound Healing; West Nile virus; Ethnicity; Fibrosis; Fibroblasts; Flavivirus; Pandemics; Pruritus; Cell Communication; Public Health; Zika Virus Infection; Gene Expression; Universities; TOR Serine-Threonine Kinases; Cellular Senescence; Latin America; Black or African American; Hair Follicle; Schools; Senescence-Associated Secretory Phenotype; Keloid; Melanocytes; RNA; Ovosiston; Vaccines; China; Pain; Hispanic or Latino; Pigmentation Disorders; Skin; Mesenchymal Stem Cells; Single-Cell Gene Expression Analysis; Inflammation; Gene Regulatory Networks; Dengue; Birds; Aging; Regeneration; Mentors; Epidermis; Stem Cells; RNA, Small Interfering; Signal Transduction; Yellow Fever; Aged; Computational Biology; Zika Virus; Hair; Phenotype; Nevus; Urodela; Internship and Residency; World Health Organization; Senotherapeutics; Epigenesis, Genetic; Culicidae; Pandemic Preparedness; Saliva; Reptiles; Sequence Analysis, RNA; Evidence Gaps; Vaccinology; Mammals; Ambystoma mexicanum; Zebrafish; Secretome; Mosquito Vectors; Students; United States; Multifactorial Inheritance; Mentoring; Genomics; Homeostasis; Goals; Brazil; Computer Simulation; Amputation, Surgical; Gene Expression Profiling; Skin Pigmentation; Multiomics</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1401,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Research; Malaria; Molecular Sequence Data; Central America; Genes, Insect; Random Allocation; Aging; In Vitro Techniques; Mating Preference, Animal; Gene Expression; Arthropods; Heterozygote; Spermatozoa; Evolution, Molecular; United States; Reproduction; DNA Copy Number Variations; Diptera; Genetic Variation; Chromosome Mapping; Computational Biology; Insecticides; Species Specificity; Genes, Homeobox; Amino Acid Sequence; Genetics; RNA; Drosophila; Ecological and Environmental Phenomena; Hybridization, Genetic; Axonemal Dyneins; South America; Gene Expression Profiling; Gene Conversion; Semen; Translocation, Genetic; Gene Duplication; Tandem Repeat Sequences; In Situ Hybridization; Phylogeny; Biological Evolution; Sequence Analysis, DNA; Cell Differentiation; Genomic Structural Variation; Larva; Reproductive Isolation; Sex Characteristics; Eukaryota; Genome; Molecular Sequence Annotation; Spiroplasma; Spain; Butterflies; Caribbean Region; Genomics; Universities; Lepidoptera; Anopheles; Tsetse Flies; Drosophila melanogaster; Dosage Compensation, Genetic; RNA, Long Noncoding; Seminal Plasma Proteins; X Chromosome; Likelihood Functions; Drosophila Proteins; Testis; Gene Expression Regulation; Insecticide Resistance; Biomass; INDEL Mutation; Selection, Genetic; Multigene Family; Transcriptome; Sequence Analysis; Insecta; Adaptation, Physiological; Spermatogenesis; Models, Genetic; Chromosomes; Genetic Fitness; Genetic Speciation</t>
+          <t>Sequence Analysis; Semen; Sex Characteristics; Research; United States; Ecological and Environmental Phenomena; Multigene Family; Evolution, Molecular; Gene Expression; Spain; Genomics; Universities; Biological Evolution; RNA, Long Noncoding; Chromosomes; Phylogeny; Drosophila; Spermatozoa; Gene Expression Profiling; Transcriptome; Insecta; Genetics; Biomass; Genetic Speciation</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1413,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Mevalonic Acid; Neural Stem Cells; Protein Serine-Threonine Kinases; Ovarian Neoplasms; Hydroxymethylglutaryl-CoA Reductase Inhibitors; WW Domains; Single-Cell Analysis; Lipid Metabolism; Bioprinting; Tissue Scaffolds; Tyrosine; Hydrogel, Polyethylene Glycol Dimethacrylate; YAP-Signaling Proteins; Gene Expression Regulation, Neoplastic; rho GTP-Binding Proteins; Myeloid Cell Leukemia Sequence 1 Protein; Machine Learning; Lipids; Tissue Engineering; Protein Multimerization; Xenograft Model Antitumor Assays; Dimerization; Neoplastic Processes; Protein Kinase Inhibitors; Hippo Signaling Pathway; Cyclin-Dependent Kinase 9; RNA Polymerase II; Phosphoproteins; Cell Line, Tumor; Cell Adhesion; Mice, Nude; Down-Regulation; Protein Kinase C-delta; Integrins; Drug Discovery; Immune Checkpoint Inhibitors; Genetic Therapy; Blood Vessels; Cell Plasticity; Polymerization; Antineoplastic Agents; Triple Negative Breast Neoplasms; Mutagens; Goals; Lipid Droplets; Motivation; Oxidation-Reduction; Peptides; Molecular Targeted Therapy; Aged; Neovascularization, Physiologic; Laminin; Epigenesis, Genetic; Indolizines; Breast Neoplasms; Optical Imaging; Cyclic N-Oxides; Apoptosis; Neoplastic Stem Cells; Cell Line; Neoplasm Invasiveness; Oxygen Consumption; Pyridinium Compounds; Fibrin; Nanoparticles; Cells, Cultured; Vesicular Transport Proteins; Biomarkers, Tumor; ErbB Receptors; Fatty Acids; Signal Transduction; Heterografts; Hyaluronic Acid; Hepatocyte Nuclear Factor 3-alpha; Von Hippel-Lindau Tumor Suppressor Protein; Cell Differentiation; Antigens, CD; Lymphocytes, Tumor-Infiltrating; dinaciclib; Coenzyme A Ligases; Vimentin; Phosphorylation; Extracellular Matrix; Salmon; Genes, Suppressor; Hypoxia; Cell Adhesion Molecules; Protein Binding; Tumor Suppressor Protein p53; Histone Demethylases; Promoter Regions, Genetic; Oxidative Phosphorylation; Metabolism; MCF-7 Cells; Endothelial Cells; Cattle; Adenosine Triphosphate; Transcription, Genetic; Prognosis; src-Family Kinases; Cell Movement; Follow-Up Studies; Carcinoma, Renal Cell; Cyclin-Dependent Kinases; Electron Transport; Transcriptional Activation; Mice, Inbred BALB C; Neoplasm Metastasis; RNA, Long Noncoding; Basic Helix-Loop-Helix Transcription Factors; Biomarkers; Cyclin-Dependent Kinase Inhibitor Proteins; Antigens, Neoplasm; Mitochondria; Immunogenic Cell Death; Binding Sites; Jumonji Domain-Containing Histone Demethylases; Neoplasm Proteins; Histone-Lysine N-Methyltransferase; Up-Regulation; Synthetic Lethal Mutations; Kidney Neoplasms; Survival Rate; Lab-On-A-Chip Devices; Neoplasms; Preliminary Data; Neoplasm Transplantation; Tumor Cells, Cultured; von Hippel-Lindau Disease; Transcription Factors; HEK293 Cells; DNA Damage; Adaptor Proteins, Signal Transducing; rho-Associated Kinases</t>
+          <t>Cyclin-Dependent Kinases; Follow-Up Studies; Cyclin-Dependent Kinase 9; Immunogenic Cell Death; Signal Transduction; Peptides; Myeloid Cell Leukemia Sequence 1 Protein; dinaciclib; Lipid Droplets; von Hippel-Lindau Disease; Heterografts; Preliminary Data; Dimerization; Synthetic Lethal Mutations; Survival Rate; Breast Neoplasms; Tyrosine; Biomarkers; Binding Sites; Up-Regulation; Lipids; Neoplasm Metastasis; Neoplasms; Metabolism; Kidney Neoplasms; Oxidative Phosphorylation; Triple Negative Breast Neoplasms; Genes, Suppressor; Lipid Metabolism; Down-Regulation; Cell Movement; Hypoxia; Adenosine Triphosphate; Motivation; Integrins; Goals; Apoptosis; ErbB Receptors; RNA Polymerase II; Electron Transport; Neoplastic Processes; Immune Checkpoint Inhibitors; Mitochondria; Fatty Acids; Basic Helix-Loop-Helix Transcription Factors; src-Family Kinases; Phosphoproteins; Carcinoma, Renal Cell</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1425,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Biodiversity; Climate Change; Plant Development; Ecosystem; Biological Evolution; Drug Resistance, Microbial; Communicable Diseases; Soil; Denitrification; Gases; Bioprinting; Nitrogen; Ammonia; Nitrogen Cycle; Printing, Three-Dimensional; Arabidopsis; Plants; Metabolism; Droughts; Seasons; Water; Ecological and Environmental Phenomena; Symbiosis; Synthetic Biology; Microbiota; Evolution, Molecular</t>
+          <t>Arabidopsis; Microbiota; Nitrogen; Printing, Three-Dimensional; Water; Ecological and Environmental Phenomena; Synthetic Biology; Gases; Ammonia; Drug Resistance, Microbial; Evolution, Molecular; Nitrogen Cycle; Metabolism; Soil; Ecosystem; Biological Evolution; Droughts; Plants; Bioprinting; Communicable Diseases; Denitrification</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1437,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Protons; Density Functional Theory; Escherichia coli; Molybdenum; Phylogeny; Electrons; Tellurium; X-Ray Absorption Spectroscopy; Protein Conformation; Formate Dehydrogenases; Hydrogenase; Recombinant Proteins; Carbon Dioxide; Biosynthetic Pathways; Circular Dichroism; Oxidoreductases; Models, Chemical; Oxidation-Reduction; Coenzymes; Nitrogen; Ammonia; Molybdoferredoxin; Carbon Monoxide; S-Adenosylmethionine; Crystallography, X-Ray; Aldehyde Oxidoreductases; Organic Chemicals; Hydrocarbons; Methanosarcina; Protein Binding; Selenious Acid; Azotobacter vinelandii; Nitrogen Fixation; Gene Expression; Methyltransferases; Chemistry, Bioinorganic; Adenosine Triphosphate; Archaeal Proteins; Bacterial Proteins; Metalloproteins; Nitrogenase; Models, Molecular; Electron Spin Resonance Spectroscopy; Molecular Structure; Biofuels; Reducing Agents; Iron-Sulfur Proteins; Sulfur; Biotechnology; Multienzyme Complexes</t>
+          <t>Carbon Dioxide; Nitrogenase; Protons; Reducing Agents; Electrons; Molybdenum; Biofuels; Organic Chemicals; Biosynthetic Pathways; Iron-Sulfur Proteins; Ammonia; Carbon Monoxide; Nitrogen; Chemistry, Bioinorganic; Sulfur; Metalloproteins; Nitrogen Fixation; Hydrocarbons</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1449,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Ficus; Escherichia coli; Xylose; Proteobacteria; Biodiversity; Students; Escherichia coli Proteins; Climate Change; Hot Temperature; Ecosystem; Whole Genome Sequencing; Terminator Regions, Genetic; Mutation; Acinetobacter; Biological Evolution; DNA-Directed RNA Polymerases; Chemotaxis; Drug Resistance, Microbial; Nutrients; Stress, Physiological; Coculture Techniques; Pseudomonas putida; Genotype; Species Specificity; Actinobacteria; Poaceae; Phenotype; Selection, Genetic; Gene Expression Regulation, Bacterial; One Health; Microbial Interactions; Internship and Residency; Computer Simulation; Acclimatization; Drug Resistance, Bacterial; Xylans; Biofilms; Rifampin; Flagella; Anti-Bacterial Agents; Anti-Infective Agents; Ecological and Environmental Phenomena; Adaptation, Physiological; Genetic Background; Genes, Bacterial; Epistasis, Genetic; Symbiosis; Anti-Infective Agents, Local; Microbial Consortia; Synthetic Biology; Plant Leaves; Microbiota; Evolution, Molecular; Fecal Microbiota Transplantation; Rho Factor; Bacteroidetes; Genetic Fitness; Bacteria</t>
+          <t>Ficus; Microbiota; Chemotaxis; Whole Genome Sequencing; Anti-Infective Agents; Students; Rifampin; Escherichia coli; Microbial Interactions; Mutation; Nutrients; Synthetic Biology; Fecal Microbiota Transplantation; Ecological and Environmental Phenomena; Drug Resistance, Microbial; Internship and Residency; Anti-Bacterial Agents; Drug Resistance, Bacterial; Evolution, Molecular; Bacteria; Biodiversity; Biological Evolution; Ecosystem; Anti-Infective Agents, Local; Selection, Genetic; Stress, Physiological; Computer Simulation; One Health; Symbiosis; Microbial Consortia; Climate Change; Acclimatization</t>
         </is>
       </c>
     </row>
@@ -1485,7 +1461,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Leadership; Students; Magnetic Resonance Imaging; Behavior Control; Rodentia; Neuroimaging; Neurobiology; Stress Disorders, Post-Traumatic; Wakefulness; Cognitive Neuroscience; Consciousness; Spatial Navigation; Cognitive Dysfunction; Latent Infection; Goals; Vacuum; Pilot Projects; Depression; Healthy Volunteers; Memory Consolidation; Cognition; Arousal; Machine Learning; Electroencephalography; Academia; Sleep; Probability; Brain; Learning; Electrophysiology; Memory, Episodic; Algorithms; Mood Disorders; Cues; Spatial Memory; Decision Making; Mental Health; Odorants; Memory</t>
+          <t>Sleep; Behavior Control; Arousal; Memory; Magnetic Resonance Imaging; Academia; Mood Disorders; Leadership; Depression; Students; Cues; Electrophysiology; Odorants; Healthy Volunteers; Neuroimaging; Algorithms; Electroencephalography; Decision Making; Mental Health; Memory Consolidation; Latent Infection; Pilot Projects; Spatial Navigation; Wakefulness; Goals; Cognitive Neuroscience; Neurobiology; Brain; Rodentia; Consciousness; Cognition; Machine Learning; Probability; Vacuum; Stress Disorders, Post-Traumatic</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1473,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Cell Proliferation; Vertebrates; Animal Fins; Chromosomal Proteins, Non-Histone; Peripheral Nervous System; Mathematical Computing; Wnt Signaling Pathway; Gonads; Germ Cells; Single-Cell Analysis; Eye Proteins; Lipid Metabolism; Biological Transport; Gene Dosage; Morphogenesis; RNA-Seq; Bone Morphogenetic Proteins; Hand-Foot Syndrome; Tretinoin; Cell Adhesion; Optics and Photonics; Cartilage; Neural Crest; Zebrafish; Mutation; Tooth; Cranial Nerves; Computational Biology; Stochastic Processes; Receptors, Retinoic Acid; Synchrotrons; Craniofacial Abnormalities; Species Specificity; Lipid Droplets; Cichlids; Fibroblast Growth Factors; Congenital Abnormalities; Amino Acid Sequence; Skeleton; Tendons; Vacuoles; Sex Determination Processes; Skull; Malawi; Branchial Region; Adipocytes; Cohesins; Parathyroid Hormone-Related Protein; Gene Expression Profiling; Structure-Activity Relationship; Cell Line; Intestines; Mammals; Receptors, Wnt; Cell Cycle Proteins; Pharynx; Biomechanical Phenomena; Refraction, Ocular; Bone and Bones; Obesity; Sequence Homology; Biological Evolution; Embryo, Nonmammalian; Signal Transduction; Calcium; Jaw; Ligaments; Cell Differentiation; Gene Knockout Techniques; Bone Development; Extracellular Matrix; Larva; Stress, Mechanical; Permeability; Quantitative Trait Loci; Animals, Genetically Modified; Refractometry; Clinical Relevance; Musculoskeletal System; Lakes; Chondrocytes; Van Maldergem Wetzburger Verloes syndrome; Cell Movement; Growth Substances; Stem Cells; Systems Biology; Regeneration; Cornea; Body Patterning; Receptor Tyrosine Kinase-like Orphan Receptors; Aquaporins; Cell Communication; Fibroblasts; Hedgehog Proteins; Rhombencephalon; Basic Helix-Loop-Helix Transcription Factors; Myocardium; X-Ray Microtomography; Embryonic Induction; Regulatory Sequences, Nucleic Acid; Embryology; Laboratories; Lipogenesis; Zebrafish Proteins; Heart; Gene Expression Regulation, Developmental; Lens, Crystalline; Cell Lineage; Cataract; Embryonic Development; Pyrophosphatases; Cell Polarity; Water; Osteogenesis; Transcription Factors; Mesoderm; Wnt Proteins; CRISPR-Associated Protein 9; Growth Plate; Phenotype</t>
+          <t>Craniofacial Abnormalities; Embryology; Systems Biology; Hand-Foot Syndrome; Zebrafish; Branchial Region; Phenotype; Transcription Factors; Cartilage; Laboratories; Larva; Cell Lineage; Growth Plate; Tendons; Skull; Quantitative Trait Loci; Embryonic Development; Van Maldergem Wetzburger Verloes syndrome; Congenital Abnormalities; Gene Expression Profiling; Embryonic Induction; Clinical Relevance; Cell Polarity; Cichlids; Skeleton</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1485,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Proteins; Cell Proliferation; Human Body; Chromatin; Fluorescent Dyes; Estrogens; Coloring Agents; Complement C1q; Single-Cell Analysis; Microtubule-Associated Proteins; Biophysics; Osteoblasts; Amyloid beta-Peptides; Single-Cell Gene Expression Analysis; TDP-43 Proteinopathies; Aging; RNA-Seq; Protein Interaction Mapping; Phosphoproteins; Bacterial Proteins; Mass Spectrometry; Cell Line, Tumor; Cilia; Multiomics; High-Throughput Nucleotide Sequencing; Cell Biology; Succinimides; Organelles; Microglia; Neurons; Synapses; Neurodegenerative Diseases; Protein Processing, Post-Translational; Triple Negative Breast Neoplasms; Goals; Epithelial Cells; Luminescent Proteins; Streptavidin; Axons; Ciliopathies; HeLa Cells; Complement Activation; Staining and Labeling; Bioengineering; Health Personnel; Microscopy, Fluorescence; Carcinogenesis; Cell Transformation, Neoplastic; Sex Factors; Gene Expression Profiling; Cell Line; Nuclear Lamina; Progranulins; Microtubules; Tight Junction Proteins; Retinal Pigment Epithelium; Culture Media, Conditioned; Signal Transduction; Alzheimer Disease; Cell Nucleus; Prefrontal Cortex; Thalamus; Plaque, Amyloid; Permeability; Astrocytes; Antibodies; DNA-Binding Proteins; Embryo, Mammalian; Mentoring; Tissues; Brain; Proteome; Sequence Analysis, RNA; Benchmarking; Proteomics; Biotechnology; Nucleic Acids; Biomarkers; Dendrites; Zonula Occludens-1 Protein; Nerve Degeneration; Gene Expression Regulation; Biotin; Genes, Reporter; Nuclear Pore; Centrioles; Early Diagnosis; Lamins; Protein Biosynthesis; Heterochromatin; Microscopy; Green Fluorescent Proteins; Actin Cytoskeleton; Transcriptome; Preliminary Data; Ribosomes; Hydrogels; Single Molecule Imaging; Complement C3b; Tight Junctions; HEK293 Cells; Mouse Embryonic Stem Cells; Receptors, Progesterone; Molecular Structure; Phenotype</t>
+          <t>Plaque, Amyloid; Microscopy; Heterochromatin; Molecular Structure; Dendrites; Cell Transformation, Neoplastic; Prefrontal Cortex; Preliminary Data; Protein Biosynthesis; Phenotype; Human Body; Receptors, Progesterone; Astrocytes; Mass Spectrometry; Protein Processing, Post-Translational; Early Diagnosis; Cell Biology; Bioengineering; Single-Cell Gene Expression Analysis; High-Throughput Nucleotide Sequencing; Biomarkers; Benchmarking; Biophysics; Tissues; Mentoring; Chromatin; Nucleic Acids; Synapses; Axons; Triple Negative Breast Neoplasms; Ribosomes; Proteome; Goals; Sex Factors; Single-Cell Analysis; Alzheimer Disease; Neurodegenerative Diseases; Organelles; Lamins; Aging; Brain; Carcinogenesis; Gene Expression Profiling; Nuclear Lamina; Transcriptome; Nerve Degeneration; Hydrogels; Cell Proliferation; Sequence Analysis, RNA; Biotechnology; Neurons; Amyloid beta-Peptides; Multiomics; Proteomics; Estrogens</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1497,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Mytilus; Population Dynamics; Biodiversity; Students; Population Density; Climate; Climate Change; Program Evaluation; Aquatic Organisms; Ecosystem; Anthropogenic Effects; Surveys and Questionnaires; Water Movements; Alaska; Temperature; Health; Carbon Dioxide; History, 21st Century; Species Specificity; Predatory Behavior; Internationality; Larva; Introduced Species; Nitrogen; Global Warming; Gastropoda; Seawater; Conservation of Natural Resources; Oxygen; Atlantic Ocean; Dose-Response Relationship, Drug; Thinking; Oceans and Seas; Social Sciences; Plants; Geography; Mentors; Heat-Shock Response; Mentoring; Ecological and Environmental Phenomena; Ecology; Maine; Writing; Data Analysis; Europe; Human Activities; Mytilus edulis; Food Supply; Hydrogen-Ion Concentration</t>
+          <t>Ecological and Environmental Phenomena; Oceans and Seas; Ecosystem; Climate Change; Introduced Species</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1509,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Protons; Atlases as Topic; Reference Standards; Mental Status and Dementia Tests; Magnetic Resonance Imaging; Reproducibility of Results; Quality Control; Biomarkers; Disease Progression; Reading; Neuroimaging; Temporal Lobe; Gray Matter; Aged, 80 and over; Entorhinal Cortex; Software; Cognitive Dysfunction; Alzheimer Disease; NFATC Transcription Factors; Amyloid beta-Peptides; Dentate Gyrus; Tacrolimus; Pattern Recognition, Physiological; Neuropsychological Tests; Repression, Psychology; Cognition; Aging; Positron-Emission Tomography; Aged; Oxygen; Pattern Recognition, Visual; Verbal Learning; Mental Recall; Image Processing, Computer-Assisted; Calcineurin Inhibitors; Cerebral Cortex; Magnetic Resonance Spectroscopy; Brain; tau Proteins; Learning; Calcineurin; Dogs; Behavior, Animal; Young Adult; Brain Mapping; Algorithms; Atrophy; Mammals; Memory; Hippocampus; Spatial Learning</t>
+          <t>Alzheimer Disease; Aging; Memory; Hippocampus; Neuroimaging; Pattern Recognition, Physiological; Repression, Psychology; Biomarkers</t>
         </is>
       </c>
     </row>
@@ -1545,7 +1521,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Vertebrates; Neocortex; Physiology, Comparative; Neurons; Problem Solving; Phylogeny; Biomedical Research; Biological Evolution; Fishes; Birds; Neural Pathways; Neurosciences; Species Specificity; Melopsittacus; Reptiles; Cerebral Cortex; Congresses as Topic; Sexual Behavior, Animal; Mammals; Hippocampus; Lissencephaly; Cell Adhesion Molecules, Neuronal</t>
+          <t>Physiology, Comparative; Biological Evolution</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1533,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Organelles; Cells, Cultured; Centers for Disease Control and Prevention, U.S.; Fallopian Tubes; Cell Culture Techniques; Carrier Proteins; Membrane Proteins; Asymptomatic Infections; Ovary; Centrosome; Cell Differentiation; Microtubule-Associated Proteins; Membranes; Centrioles; Goals; Epithelial Cells; Oocytes; Chlamydia trachomatis; Microbiology; Golgi Apparatus; Chlamydia; HeLa Cells; Microscopy; RNA; Vacuoles; Cell Biology; Staining and Labeling; Causality; Cell Cycle; Pregnancy, Ectopic; Epithelium; Ubiquitin-Protein Ligases; Chlamydia Infections; Infertility; Phosphoproteins; Microbiota; Pregnancy; Microscopy, Electron; United States; Cilia; Bacteria; Cell Cycle Proteins; Stem Cells</t>
+          <t>Pregnancy; Oocytes; Staining and Labeling; Microscopy; Centers for Disease Control and Prevention, U.S.; Ovary; Microbiota; Pregnancy, Ectopic; Fallopian Tubes; Asymptomatic Infections; Chlamydia Infections; RNA; United States; Cell Culture Techniques; Chlamydia trachomatis; Microbiology; Cell Biology; Membranes; Epithelium; Membrane Proteins; Bacteria; Chlamydia; Golgi Apparatus; Cilia; Goals; Causality; Cell Cycle; Organelles; Vacuoles; Centrosome; Infertility; Stem Cells</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1545,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>GABA-A Receptor Antagonists; Neuroprotective Agents; Quinoxalines; Cognitive Dysfunction; Excitatory Amino Acid Antagonists; Nicotine; Nicotinic Antagonists; Conditioning, Classical; Tyrosine; Receptors, Nicotinic; Allosteric Regulation; Tobacco Use Disorder; Cognition; Rats, Sprague-Dawley; In Vitro Techniques; CA1 Region, Hippocampal; N-Methylaspartate; Stereotyped Behavior; Neuronal Plasticity; Memory; Mortality, Premature; Nicotiana; Theta Rhythm; Action Potentials; Synapses; Xenopus laevis; Mutation; Quinolines; Locomotion; Tobacco Use; Valine; Receptors, Muscarinic; Epigenesis, Genetic; Caspase 3; alpha7 Nicotinic Acetylcholine Receptor; Behavior, Animal; Histones; Cigarette Smoking; Pregnancy; Bicuculline; Hippocampus; Adolescent; Recognition, Psychology; Long-Term Synaptic Depression; Patch-Clamp Techniques; Signal Transduction; Age Factors; Phosphorylation; Pyramidal Cells; Prefrontal Cortex; Learning Disabilities; Acetylation; Interneurons; Animals, Genetically Modified; Prenatal Exposure Delayed Effects; Anxiety; Brain; Maternal Exposure; Memory Disorders; Spatial Memory; Transcription, Genetic; Longevity; Fear; src-Family Kinases; Tobacco Smoking; Schizophrenia; Receptors, AMPA; Receptor, Muscarinic M1; Receptors, N-Methyl-D-Aspartate; Actins; Nicotinic Agonists; Receptors, Metabotropic Glutamate; Oocytes; Smoking; Neuregulin-1; Up-Regulation; Lactation; Depsipeptides; Gene Expression Regulation, Developmental; Cause of Death; Smoking Cessation; Long-Term Potentiation; Animals, Newborn; Excitatory Postsynaptic Potentials; Reward</t>
+          <t>Pregnancy; Adolescent; Signal Transduction; Nicotiana; Pyramidal Cells; Cognitive Dysfunction; Tobacco Smoking; Mutation; Cause of Death; Tobacco Use Disorder; Animals, Genetically Modified; Transcription, Genetic; Tyrosine; Up-Regulation; Tobacco Use; Mortality, Premature; Smoking Cessation; Epigenesis, Genetic; Phosphorylation; Nicotine; Acetylation; Reward; Schizophrenia; Brain; Neuregulin-1; Longevity; Histones; Cognition; Smoking; Hippocampus; Receptors, N-Methyl-D-Aspartate; src-Family Kinases</t>
         </is>
       </c>
     </row>
@@ -1581,7 +1557,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Spleen; Cell Proliferation; Drug Administration Schedule; Ovarian Neoplasms; DNA; Spermatocytes; Germ Cells; Splenomegaly; Biological Transport; Tumor Microenvironment; Marsupialia; Gene Expression Regulation, Neoplastic; Meiosis; Genome, Human; Lupus Erythematosus, Systemic; CCCTC-Binding Factor; RNA-Seq; Neoplastic Processes; Transgenes; Colonic Neoplasms; Algorithms; Gene Frequency; Cell Line, Tumor; Specific Pathogen-Free Organisms; Tretinoin; Evolution, Molecular; Interferon-alpha; Trans-Activators; RNA, Untranslated; Down-Regulation; Epigenomics; Chromosomes, Mammalian; Disease Progression; Mutation; Clustered Regularly Interspaced Short Palindromic Repeats; Cell Plasticity; Computational Biology; Software; Synaptonemal Complex; Organoids; Goals; Cell Survival; Sex Chromosomes; Real-Time Polymerase Chain Reaction; Terpenes; Genetics; RNA; Genomic Imprinting; Staining and Labeling; Epigenesis, Genetic; Bacterial Translocation; Contraindications, Drug; Homeodomain Proteins; Microscopy, Fluorescence; MicroRNAs; Embryonic Stem Cells; Precision Medicine; Lymphadenopathy; Carcinogenesis; Breast Neoplasms; Optical Imaging; Mice, Inbred MRL lpr; Gene Expression Profiling; Neoplastic Stem Cells; In Situ Hybridization, Fluorescence; Vitamin A; Glutamine; Mammals; Lymphocyte Depletion; Cell Cycle Proteins; Chromosomes, Human, X; Cells, Cultured; Biological Evolution; Nucleic Acid Conformation; Forkhead Transcription Factors; Dysbiosis; Y Chromosome; Sequence Analysis, DNA; Molecular Biology; Signal Transduction; Health; Stress, Physiological; Cell Differentiation; Immunosuppressive Agents; Lupus Nephritis; Life Style; Sex Characteristics; Toll-Like Receptor 5; DNA-Binding Proteins; Genome; Oxidative Phosphorylation; Eutheria; Brain; Genomics; Carcinoma, Hepatocellular; Prognosis; Drosophila melanogaster; Incidence; RNA, Guide, CRISPR-Cas Systems; Stem Cells; Mice, Inbred BALB C; Hemizygote; RNA, Long Noncoding; Fibroblasts; Biomarkers; X Chromosome; Infertility, Male; Gene Editing; Binding Sites; Drosophila Proteins; Gene Expression Regulation; Phenotype; Liver Neoplasms; Selection, Genetic; Glomerulonephritis; Multigene Family; Drug Synergism; Lactobacillus; RNA, Small Interfering; Metabolic Reprogramming; Gastrointestinal Microbiome; RNA Interference; Microscopy; Neoplasms; Kidney; Cell Lineage; Preliminary Data; Genital Neoplasms, Female; Embryonic Development; Genetic Linkage; Fetal Stem Cells; Genes, X-Linked; Alleles; Proteinuria; RNA, Ribosomal, 16S; Mouse Embryonic Stem Cells; Dendritic Cells; X Chromosome Inactivation; Models, Genetic; Blastocyst; Genetic Fitness; RNA-Binding Proteins</t>
+          <t>Sex Chromosomes; X Chromosome; Ovarian Neoplasms; Life Style; Mammals; Sex Characteristics; Preliminary Data; Computational Biology; X Chromosome Inactivation; RNA, Untranslated; RNA; Gene Editing; Mutation; Breast Neoplasms; Chromosomes, Human, X; Marsupialia; Epigenomics; Eutheria; Genital Neoplasms, Female; Biomarkers; Algorithms; Multigene Family; Metabolic Reprogramming; Prognosis; Incidence; Clustered Regularly Interspaced Short Palindromic Repeats; Glutamine; Evolution, Molecular; Y Chromosome; Health; Oxidative Phosphorylation; Cell Survival; Biological Evolution; RNA, Long Noncoding; Epigenesis, Genetic; Down-Regulation; Tumor Microenvironment; Liver Neoplasms; Embryonic Development; Goals; Carcinoma, Hepatocellular; Cell Differentiation; RNA, Guide, CRISPR-Cas Systems; Stress, Physiological; Molecular Biology; Trans-Activators; Colonic Neoplasms; Fetal Stem Cells; Brain; Carcinogenesis; Precision Medicine; Neoplastic Processes; Microscopy, Fluorescence; Gene Expression Profiling; Cell Proliferation; Genetics; Genes, X-Linked; Optical Imaging; Organoids; Stem Cells</t>
         </is>
       </c>
     </row>
@@ -1593,7 +1569,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Stroke; Cell Proliferation; Wound Healing; Gene Regulatory Networks; Aged, 80 and over; Single-Cell Analysis; Encephalitis, Japanese; Amyloid beta-Peptides; Autism Spectrum Disorder; Aging; Pseudogenes; Rats, Sprague-Dawley; Myelin Sheath; RNA-Seq; Demyelinating Diseases; Encephalitis Virus, Japanese; Tauopathies; Gene Expression; Apolipoproteins E; Oligodendrocyte Precursor Cells; Memory; Multiomics; Microglia; Epigenomics; RNA Splicing; Parkinsonian Disorders; Neurons; Disease Progression; Integrins; Recurrence; Genetic Variation; Mutation; Neurodegenerative Diseases; Substance-Related Disorders; Goals; Chromatin Immunoprecipitation Sequencing; Immunity, Innate; Cuprizone; Axons; Genetics; Aged; Myeloid Cells; RNA; Epigenesis, Genetic; Down Syndrome; tau Proteins; MicroRNAs; Neuroinflammatory Diseases; Habenula; Gene Expression Profiling; Cell Line; NF-KappaB Inhibitor alpha; Cellular Reprogramming; Ganglia, Spinal; White Matter; NF-kappa B; Receptors, Immunologic; Signal Transduction; Spinal Cord Injuries; Oligodendroglia; Alzheimer Disease; Occipital Lobe; Cell Nucleus; Sterol Regulatory Element Binding Protein 1; Plaque, Amyloid; Spinal Cord; RNA, Small Nuclear; Astrocytes; Cocaine; Brain; Genomics; Sequence Analysis, RNA; Spatial Memory; Multiple Sclerosis; Proteomics; Systems Biology; Cell Communication; Gene Expression Regulation; Sensory Receptor Cells; Neuroglia; Resilience, Psychological; Nervous System Malformations; Remyelination; Transcriptome; Central Nervous System; Membrane Glycoproteins; Nerve Regeneration; Transcription Factors; Parkinson Disease; Fatty Acids, Volatile; Inflammation</t>
+          <t>Spatial Memory; Plaque, Amyloid; Myelin Sheath; White Matter; Parkinson Disease; Occipital Lobe; Sterol Regulatory Element Binding Protein 1; RNA; Pseudogenes; Epigenomics; Nervous System Malformations; RNA-Seq; Neuroinflammatory Diseases; RNA, Small Nuclear; Oligodendroglia; Gene Expression; Inflammation; Genomics; Disease Progression; Chromatin Immunoprecipitation Sequencing; Multiple Sclerosis; Parkinsonian Disorders; Goals; Substance-Related Disorders; Single-Cell Analysis; Alzheimer Disease; Neurodegenerative Diseases; Brain; Demyelinating Diseases; Tauopathies; Gene Expression Profiling; Transcriptome; Genetics; Sequence Analysis, RNA; Neurons; Proteomics</t>
         </is>
       </c>
     </row>
@@ -1605,7 +1581,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Wildfires; Population Dynamics; Carbon; Biodiversity; Students; Additional Terms; Vertebrates; Diet; Climate Change; Biological Specimen Banks; Ecosystem; Anthropogenic Effects; Technology; Data Science; Salinity; Interdisciplinary Research; Workforce; Remote Sensing Technology; Environmental Monitoring; Environmental Indicators; Nutrients; Temperature; Carbon Dioxide; California; Biota; Smoke; Ponds; Remote Sensing; Biomass; Predatory Behavior; Fresh Water; Plankton; Forests; North America; Introduced Species; Nitrogen; Literacy; Resilience, Psychological; Zooplankton; Antelopes; Fires; Hydrobiology; Organic Chemicals; Water Quality; Freshwater Biology; Mentors; Research Design; Seasons; Food Chain; Hunting; Guidelines as Topic; Ecological and Environmental Phenomena; Ecology; Mobile Applications; Lakes; Time Factors; Phytoplankton; Microbiota; Capacity Building; Planets; Dissolved Organic Matter; Eutrophication; Europe; Feeding Behavior; Bacteria</t>
+          <t>Anthropogenic Effects; Remote Sensing Technology; Diet; Data Science; Interdisciplinary Research; Mobile Applications; Hydrobiology; Students; Biological Specimen Banks; Ecological and Environmental Phenomena; Remote Sensing; Additional Terms; Vertebrates; Introduced Species; Time Factors; Lakes; Resilience, Psychological; Biota; Food Chain; Literacy; Ecosystem; Biodiversity; Temperature; Capacity Building; Environmental Indicators; Zooplankton; Workforce; Research Design; Feeding Behavior; Ponds; Plankton; Mentors; Technology; Freshwater Biology; Ecology; Hunting; Planets; Climate Change</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1593,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Receptors, Complement; Microglia; RNA Splicing; Receptors, Immunologic; Neurons; Synapses; Metabolomics; Disease Progression; ATP-Binding Cassette Transporters; Genetic Variation; Mutation; Receptor, Anaphylatoxin C5a; Complement C1q; Phagocytosis; Neurodegenerative Diseases; Caregivers; Signal Transduction; Calcium; Amyloid; Allergy and Immunology; Biological Phenomena; Amyloid beta-Protein Precursor; Cognitive Dysfunction; Genotype; Alzheimer Disease; Neuroprotection; Immunologic Factors; Amyloid beta-Peptides; Complement C5a; Immunity, Innate; Complement System Proteins; Cuprizone; Immune System; Neuroglia; Plaque, Amyloid; Resilience, Psychological; Cognition; Gene Knock-In Techniques; Sex Characteristics; Gastrointestinal Microbiome; COVID-19; Astrocytes; Aged; Microscopy; Complement Activation; Central Nervous System; RNA-Seq; Demyelinating Diseases; Membrane Glycoproteins; Lysosomes; Brain; tau Proteins; Tauopathies; Communicable Disease Control; Gene Expression; Neuroinflammatory Diseases; Nervous System Diseases; Long-Term Potentiation; Memory Disorders; Therapeutics; hydrocinnamate-cyclo(ornithyl-prolyl-cyclohexylalanyl-tryptophyl-arginyl); Apolipoproteins E; Neuronal Plasticity; Microbiota; Hippocampus; Incidence; Inflammation</t>
+          <t>Plaque, Amyloid; Microscopy; Immune System; Memory Disorders; Immunologic Factors; Aged; hydrocinnamate-cyclo(ornithyl-prolyl-cyclohexylalanyl-tryptophyl-arginyl); Phagocytosis; Cognitive Dysfunction; Microglia; Astrocytes; Therapeutics; Allergy and Immunology; RNA-Seq; Neuroinflammatory Diseases; Incidence; Gene Expression; Synapses; Inflammation; Disease Progression; Receptor, Anaphylatoxin C5a; Amyloid; Complement System Proteins; Neuroprotection; Neurodegenerative Diseases; Alzheimer Disease; Brain; Complement C1q; Complement C5a; Complement Activation; Immunity, Innate; Cognition; Hippocampus; Neurons; Lysosomes</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1605,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Regeneration; Microtubules; Neurons; Cytoskeleton; Dendrites; Integrins; Actins; Mitochondria; Cell Death; Peripheral Nervous System; Neurodegenerative Diseases; Neuroprotective Agents; Signal Transduction; Calcium; Neurites; Software; Casein Kinase Idelta; Goals; Neuroprotection; Sensory Receptor Cells; Extracellular Matrix; Time-Lapse Imaging; Peptides; Huntington Disease; Neuroglia; Axons; Blood-Brain Barrier; Proteolysis; Potassium Channels, Inwardly Rectifying; Actin Cytoskeleton; Neurogenesis; Ankyrins; Mentors; Drosophila; Energy Metabolism; Endothelial Cells; Nerve Regeneration; Transgenes; Adenosine Triphosphate; Mitochondrial Dynamics; Gene Expression Profiling; polyglutamine; Alleles; Glutamine; Drosophila melanogaster; Spinocerebellar Ataxias</t>
+          <t>Alleles; Signal Transduction; Dendrites; Cytoskeleton; Microtubules; polyglutamine; Spinocerebellar Ataxias; Sensory Receptor Cells; Nerve Regeneration; Time-Lapse Imaging; Neuroprotective Agents; Energy Metabolism; Glutamine; Drosophila melanogaster; Actins; Axons; Peripheral Nervous System; Neuroprotection; Adenosine Triphosphate; Goals; Neurogenesis; Transgenes; Cell Death; Huntington Disease; Mitochondrial Dynamics; Drosophila; Gene Expression Profiling; Proteolysis; Mitochondria; Regeneration; Mentors; Actin Cytoskeleton; Neurons; Neurites</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1617,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Proteins; Deep Learning; Neural Stem Cells; Chromatin; Trinucleotide Repeats; Cognitive Dysfunction; Synapsins; Autophagy; Sumoylation; Cerebral Cortex; Corpus Striatum; Algorithms; Epigenomics; Neurons; Synapses; Disease Progression; Integrins; Terminology as Topic; Mutation; Induced Pluripotent Stem Cells; Clustered Regularly Interspaced Short Palindromic Repeats; Neurodegenerative Diseases; Genetic Association Studies; Proteostasis; Case-Control Studies; Goals; Chromatin Immunoprecipitation Sequencing; Intranuclear Inclusion Bodies; Peptides; Mitochondrial Proteins; HeLa Cells; Aged; RNA; Epigenesis, Genetic; Synucleins; Genetic Diseases, X-Linked; Gene Expression Profiling; Histones; Optogenetics; Ataxin-1; Cells, Cultured; DNA Breaks, Double-Stranded; Calcium Signaling; Ubiquitin; Signal Transduction; Cell Differentiation; Trinucleotide Repeat Expansion; Alzheimer Disease; Extracellular Matrix; Frontotemporal Dementia; Huntington Disease; Motor Neurons; Lewy Bodies; SUMO-1 Protein; Protein Binding; DNA-Binding Proteins; Promoter Regions, Genetic; Lysosomes; Exons; Brain; Endothelial Cells; Registries; Proteome; Transcription, Genetic; Proteomics; Receptors, Antigen, T-Cell; Stem Cells; Systems Biology; Fibroblasts; Huntingtin Protein; Mitochondria; Biomedical Research; Gene Editing; Amyotrophic Lateral Sclerosis; Pluripotent Stem Cells; Brain-Derived Neurotrophic Factor; Frontotemporal Lobar Degeneration; Gene Expression Regulation; Poly Adenosine Diphosphate Ribose; DNA Repair; Neuroglia; Blood-Brain Barrier; Microscopy; Artificial Intelligence; Transcriptome; Ubiquitin-Protein Ligases; Nervous System Diseases; Parkinson Disease; DNA Damage; Spinocerebellar Ataxias; Phenotype; RNA-Binding Proteins</t>
+          <t>Microscopy; Deep Learning; Peptides; Induced Pluripotent Stem Cells; Systems Biology; HeLa Cells; Parkinson Disease; Synucleins; Cognitive Dysfunction; Registries; Genetic Diseases, X-Linked; DNA-Binding Proteins; RNA; Neurons; Gene Editing; Ubiquitin-Protein Ligases; Mutation; Amyotrophic Lateral Sclerosis; Exons; Clustered Regularly Interspaced Short Palindromic Repeats; Lewy Bodies; DNA Breaks, Double-Stranded; Goals; DNA Repair; DNA Damage; SUMO-1 Protein; Alzheimer Disease; Neurodegenerative Diseases; Frontotemporal Lobar Degeneration; Huntington Disease; Brain; Sumoylation; Frontotemporal Dementia; Gene Expression Profiling; Transcriptome; Mitochondria; Optogenetics; Proteostasis; Intranuclear Inclusion Bodies; Receptors, Antigen, T-Cell; Proteomics; Stem Cells</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1629,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Tandem Repeat Sequences; Genome, Insect; Quantitative Trait, Heritable; X Chromosome; Phylogeny; Mutation; Genetic Variation; Biological Evolution; Likelihood Functions; Pedigree; Genetic Predisposition to Disease; Computational Biology; Web Browser; Uncertainty; Software; Genetics, Population; Genotype; Selection, Genetic; Haplotypes; Polymorphism, Genetic; Computer Simulation; Acclimatization; Gene Dosage; Genetic Loci; Multifactorial Inheritance; Genome, Human; Quantitative Trait Loci; Normal Distribution; Genome-Wide Association Study; Genome; Recombination, Genetic; Exons; Drosophila; Ecological and Environmental Phenomena; Adaptation, Physiological; Zea mays; Genomics; Drosophila simulans; Algorithms; United Kingdom; Epistasis, Genetic; Heterozygote; Time Factors; 5' Untranslated Regions; Alleles; Genetic Markers; Gene Frequency; Evolution, Molecular; Gene Duplication; 3' Untranslated Regions; Environment; Models, Genetic; Polymorphism, Single Nucleotide; Domestication; Phenotype; Demography</t>
+          <t>Computer Simulation; Ecological and Environmental Phenomena; Genetics, Population; Algorithms; Phylogeny</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1641,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Spleen; Cell Proliferation; Forkhead Box Protein O3; Diet; Research; Macrophages; Ubiquitination; Chromatin; P-selectin ligand protein; Coloring Agents; Genetic Predisposition to Disease; Membrane Proteins; Tumor Microenvironment; Cognitive Dysfunction; Lymphocytic choriomeningitis virus; Programmed Cell Death 1 Receptor; Morbidity; Lymphocytic Choriomeningitis; Risk Factors; Antigens; Immunosuppression Therapy; Immune System; Aging; Flow Cytometry; Cognition; Influenza A Virus, H1N1 Subtype; Delivery of Health Care; SARS-CoV-2; Seven in Absentia Proteins; Vaccines; Memory T Cells; Cell Line, Tumor; Financing, Organized; P-Selectin; Immunologic Techniques; Ubiquitin-Protein Ligase Complexes; Mutation; CD8-Positive T-Lymphocytes; Immune Checkpoint Inhibitors; Dengue; Allergy and Immunology; Chemokine CCL17; Autoimmunity; Prion Proteins; Cell Survival; Immunologic Memory; Goals; Ligands; Molecular Targeted Therapy; HIV Infections; T-Lymphocytes; Myeloid Cells; Aged; Epigenesis, Genetic; Tumor Escape; Antiviral Agents; Adaptive Immunity; Metabolic Networks and Pathways; AMP-Activated Protein Kinases; Immune Checkpoint Proteins; Gene Expression Profiling; Neoadjuvant Therapy; Skin Neoplasms; CD4-Positive T-Lymphocytes; Intestines; Hepatitis B; Immunologic Surveillance; Neoplasms, Second Primary; Nuclear Proteins; Arm; Persistent Infection; Feasibility Studies; protein phosphatase 6; Influenza A Virus, H7N9 Subtype; Disease-Free Survival; Calcium Signaling; Ubiquitin; Virus Diseases; Biomarkers, Tumor; Homeostasis; Molecular Biology; Signal Transduction; Unfolded Protein Response; Cell Differentiation; T-Cell Exhaustion; Lymphocytes, Tumor-Infiltrating; Alzheimer Disease; T-Lymphocytes, Regulatory; Hepatitis A Virus Cellular Receptor 2; HMGB2 Protein; Brain; Adoptive Transfer; Immune Tolerance; Sequence Analysis, RNA; ADP-ribosyl Cyclase; Treatment Outcome; B7-H1 Antigen; Microbiota; Longevity; Immunity; Cell Movement; Receptors, Antigen, T-Cell; Incidence; Hemorrhagic Fever, Ebola; Lymph Nodes; Ficus; Melanoma; Hepatitis C; Amyotrophic Lateral Sclerosis; Caregivers; Intravital Microscopy; Military Personnel; Antimicrobial Cationic Peptides; Immunomodulation; Antibodies, Blocking; Immunotherapy; Gastrointestinal Microbiome; PrPC Proteins; Up-Regulation; Microscopy; Natural Killer T-Cells; Neoplasms; Chemokine CCL22; Preliminary Data; Survival Rate; Membrane Glycoproteins; Immunoglobulin G; Ubiquitin-Protein Ligases; Lymphocyte Activation; Transcription Factors; Dendritic Cells; Phosphoprotein Phosphatases; Phenotype; Bacteria</t>
+          <t>Ficus; Influenza A Virus, H1N1 Subtype; Ligands; Preliminary Data; Immunotherapy; Coloring Agents; Dendritic Cells; Melanoma; CD8-Positive T-Lymphocytes; Lymphocytic choriomeningitis virus; Amyotrophic Lateral Sclerosis; Neoplasms; Incidence; Financing, Organized; Cell Movement; Immunosuppression Therapy; Antiviral Agents; Memory T Cells; Longevity; Cognition; Receptors, Antigen, T-Cell; Neoadjuvant Therapy; Flow Cytometry; Autoimmunity; Immune System; Cognitive Dysfunction; Persistent Infection; Immunologic Techniques; Vaccines; Feasibility Studies; Delivery of Health Care; Up-Regulation; Genetic Predisposition to Disease; Immunoglobulin G; Macrophages; Chromatin; Dengue; Tumor Microenvironment; Alzheimer Disease; Molecular Biology; Aging; Calcium Signaling; Immune Checkpoint Inhibitors; Antigens; Immunity; Neoplasms, Second Primary; Signal Transduction; Lymph Nodes; Aged; Antibodies, Blocking; Phosphoprotein Phosphatases; HIV Infections; Immune Checkpoint Proteins; Research; P-Selectin; Transcription Factors; Hepatitis B; Myeloid Cells; Natural Killer T-Cells; ADP-ribosyl Cyclase; Disease-Free Survival; Adaptive Immunity; Epigenesis, Genetic; Hemorrhagic Fever, Ebola; Risk Factors; Programmed Cell Death 1 Receptor; B7-H1 Antigen; Arm; Spleen; Sequence Analysis, RNA; T-Lymphocytes; Metabolic Networks and Pathways; Treatment Outcome; Caregivers; Microscopy; CD4-Positive T-Lymphocytes; Virus Diseases; AMP-Activated Protein Kinases; Survival Rate; Skin Neoplasms; Military Personnel; Influenza A Virus, H7N9 Subtype; Mutation; Allergy and Immunology; protein phosphatase 6; Hepatitis C; Intravital Microscopy; Homeostasis; T-Cell Exhaustion; Goals; Cell Differentiation; P-selectin ligand protein; SARS-CoV-2; Brain; HMGB2 Protein; Gene Expression Profiling; Lymphocyte Activation; Morbidity</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1653,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Genes, Fungal; Students; Computers; Climate Change; Alternaria; West Nile virus; Songbirds; Metagenomics; Thermotolerance; West Nile Fever; Uncertainty; Temperature; Crop Production; California; Genotype; Forests; Neurospora; Climate Models; Research Design; Droughts; Arthropods; United States; Canada; Hydrogen-Ion Concentration; Metagenome; Mycorrhizae; Seeds; Survivorship; Soil Microbiology; Databases, Factual; Neon; Poaceae; Goals; Altitude; Grassland; Acclimatization; Cold Temperature; Extracellular Polymeric Substance Matrix; Ecological and Environmental Phenomena; Dermabrasion; Ants; Gene Expression Profiling; Carbon Cycle; Fungi; Nanoparticles; Actinomycetales; Carbon; Wildfires; Reproducibility of Results; Hot Temperature; Ecosystem; Carbon Dioxide; Nitrogen; Hyphae; Molecular Sequence Annotation; Ecology; Hawaii; Lepidoptera; Plant Leaves; Microbiota; Longevity; Incidence; Seedlings; Plant Development; Atmosphere; Life History Traits; Soil; Quantum Dots; Biomass; Carbon Sequestration; Resilience, Psychological; Information Dissemination; Plants; Water; Adaptation, Physiological; Farmers; Bacteria</t>
+          <t>Hawaii; Actinomycetales; Hot Temperature; Microbiota; Plant Development; Farmers; Students; Forests; Seeds; Soil Microbiology; United States; Survivorship; Thermotolerance; Computers; Water; Ecological and Environmental Phenomena; Dermabrasion; Carbon; Extracellular Polymeric Substance Matrix; Crop Production; Neon; Carbon Dioxide; Poaceae; Mycorrhizae; Resilience, Psychological; Soil; Bacteria; Wildfires; Genotype; Ecosystem; Temperature; Climate Models; Goals; Droughts; Research Design; Plants; Longevity; Gene Expression Profiling; Ecology; Alternaria; Seedlings; Fungi; Information Dissemination; Climate Change; Grassland</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1665,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Molecular Dynamics Simulation; Escherichia coli; Escherichia coli Proteins; Stigmatella aurantiaca; Polyketide Synthases; Thiosugars; Binding Sites; Drug Design; Catalytic Domain; Protein Conformation; Acyl Carrier Protein; Acylation; Molecular Docking Simulation; Acetyl Coenzyme A; Protein Structure, Tertiary; Recombinant Proteins; Biosynthetic Pathways; Fatty Acid Synthases; Cross-Linking Reagents; Antineoplastic Agents; Biomimetics; Goals; Hydrocarbons, Brominated; Oxidoreductases; Ligands; Acyl-CoA Dehydrogenases; Substrate Specificity; Protein Domains; Oxidation-Reduction; NADP; Molecular Mimicry; Biocatalysis; Amino Acid Sequence; Computer Simulation; Streptomyces; Alcohol Oxidoreductases; Mutagenesis, Site-Directed; Pantetheine; Polyketides; Hydro-Lyases; Ochromonas; 3-Oxoacyl-(Acyl-Carrier-Protein) Synthase; Alcohols; COVID-19; Crystallography, X-Ray; Lipids; Polyenes; Machine Learning; Peptide Synthases; Protein Multimerization; Protein Binding; Protein Engineering; Structural Homology, Protein; Molecular Probes; Biological Products; Malonyl Coenzyme A; Big Data; Polyphenols; Bacterial Proteins; Daunorubicin; Carbon-Carbon Ligases; Sequence Homology, Amino Acid; Ethers, Cyclic; Aromatase; Mutagenesis; Post-Acute COVID-19 Syndrome; Gene Library; Models, Molecular; Molecular Structure; Acyl Coenzyme A; Molecular Conformation; Crystallography; Fatty Acid Synthase, Type II; Bacteria; Protein Interaction Domains and Motifs</t>
+          <t>Polyketides; Big Data; Mutagenesis; Biological Products; Catalytic Domain; Antineoplastic Agents; Crystallography; Post-Acute COVID-19 Syndrome; Drug Design; Machine Learning; COVID-19; Goals; Polyketide Synthases; Daunorubicin</t>
         </is>
       </c>
     </row>
@@ -1701,7 +1677,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Embryoid Bodies; Epstein-Barr Virus Infections; Graft vs Host Disease; Neural Stem Cells; Macrophages; HL-60 Cells; Killer Cells, Natural; Wnt Signaling Pathway; Toxoplasmosis; Epitopes; Single-Cell Analysis; Coculture Techniques; Lentivirus; Oxidoreductases; Sirolimus; Single-Cell Gene Expression Analysis; Immunosuppression Therapy; Monocytes; Mechanistic Target of Rapamycin Complex 1; Hepatitis, Viral, Animal; Organ Specificity; Myelin Sheath; Demyelinating Diseases; Gene Expression; Algorithms; Vaccines; Interferon-gamma; Cell Adhesion; Multiomics; Encephalomyelitis, Autoimmune, Experimental; Microglia; Stem Cell Transplantation; Autoimmune Diseases; Neurons; CD8-Positive T-Lymphocytes; Induced Pluripotent Stem Cells; Neurodegenerative Diseases; Esophageal Neoplasms; Allergy and Immunology; Autoimmunity; Goals; Fluticasone; Immunity, Innate; Substrate Specificity; Transfection; Axons; Herpesvirus 4, Human; Histocompatibility Antigens Class II; T-Lymphocytes; Myeloid Cells; Tumor Escape; Vaccination; Breast Neoplasms; Lewis X Antigen; Neuroinflammatory Diseases; Antibody Formation; CD4-Positive T-Lymphocytes; RNA, Neoplasm; Th17 Cells; Persistent Infection; Transforming Growth Factor beta; White Matter; Cells, Cultured; Image Cytometry; Myeloid-Derived Suppressor Cells; Murine hepatitis virus; Mesenchymal Stem Cells; Biomarkers, Tumor; Mice, Congenic; Immunization; Forkhead Transcription Factors; Coronavirus Infections; Signal Transduction; Genetic Vectors; Exosomes; Cell Differentiation; Hematopoietic Stem Cell Transplantation; Transplantation, Homologous; Immunosuppressive Agents; Oligodendroglia; Alzheimer Disease; T-Lymphocytes, Regulatory; Spinal Cord; Astrocytes; Receptors, CCR2; Signaling Lymphocytic Activation Molecule Family; Meningitis, Aseptic; Bone Marrow Transplantation; Brain; CD4 Antigens; Endothelial Cells; Immune Tolerance; Transcytosis; Multiprotein Complexes; Cell Movement; Multiple Sclerosis; Antibodies, Monoclonal, Humanized; Receptors, Antigen, T-Cell; Follow-Up Studies; Interleukins; beta Catenin; Stem Cells; Lipopolysaccharides; Biomarkers; RNA, Messenger; Cell Death; Recombinant Fusion Proteins; N-Acetylneuraminic Acid; TOR Serine-Threonine Kinases; Carcinoembryonic Antigen; Caveolin 1; Vaccine Efficacy; Histocompatibility Antigens Class I; CX3C Chemokine Receptor 1; Laboratories; aducanumab; Ribosomal Protein S6 Kinases, 70-kDa; Blood-Brain Barrier; Diacylglycerol Kinase; Immunotherapy; Mice, Inbred Strains; Mesenchymal Stem Cell Transplantation; CD11a Antigen; Remyelination; Gene Expression Regulation, Developmental; Green Fluorescent Proteins; Transcriptome; Central Nervous System; Preliminary Data; Membrane Glycoproteins; Endothelium, Vascular; Lymphocyte Activation; Cell- and Tissue-Based Therapy; Immunity, Cellular; Animals, Newborn; Microscopy, Fluorescence, Multiphoton; Human Embryonic Stem Cells; Immunologic Factors; Inflammation; Interleukin-10</t>
+          <t>Antibody Formation; Follow-Up Studies; Autoimmunity; Herpesvirus 4, Human; White Matter; Neural Stem Cells; Preliminary Data; Epitopes; Immunotherapy; Persistent Infection; Immunity, Cellular; aducanumab; Microglia; Laboratories; Vaccines; Image Cytometry; Astrocytes; CD8-Positive T-Lymphocytes; Allergy and Immunology; Single-Cell Gene Expression Analysis; Vaccination; Esophageal Neoplasms; Tumor Escape; Macrophages; Inflammation; Antibodies, Monoclonal, Humanized; T-Lymphocytes, Regulatory; Meningitis, Aseptic; Immune Tolerance; Vaccine Efficacy; Multiple Sclerosis; Epstein-Barr Virus Infections; Goals; Remyelination; Cell Death; Alzheimer Disease; Killer Cells, Natural; Encephalomyelitis, Autoimmune, Experimental; Immunization; Immunity, Innate; Murine hepatitis virus; Multiomics; Receptors, Antigen, T-Cell; T-Lymphocytes; Stem Cells</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1689,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Proteins; Cell Proliferation; Students; Kinesins; Ubiquitination; Protein Serine-Threonine Kinases; Chromatin; Neurofibromatosis 2; Gene Regulatory Networks; Neurilemmoma; TEA Domain Transcription Factors; Serine-Threonine Kinase 3; Microtubule-Associated Proteins; Loss of Function Mutation; Autophagy-Related Protein 8 Family; Morbidity; Head and Neck Neoplasms; Phosphoric Monoester Hydrolases; Mutation, Missense; Lung Neoplasms; Neurofibromin 2; Gene Expression Regulation, Neoplastic; Autophagy; Mechanistic Target of Rapamycin Complex 1; Lipids; Hippo Signaling Pathway; Protein Interaction Mapping; Mass Spectrometry; Cell Line, Tumor; Organelles; Physiological Phenomena; Intercellular Signaling Peptides and Proteins; Glucose; Mutation; Interdisciplinary Research; Publishing; Goals; Cell Survival; Protein Interaction Maps; Immunity, Innate; Histone Deacetylase 2; Tumor Escape; Drosophila; Breast Neoplasms; Carcinogenesis; Metabolic Networks and Pathways; AMP-Activated Protein Kinases; Writing; Apoptosis; Cell Transformation, Neoplastic; Histones; Organ Size; Glycosylation; Mammals; MAP Kinase Signaling System; Ependymoma; Microtubules; Serine; Adolescent; Glycogen Synthase Kinase 3 beta; Florida; Homeostasis; Signal Transduction; Histone Deacetylases; Endoderm; Cell Differentiation; Receptor, Notch1; Sequence Deletion; Meningeal Neoplasms; Phosphorylation; Dyneins; Cholesterol; Genes, Neurofibromatosis 2; N-Myc Proto-Oncogene Protein; Histone Deacetylase 1; Acetylation; Fertilization; Tumor Suppressor Proteins; Brain; Carcinoma, Hepatocellular; B7-H1 Antigen; Proteomics; Genetic Background; Stem Cells; Dynactin Complex; Regeneration; Body Patterning; RNA, Long Noncoding; Drosophila Proteins; Drug Resistance, Neoplasm; Intracellular Signaling Peptides and Proteins; Genes, Regulator; Liver Neoplasms; Pyridines; Immunotherapy; Non-alcoholic Fatty Liver Disease; Meningioma; Calmodulin-Binding Proteins; Gene Expression Regulation, Developmental; Neoplasms; Embryonic Development; Ubiquitin-Protein Ligases; Transcription Factors; Child; Cues; Adaptor Proteins, Signal Transducing; Blastocyst; Inflammation</t>
+          <t>Metabolic Networks and Pathways; Fertilization; Adolescent; Signal Transduction; Hippo Signaling Pathway; Adaptor Proteins, Signal Transducing; Florida; Mammals; Interdisciplinary Research; Cell Transformation, Neoplastic; Glucose; Body Patterning; Students; AMP-Activated Protein Kinases; Transcription Factors; Drug Resistance, Neoplasm; Mutation; MAP Kinase Signaling System; Meningeal Neoplasms; Cues; TEA Domain Transcription Factors; Lipids; Neoplasms; Meningioma; Protein Serine-Threonine Kinases; Intercellular Signaling Peptides and Proteins; Writing; Cell Survival; Physiological Phenomena; Homeostasis; Goals; Neurofibromatosis 2; Publishing; Organ Size; Apoptosis; Child; Neurilemmoma; Protein Interaction Maps; Brain; Genetic Background; Carcinogenesis; Drosophila; Regeneration; Ependymoma; Cell Proliferation; Sequence Deletion; Morbidity; Genes, Neurofibromatosis 2; Stem Cells</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1701,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Body Patterning; Protein Serine-Threonine Kinases; Drosophila Proteins; Homeostasis; Drosophila melanogaster; Gene Expression Regulation; Stress, Physiological; Inactivation, Metabolic; Mosaicism; Phosphorylation; N-Acetylglucosaminyltransferases; Genetics; Protein Biosynthesis; HeLa Cells; Synthetic Lethal Mutations; Gene Expression Regulation, Developmental; DNA-Binding Proteins; Tumor Suppressor Proteins; Hippo Signaling Pathway; Drosophila; Transcription Factors; Transgenes; Transcription, Genetic; HEK293 Cells; Developmental Biology; Alleles; Transcription Factor MTF-1; Cell Line, Tumor; Zinc; Proteoglycans; Cadmium; Phenotype; Infertility, Female; Germ-Line Mutation</t>
+          <t>Drosophila; Genetics; Transcription, Genetic; Developmental Biology; Protein Biosynthesis; Proteoglycans</t>
         </is>
       </c>
     </row>
@@ -1737,21 +1713,17 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Vancomycin; Receptors, Complement; Bacterial Infections; Students; Human Body; Pseudomonas aeruginosa; Adjuvants, Pharmaceutic; Macrophages; Colon; Diet; Diabetes Mellitus, Type 2; DNA; Respiratory System; Research Personnel; Metagenomics; Complement C1q; Nutrients; Pneumonia; Gram-Negative Bacteria; Inflammatory Bowel Diseases; Pandemics; Genotype; Enterococcus; Amyloid beta-Peptides; Tobacco Smoke Pollution; Surface-Active Agents; Bacteria, Anaerobic; Patient Discharge; Respiratory Mucosa; Aging; Gene Knock-In Techniques; Western World; Volunteers; Informed Consent; Volatile Organic Compounds; Wastewater; Research Design; Anti-Infective Agents; Microbial Sensitivity Tests; Fellowships and Scholarships; Colonic Neoplasms; Bacteremia; Mass Spectrometry; Longitudinal Studies; Host Microbial Interactions; United States; Planets; Bacteria; High-Throughput Nucleotide Sequencing; Hydrogen-Ion Concentration; Biodiversity; Diet Therapy; Metagenome; Autoimmune Diseases; Metabolomics; Probiotics; Mutation; Antioxidants; Immunosenescence; Interdisciplinary Research; Sewage; Neurodegenerative Diseases; Feedback; Computational Biology; Virome; Digestion; Ecuador; Cross Infection; Case-Control Studies; Compassionate Use Trials; Goals; Autistic Disorder; Pilot Projects; Random Forest; Microbiology; Healthy Volunteers; Cryopreservation; Respiration; Bronchoalveolar Lavage Fluid; COVID-19; Aged; RNA; Lung; Antineoplastic Agents, Hormonal; Mentors; Prevalence; Hunting; Bacterial Physiological Phenomena; Microscopy, Fluorescence; Breast Neoplasms; Epithelium; Colonoscopy; Chromatography, Gas; Neuroinflammatory Diseases; Gene Expression Profiling; Staphylococcus aureus; Translational Science, Biomedical; Demography; Recommended Dietary Allowances; Enterococcus faecalis; Pseudomonas; Feasibility Studies; Leadership; Reproducibility of Results; Stomach; Ecosystem; Hospitalization; Obesity; Biological Evolution; Retrospective Studies; Dysbiosis; Communicable Diseases; Drug Resistance, Microbial; Sequence Analysis, DNA; Molecular Biology; Intestine, Small; Angiotensin-Converting Enzyme Inhibitors; Myeloproliferative Disorders; Viruses; Health; Fermentation; Alzheimer Disease; Genome Size; Public Health; Internship and Residency; Diet, Mediterranean; Sex Characteristics; Gas Chromatography-Mass Spectrometry; Metabolome; Hypersensitivity; Dementia; Diagnosis; Anti-Bacterial Agents; Molecular Sequence Annotation; Diabetes Mellitus, Type 1; Brain; Morocco; Ecology; Genomics; Respiration Disorders; Critical Illness; Cohort Studies; Sequence Analysis, RNA; Angiotensin Receptor Antagonists; Microbiota; Glycoside Hydrolases; Benchmarking; Immunity; Appendectomy; Global Health; Incidence; Inpatients; Escherichia coli; Staphylococcal Infections; Germ-Free Life; Sputum; Biomarkers; Immunocompromised Host; Gastroenterology; Melanoma; Caregivers; Individuality; Stenotrophomonas maltophilia; Phage Therapy; Streptococcus; Tamoxifen; Data Management; Host Specificity; Estonia; Vaccine Efficacy; Ethics Committees, Research; Appendicitis; Bacteriophages; Laboratories; Adjuvants, Immunologic; Drug Resistance, Bacterial; Resilience, Psychological; Brain-Gut Axis; Freezing; Immunotherapy; Methicillin-Resistant Staphylococcus aureus; Gastrointestinal Microbiome; Biofilms; Wastewater-Based Epidemiological Monitoring; Microscopy; Premature Birth; Clostridium Infections; Life Cycle Stages; Culture Media; Tetracycline; Neoplasms; Transcriptome; Staphylococcus; Preliminary Data; Endometriosis; Stenotrophomonas; Societies, Scientific; Dietary Fiber; Coliphages; Cystic Fibrosis; Young Adult; Child; Respiratory Tract Infections; RNA, Ribosomal, 16S; Dendritic Cells; Fecal Microbiota Transplantation; Outcome Assessment, Health Care; Fatty Acids, Volatile; Inflammation</t>
+          <t>Metabolomics; Vancomycin; Metabolome; Angiotensin Receptor Antagonists; Critical Illness; Diet Therapy; Pseudomonas aeruginosa; Chromatography, Gas; Preliminary Data; Clostridium Infections; Leadership; Staphylococcus aureus; Diabetes Mellitus, Type 1; Anti-Infective Agents; Pneumonia; Escherichia coli; Dendritic Cells; Inpatients; Phage Therapy; Pandemics; Respiratory Tract Infections; Fermentation; High-Throughput Nucleotide Sequencing; Benchmarking; Public Health; Neoplasms; Incidence; Adjuvants, Immunologic; Feedback; Informed Consent; Pseudomonas; Inflammatory Bowel Diseases; Stenotrophomonas maltophilia; Ecosystem; Angiotensin-Converting Enzyme Inhibitors; Health; Compassionate Use Trials; Respiratory Mucosa; Gas Chromatography-Mass Spectrometry; Bacteria, Anaerobic; Volatile Organic Compounds; Respiration Disorders; Staphylococcus; Premature Birth; Stenotrophomonas; Gram-Negative Bacteria; Biofilms; Appendectomy; Planets; Longitudinal Studies; Diet; Enterococcus faecalis; Volunteers; Interdisciplinary Research; DNA; Stomach; Adjuvants, Pharmaceutic; Human Body; Respiration; RNA; Reproducibility of Results; Drug Resistance, Microbial; Feasibility Studies; Morocco; Global Health; Hydrogen-Ion Concentration; Anti-Bacterial Agents; Research Personnel; Bacteria; Pilot Projects; Life Cycle Stages; Macrophages; Inflammation; Colon; Vaccine Efficacy; Translational Science, Biomedical; Gastrointestinal Microbiome; Hospitalization; Genome Size; Diagnosis; Alzheimer Disease; Molecular Biology; Child; Aging; Fellowships and Scholarships; Transcriptome; Mentors; Hunting; Virome; Immunity; Prevalence; Lung; Communicable Diseases; Bacteremia; Outcome Assessment, Health Care; Cystic Fibrosis; Autoimmune Diseases; Bacterial Physiological Phenomena; Aged; Computational Biology; Microbiota; Western World; COVID-19; Diabetes Mellitus, Type 2; Gastroenterology; Obesity; Laboratories; Mass Spectrometry; Host Specificity; Immunosenescence; Biomarkers; Internship and Residency; Individuality; Digestion; Autistic Disorder; Colonoscopy; Hypersensitivity; Wastewater; Wastewater-Based Epidemiological Monitoring; Demography; Sequence Analysis, RNA; Metagenome; Microscopy; Random Forest; Enterococcus; Fatty Acids, Volatile; Students; Methicillin-Resistant Staphylococcus aureus; Sewage; Bacteriophages; Glycoside Hydrolases; Patient Discharge; Mutation; Nutrients; Fecal Microbiota Transplantation; Microbiology; Healthy Volunteers; Epithelium; Cross Infection; Appendicitis; Resilience, Psychological; Data Management; Probiotics; Bacterial Infections; Genomics; Molecular Sequence Annotation; Goals; Research Design; Coliphages; Intestine, Small; Dietary Fiber; Colonic Neoplasms; Recommended Dietary Allowances; Ecuador; Gene Expression Profiling; Immunocompromised Host; Viruses; Staphylococcal Infections; Ethics Committees, Research</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Wiles, Travis</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Uropathogenic Escherichia coli; Students; Vibrio; Macrophages; Urinary Tract; Climate Change; Chemotaxis; Virulence; Predatory Behavior; Microbial Interactions; DNA Transposable Elements; Immune System; Gene Knock-In Techniques; Hyperglycemia; Gene Transfer, Horizontal; Bacterial Proteins; Host Microbial Interactions; Evolution, Molecular; Reactive Oxygen Species; Planets; High-Throughput Nucleotide Sequencing; Gastrointestinal Tract; Antibiosis; Food Supply; Inflammation; Stem Cell Transplantation; Diabetes Mellitus; SOXE Transcription Factors; Zebrafish; Anti-Inflammatory Agents; SOS Response, Genetics; Leukocyte Count; Disease Transmission, Infectious; Mutation; Antioxidants; Animals, Wild; Feedback; Vibrio cholerae; Locomotion; Colony Count, Microbial; Species Specificity; Goals; Motivation; Gastrointestinal Motility; Oxidation-Reduction; Peptides; Microbiology; Genetics; Bacterial Physiological Phenomena; Aeromonas veronii; Microscopy, Fluorescence; Type VI Secretion Systems; Neutrophils; Synthetic Biology; Intestines; Mammals; Population Dynamics; Feasibility Studies; Proteobacteria; Cell Count; Genome, Bacterial; Ecosystem; Phylogeny; Biological Evolution; Dysbiosis; Drug Resistance, Microbial; Sequence Analysis, DNA; Homeostasis; Models, Statistical; Genetic Engineering; Metronidazole; Public Health; Gene Knockout Techniques; Larva; Tumor Necrosis Factor-alpha; Host-Pathogen Interactions; Animals, Genetically Modified; Anti-Bacterial Agents; Genetic Techniques; Ecology; Symbiosis; Enteric Nervous System; Aeromonas; Virulence Factors; Microbiota; Mutagenesis; Systems Biology; Escherichia coli; Germ-Free Life; Soil; Gene Expression Regulation; Urinary Tract Infections; Spatio-Temporal Analysis; Bacteriophages; Nitroreductases; Zebrafish Proteins; Gastrointestinal Microbiome; Gene Flow; Plants; Imaging, Three-Dimensional; Plasmids; Disease Resistance; Microbial Consortia; Bacterial Adhesion; DNA Damage; Chromosomes; Phenotype; Bacteria</t>
-        </is>
-      </c>
+          <t xml:space="preserve">Wiles, TJ </t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1761,7 +1733,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Memory, Long-Term; Chromatin; DNA; Radiation Exposure; Gene Regulatory Networks; Drug-Seeking Behavior; Nicotine; Circadian Rhythm; Amyloid beta-Peptides; Autism Spectrum Disorder; Conditioning, Classical; Acetate-CoA Ligase; Memory Consolidation; Cognition; Aging; Polymerase Chain Reaction; Color Vision Defects; Demyelinating Diseases; Research Design; Gene Expression; Physical Conditioning, Animal; Neuronal Plasticity; Mass Spectrometry; Trans-Activators; Cholinergic Neurons; Memory; Intellectual Disability; Blotting, Western; High-Throughput Nucleotide Sequencing; Occupations; Microglia; RNA Splicing; Epigenomics; Nucleus Accumbens; Neurons; Synapses; Recurrence; Polyadenylation; Genetic Variation; Mutation; Synaptic Transmission; Entropy; Neurodegenerative Diseases; Chin; Substance-Related Disorders; Chromatin Immunoprecipitation; Neurosciences; Cuprizone; Mental Disorders; Genetics; Adverse Childhood Experiences; RNA, Catalytic; Epigenesis, Genetic; Wood; Neuroinflammatory Diseases; Habenula; Gene Expression Profiling; Histones; Mental Health; Radiotherapy Dosage; Hippocampus; Nucleosomes; Reproducibility of Results; Receptors, Immunologic; Calcium; N-nitrosoiminodiacetic acid; Acetyl Coenzyme A; Alzheimer Disease; Brain Neoplasms; Plaque, Amyloid; Acetylation; Interneurons; Antibodies; DNA-Binding Proteins; Cocaine; Anxiety; Promoter Regions, Genetic; Activin Receptors, Type I; Brain; Genomics; Universities; Sequence Analysis, RNA; Spatial Memory; Longevity; histone deacetylase 3; Fear; Histone Code; Proteomics; Radiotherapy; Cholinergic Agents; RNA, Messenger; X Chromosome; Radiation Dose Hypofractionation; Dopaminergic Neurons; Brain-Derived Neurotrophic Factor; Gene Expression Regulation; Medium Spiny Neurons; DNA Methylation; Jumonji Domain-Containing Histone Demethylases; Immunohistochemistry; Epigenetic Memory; Neuroglia; Resilience, Psychological; Neurogenesis; Transcriptome; Preliminary Data; Membrane Glycoproteins; Sleep; Life Change Events; Transcription Factors; Long-Term Potentiation; Child; Cues; Genes, X-Linked; Leucine Zippers; Pharmaceutical Preparations; Reward; Censuses; RNA-Binding Proteins</t>
+          <t>Occupations; X Chromosome; Memory; Cholinergic Agents; Preliminary Data; DNA; Antibodies; Dopaminergic Neurons; Wood; Anxiety; Acetyl Coenzyme A; Polymerase Chain Reaction; N-nitrosoiminodiacetic acid; Transcription Factors; Nucleus Accumbens; Cholinergic Neurons; Cocaine; Nucleosomes; Calcium; Chin; Mass Spectrometry; Cues; Epigenomics; Long-Term Potentiation; Autism Spectrum Disorder; Memory, Long-Term; High-Throughput Nucleotide Sequencing; histone deacetylase 3; Chromatin Immunoprecipitation; Memory Consolidation; Proteomics; Neurosciences; Gene Expression; Neuronal Plasticity; Chromatin; Drug-Seeking Behavior; Synapses; Genomics; Gene Regulatory Networks; Universities; Immunohistochemistry; Epigenesis, Genetic; Adverse Childhood Experiences; Recurrence; Epigenetic Memory; Histone Code; Habenula; Substance-Related Disorders; DNA Methylation; Intellectual Disability; Research Design; Alzheimer Disease; Life Change Events; Neurodegenerative Diseases; Nicotine; Acetylation; Reward; Trans-Activators; Brain; Leucine Zippers; Longevity; Gene Expression Profiling; Aging; Transcriptome; Histones; Interneurons; Pharmaceutical Preparations; Medium Spiny Neurons; Color Vision Defects; Hippocampus; Genetics; Sequence Analysis, RNA; Blotting, Western; Neurons; Genes, X-Linked; Censuses</t>
         </is>
       </c>
     </row>
@@ -1773,9 +1745,41 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Theta Rhythm; White Matter; Biomarkers; Nucleus Accumbens; Magnetic Resonance Imaging; Biological Specimen Banks; Adolescent; Ecosystem; Prospective Studies; Drug Discovery; Surveys and Questionnaires; Neuroimaging; Interdisciplinary Research; Aged, 80 and over; Amygdala; Stress Disorders, Post-Traumatic; Neural Pathways; Midline Thalamic Nuclei; Age Factors; Wakefulness; Publishing; Amyloid; Quality of Life; Cognitive Dysfunction; Cerebrovascular Disorders; Computational Biology; Reward; Alzheimer Disease; Psychiatry; Motivation; Amyloid beta-Peptides; Risk Factors; Polyethylene Terephthalates; Anhedonia; Pattern Recognition, Physiological; Peptide Fragments; Depression; Mental Disorders; Neuropsychological Tests; Electrophysiological Phenomena; Exercise; Memory Consolidation; Cognition; Aging; Clinical Trials as Topic; Positron-Emission Tomography; UK Biobank; Aged; Mental Recall; Adverse Childhood Experiences; Artificial Intelligence; Dementia; Machine Learning; Oceans and Seas; Anxiety; Sleep; Emotions; Brain; Down Syndrome; tau Proteins; Learning; Memory, Episodic; Memory Disorders; Young Adult; Child; Nervous System Diseases; Writing; Consensus; Anniversaries and Special Events; Polysomnography; Memory; Hippocampus; Phenotype; Neocortex</t>
-        </is>
-      </c>
+          <t>Polyethylene Terephthalates; Longitudinal Studies; Entorhinal Cortex; Follow-Up Studies; Data Science; Memory; Gamma Rhythm; Magnetic Resonance Imaging; Memory Disorders; Interdisciplinary Research; Proteostasis Deficiencies; Computational Biology; Prefrontal Cortex; Consensus; Depression; Cognitive Dysfunction; tau Proteins; Stress Disorders, Post-Traumatic; Policy; Neuropsychology; Anxiety; Data Aggregation; Neurophysiology; Cohort Studies; Software; Biological Specimen Banks; Documentation; Primates; Positron-Emission Tomography; Clinical Trials as Topic; Neuroimaging; Biomarkers; Pattern Recognition, Physiological; Neuropsychological Tests; Psychiatry; Learning; Data Management; Data Collection; Physicians; Writing; Financial Management; Adverse Childhood Experiences; Drug Discovery; Amyloid; Motivation; Goals; Metadata; Publishing; Saliva; Alzheimer Disease; Premature Birth; Child; Computer Simulation; Nervous System Diseases; Infant, Newborn; Brain; Mental Disorders; Aging; Anniversaries and Special Events; Oceans and Seas; Mentors; Compulsive Behavior; Artificial Intelligence; Cognition; Hippocampus; Memory, Episodic; Community-Institutional Relations; Machine Learning; Interneurons; Dementia; Spectrum Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Konieczny, Piotr</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Pizzagalli, Diego</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Kim, Seungsoo</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Xue, Katherine</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>